<commit_message>
organisation fichier et travail élévations
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\guide2023\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0968FF-1BAA-45F0-9E62-AA8267671E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52251252-A14D-0D4B-B14C-07923CFB2482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41490" yWindow="540" windowWidth="32085" windowHeight="19680" tabRatio="758" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41500" yWindow="540" windowWidth="32760" windowHeight="26460" tabRatio="758" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="183">
   <si>
     <t>GPM</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>&amp;#8505;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; Modifier les </t>
+  </si>
+  <si>
+    <t>a modifier pour que symbol fit avec les sorties de ridewithgps pour diminuer modif manuelle</t>
+  </si>
+  <si>
+    <t>Info, Right, Left, Climb, Danger, Slight Right, Slight Left, Food, Sprint, Straight</t>
   </si>
 </sst>
 </file>
@@ -672,6 +681,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -722,7 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -777,6 +787,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -930,7 +941,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -968,7 +979,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1074,7 +1085,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1248,30 +1259,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="24" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1288,15 +1304,15 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -1310,7 +1326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -1325,7 +1341,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -1354,7 +1370,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -1376,21 +1392,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>54</v>
       </c>
@@ -1404,7 +1420,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1418,7 +1434,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>15</v>
       </c>
@@ -1432,7 +1448,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="16" t="s">
         <v>59</v>
       </c>
@@ -1446,7 +1462,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
@@ -1460,7 +1476,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1474,7 +1490,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1488,7 +1504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>17</v>
       </c>
@@ -1502,7 +1518,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1532,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>33</v>
       </c>
@@ -1530,7 +1546,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
@@ -1544,7 +1560,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="16" t="s">
         <v>13</v>
       </c>
@@ -1558,7 +1574,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +1588,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>48</v>
       </c>
@@ -1586,7 +1602,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>49</v>
       </c>
@@ -1600,7 +1616,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>24</v>
       </c>
@@ -1614,7 +1630,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -1628,7 +1644,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -1640,6 +1656,16 @@
       </c>
       <c r="D18" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="16" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1662,17 +1688,17 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.875" customWidth="1"/>
-    <col min="11" max="11" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1707,7 +1733,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1744,7 +1770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1781,7 +1807,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1816,7 +1842,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1853,7 +1879,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1890,7 +1916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1927,7 +1953,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1983,19 +2009,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -2009,7 +2035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2024,7 +2050,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -2039,7 +2065,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2054,7 +2080,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -2069,7 +2095,7 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -2084,7 +2110,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -2099,7 +2125,7 @@
       </c>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>24.6</v>
       </c>
@@ -2114,7 +2140,7 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>27</v>
       </c>
@@ -2129,7 +2155,7 @@
       </c>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>35</v>
       </c>
@@ -2144,7 +2170,7 @@
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>39.5</v>
       </c>
@@ -2159,7 +2185,7 @@
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.4</v>
       </c>
@@ -2174,7 +2200,7 @@
       </c>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>55.7</v>
       </c>
@@ -2189,7 +2215,7 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -2204,7 +2230,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -2219,7 +2245,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -2234,7 +2260,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -2249,7 +2275,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -2264,7 +2290,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>76.900000000000006</v>
       </c>
@@ -2279,7 +2305,7 @@
       </c>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.5</v>
       </c>
@@ -2294,7 +2320,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>77.8</v>
       </c>
@@ -2309,7 +2335,7 @@
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>92.5</v>
       </c>
@@ -2324,7 +2350,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>98</v>
       </c>
@@ -2339,7 +2365,7 @@
       </c>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>101.2</v>
       </c>
@@ -2354,7 +2380,7 @@
       </c>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>101.7</v>
       </c>
@@ -2369,7 +2395,7 @@
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>104.1</v>
       </c>
@@ -2384,7 +2410,7 @@
       </c>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>107.5</v>
       </c>
@@ -2399,7 +2425,7 @@
       </c>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>107.9</v>
       </c>
@@ -2414,7 +2440,7 @@
       </c>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>108</v>
       </c>
@@ -2429,7 +2455,7 @@
       </c>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>108.2</v>
       </c>
@@ -2444,12 +2470,12 @@
       </c>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -2459,7 +2485,7 @@
       </c>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>109</v>
       </c>
@@ -2474,7 +2500,7 @@
       </c>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>109.15</v>
       </c>
@@ -2489,7 +2515,7 @@
       </c>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>109.35</v>
       </c>
@@ -2504,7 +2530,7 @@
       </c>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>109.75</v>
       </c>
@@ -2519,7 +2545,7 @@
       </c>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="9">
         <v>110.15</v>
       </c>
@@ -2534,7 +2560,7 @@
       </c>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>110.7</v>
       </c>
@@ -2549,7 +2575,7 @@
       </c>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="9">
         <v>110.75</v>
       </c>
@@ -2564,7 +2590,7 @@
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>111.2</v>
       </c>
@@ -2579,7 +2605,7 @@
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>114.4</v>
       </c>
@@ -2594,7 +2620,7 @@
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>117.6</v>
       </c>
@@ -2609,7 +2635,7 @@
       </c>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2621,18 +2647,18 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD42"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -2646,7 +2672,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2660,7 +2686,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -2674,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2688,7 +2714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -2702,7 +2728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -2716,7 +2742,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -2730,7 +2756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>24.6</v>
       </c>
@@ -2744,7 +2770,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>27</v>
       </c>
@@ -2758,7 +2784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>35</v>
       </c>
@@ -2772,7 +2798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>39.5</v>
       </c>
@@ -2786,7 +2812,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.4</v>
       </c>
@@ -2800,7 +2826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>55.7</v>
       </c>
@@ -2814,7 +2840,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -2828,7 +2854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -2842,7 +2868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -2856,7 +2882,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -2870,7 +2896,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -2884,7 +2910,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>76.900000000000006</v>
       </c>
@@ -2898,7 +2924,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.5</v>
       </c>
@@ -2912,7 +2938,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>77.8</v>
       </c>
@@ -2926,7 +2952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>92.5</v>
       </c>
@@ -2940,7 +2966,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>98</v>
       </c>
@@ -2954,7 +2980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>101.2</v>
       </c>
@@ -2968,7 +2994,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>101.7</v>
       </c>
@@ -2982,7 +3008,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>104.1</v>
       </c>
@@ -2996,7 +3022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>107.5</v>
       </c>
@@ -3010,7 +3036,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>107.9</v>
       </c>
@@ -3024,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>108</v>
       </c>
@@ -3038,7 +3064,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>108.2</v>
       </c>
@@ -3052,12 +3078,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -3066,7 +3092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>109</v>
       </c>
@@ -3080,7 +3106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>109.15</v>
       </c>
@@ -3094,7 +3120,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>109.35</v>
       </c>
@@ -3108,7 +3134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>109.75</v>
       </c>
@@ -3122,7 +3148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="9">
         <v>110.15</v>
       </c>
@@ -3136,7 +3162,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <v>110.7</v>
       </c>
@@ -3150,7 +3176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="9">
         <v>110.75</v>
       </c>
@@ -3164,7 +3190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>111.2</v>
       </c>
@@ -3178,7 +3204,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>114.4</v>
       </c>
@@ -3192,7 +3218,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>115</v>
       </c>
@@ -3206,7 +3232,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3221,15 +3247,15 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -3243,7 +3269,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3257,7 +3283,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -3271,7 +3297,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -3285,7 +3311,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -3299,7 +3325,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3314,15 +3340,15 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -3336,7 +3362,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3351,7 +3377,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -3366,7 +3392,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -3381,7 +3407,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -3396,259 +3422,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3663,15 +3689,15 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -3685,7 +3711,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3699,7 +3725,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -3713,7 +3739,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -3727,7 +3753,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -3741,223 +3767,223 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3972,15 +3998,15 @@
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>155</v>
       </c>
@@ -3994,7 +4020,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4009,7 +4035,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4024,7 +4050,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4039,7 +4065,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4054,259 +4080,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajustement pour utiliser mêmes termes que RWG
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52251252-A14D-0D4B-B14C-07923CFB2482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE881B0-85B2-1C4F-BBDD-ECABB82258AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41500" yWindow="540" windowWidth="32760" windowHeight="26460" tabRatio="758" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="209">
   <si>
     <t>GPM</t>
   </si>
@@ -104,27 +104,6 @@
     <t>Heure_dep</t>
   </si>
   <si>
-    <t>GAUCHE</t>
-  </si>
-  <si>
-    <t>DANGER</t>
-  </si>
-  <si>
-    <t>VERT</t>
-  </si>
-  <si>
-    <t>INFO</t>
-  </si>
-  <si>
-    <t>SPRINT</t>
-  </si>
-  <si>
-    <t>DROITE</t>
-  </si>
-  <si>
-    <t>DEPART</t>
-  </si>
-  <si>
     <t>Pont</t>
   </si>
   <si>
@@ -134,27 +113,15 @@
     <t>Ville de McWatters</t>
   </si>
   <si>
-    <t>UP</t>
-  </si>
-  <si>
-    <t>GIRATOIRE</t>
-  </si>
-  <si>
     <t>Rond-point (prendre 2e sortie tout droit)</t>
   </si>
   <si>
     <t>Roundabout (use 2nd exit straight ahead)</t>
   </si>
   <si>
-    <t>UTURN</t>
-  </si>
-  <si>
     <t>Emoji</t>
   </si>
   <si>
-    <t>FIN</t>
-  </si>
-  <si>
     <t>Info</t>
   </si>
   <si>
@@ -164,9 +131,6 @@
     <t>Arrivée finale</t>
   </si>
   <si>
-    <t>MAIRE</t>
-  </si>
-  <si>
     <t>Sprint bonif</t>
   </si>
   <si>
@@ -209,12 +173,6 @@
     <t>Tout droit</t>
   </si>
   <si>
-    <t>LEGER_GAUCHE</t>
-  </si>
-  <si>
-    <t>LEGER_DROITE</t>
-  </si>
-  <si>
     <t>Déviation gauche</t>
   </si>
   <si>
@@ -242,9 +200,6 @@
     <t>Start of 3rd lap</t>
   </si>
   <si>
-    <t>CLOCHE</t>
-  </si>
-  <si>
     <t>Dernier passage</t>
   </si>
   <si>
@@ -368,9 +323,6 @@
     <t>116 km</t>
   </si>
   <si>
-    <t>KM_Neut</t>
-  </si>
-  <si>
     <t>Liens</t>
   </si>
   <si>
@@ -533,18 +485,6 @@
     <t>KM_reel</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>https://unicode-table.com/</t>
-  </si>
-  <si>
-    <t>A effacer plus tard</t>
-  </si>
-  <si>
-    <t>Info_FR_ANG plus necassiare</t>
-  </si>
-  <si>
     <t>Points GPM (Chemin Bousquet)</t>
   </si>
   <si>
@@ -605,13 +545,151 @@
     <t>&amp;#8505;</t>
   </si>
   <si>
-    <t xml:space="preserve">--&gt; Modifier les </t>
-  </si>
-  <si>
-    <t>a modifier pour que symbol fit avec les sorties de ridewithgps pour diminuer modif manuelle</t>
-  </si>
-  <si>
-    <t>Info, Right, Left, Climb, Danger, Slight Right, Slight Left, Food, Sprint, Straight</t>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Climb</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Slight Left</t>
+  </si>
+  <si>
+    <t>Slight Right</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>Uturn</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Mayor</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Ravitaillement</t>
+  </si>
+  <si>
+    <t>Feeding</t>
+  </si>
+  <si>
+    <t>&amp;#127868;</t>
+  </si>
+  <si>
+    <t>Commanditaire</t>
+  </si>
+  <si>
+    <t>Agnico-Eagle</t>
+  </si>
+  <si>
+    <t>Québec</t>
+  </si>
+  <si>
+    <t>Eldorado Gold</t>
+  </si>
+  <si>
+    <t>Partenariat Canadian Malartic</t>
+  </si>
+  <si>
+    <t>Résolu Produits forestiers</t>
+  </si>
+  <si>
+    <t>CSS Harricana</t>
+  </si>
+  <si>
+    <t>Ville d'Amos</t>
+  </si>
+  <si>
+    <t>KM_Total</t>
+  </si>
+  <si>
+    <t>KM_Neutres</t>
+  </si>
+  <si>
+    <t>KM_Route</t>
+  </si>
+  <si>
+    <t>KM_par_tours</t>
+  </si>
+  <si>
+    <t>Distance_en_circuit</t>
+  </si>
+  <si>
+    <t>Distance_totale</t>
+  </si>
+  <si>
+    <t>Jour</t>
+  </si>
+  <si>
+    <t>Mardi</t>
+  </si>
+  <si>
+    <t>Mercredi</t>
+  </si>
+  <si>
+    <t>Jeudi AM</t>
+  </si>
+  <si>
+    <t>Jeudi PM</t>
+  </si>
+  <si>
+    <t>Vendredi</t>
+  </si>
+  <si>
+    <t>Samedi</t>
+  </si>
+  <si>
+    <t>Dimanche</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday AM</t>
+  </si>
+  <si>
+    <t>Thursday PM</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Début ravitaillement</t>
+  </si>
+  <si>
+    <t>Feed opening</t>
   </si>
 </sst>
 </file>
@@ -621,7 +699,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -683,6 +761,12 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -704,7 +788,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -727,12 +811,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -787,13 +891,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -801,6 +908,100 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -902,10 +1103,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{79621ADF-BB4D-43DD-9212-CA2BBF632E2C}" name="Symbol"/>
+    <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
     <tableColumn id="2" xr3:uid="{A1F7DBB1-855B-47BD-8E57-AFA08ED6A331}" name="Emoji"/>
     <tableColumn id="4" xr3:uid="{058306AC-A829-446D-A49F-89A6635464AB}" name="Info_FR"/>
     <tableColumn id="3" xr3:uid="{8133986C-B8E6-4347-8AAA-93A4F524E2BA}" name="Info_ANG"/>
@@ -915,23 +1116,36 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:K8" totalsRowShown="0">
-  <autoFilter ref="A1:K8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:T9" totalsRowShown="0">
+  <autoFilter ref="A1:T9" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{F159CC0E-186F-4E03-998F-71303E6AFF37}" name="Etape"/>
+    <tableColumn id="19" xr3:uid="{3543EB43-316C-0F44-B3AA-B931646E7365}" name="Jour"/>
+    <tableColumn id="18" xr3:uid="{0D4EFF62-DD86-2240-BAFF-EEDA66BC4B15}" name="Day"/>
+    <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
+    <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep"/>
-    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide">
-      <calculatedColumnFormula>IF(G2&gt;0,G2+3,"")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
+    <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
+    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="KM_Route"/>
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="4">
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy"/>
-    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent">
-      <calculatedColumnFormula>IF(G2&gt;0,G2-2,"")</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="3">
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="KM_Neut"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="2">
+      <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="0">
+      <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataCellStyle="Lien hypertexte"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1259,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1272,23 +1486,24 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="24" t="s">
-        <v>180</v>
-      </c>
+      <c r="A4" s="24"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1301,7 +1516,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1314,16 +1529,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -1331,13 +1546,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -1346,13 +1561,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -1361,13 +1576,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
@@ -1375,13 +1590,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1392,15 +1607,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
@@ -1408,597 +1622,858 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
-        <v>15</v>
+      <c r="A3" t="s">
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="16" t="s">
-        <v>59</v>
+      <c r="A4" t="s">
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
-        <v>29</v>
+      <c r="A5" t="s">
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="16" t="s">
-        <v>17</v>
+      <c r="A8" t="s">
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
-        <v>0</v>
+      <c r="A9" t="s">
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
-        <v>33</v>
+      <c r="A10" t="s">
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>47</v>
-      </c>
       <c r="D11" s="16" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
-        <v>13</v>
+      <c r="A12" t="s">
+        <v>163</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="16" t="s">
-        <v>18</v>
+      <c r="A13" t="s">
+        <v>162</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
-        <v>48</v>
+      <c r="A14" t="s">
+        <v>164</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
-        <v>49</v>
+      <c r="A15" t="s">
+        <v>165</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="16" t="s">
-        <v>24</v>
+      <c r="A16" t="s">
+        <v>172</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="16" t="s">
-        <v>27</v>
+      <c r="A17" t="s">
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>157</v>
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>175</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B18" r:id="rId1" xr:uid="{AC4CA5F9-B604-444E-9D9C-32AE4395CC8A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.83203125" customWidth="1"/>
-    <col min="11" max="11" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" t="s">
+        <v>188</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" t="s">
-        <v>110</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2">
+        <v>199</v>
+      </c>
+      <c r="D2" s="27">
+        <v>43656</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="I2" s="25">
         <v>15</v>
       </c>
-      <c r="F2">
-        <f>IF(G2&gt;0,G2+3,"")</f>
+      <c r="J2">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="25">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="Q2">
+        <f>IF(R2&gt;0,R2+3,"")</f>
         <v>46</v>
       </c>
-      <c r="G2">
+      <c r="R2">
         <v>43</v>
       </c>
-      <c r="H2">
-        <f>IF(G2&gt;0,G2-2,"")</f>
+      <c r="S2" s="25">
+        <f>IF(R2&gt;0,R2-2,"")</f>
         <v>41</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="T2" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="D3" s="27">
+        <v>43657</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="I3" s="25">
         <v>45</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" si="0">IF(G3&gt;0,G3+3,"")</f>
+      <c r="J3">
+        <v>98.3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>95.3</v>
+      </c>
+      <c r="M3" s="21">
+        <v>4</v>
+      </c>
+      <c r="N3" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="O3" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>21.6</v>
+      </c>
+      <c r="P3" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>116.9</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q8" si="0">IF(R3&gt;0,R3+3,"")</f>
         <v>46</v>
       </c>
-      <c r="G3">
+      <c r="R3">
         <v>43</v>
       </c>
-      <c r="H3">
-        <f>IF(G3&gt;0,G3-2,"")</f>
+      <c r="S3" s="25">
+        <f>IF(R3&gt;0,R3-2,"")</f>
         <v>41</v>
       </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3" s="21">
-        <v>4</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="T3" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>10</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>48</v>
+      </c>
+      <c r="R4">
+        <v>46</v>
+      </c>
+      <c r="S4" s="25">
+        <v>44</v>
+      </c>
+      <c r="T4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>48</v>
-      </c>
-      <c r="G4">
-        <v>46</v>
-      </c>
-      <c r="H4">
-        <v>44</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="21">
-        <v>0</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5">
+        <v>202</v>
+      </c>
+      <c r="D5" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5">
         <v>18</v>
       </c>
-      <c r="E5">
+      <c r="I5" s="25">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="J5">
+        <v>59.4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>57.4</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>57.4</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="G5">
+      <c r="R5">
         <v>46</v>
       </c>
-      <c r="H5">
-        <f>IF(G5&gt;0,G5-2,"")</f>
+      <c r="S5" s="25">
+        <f>IF(R5&gt;0,R5-2,"")</f>
         <v>44</v>
       </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5" s="21">
-        <v>0</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="T5" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6">
+        <v>203</v>
+      </c>
+      <c r="D6" s="27">
+        <v>43659</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6">
         <v>14</v>
       </c>
-      <c r="E6">
+      <c r="I6" s="25">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="J6">
+        <v>145</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>140</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="25">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>140</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="G6">
+      <c r="R6">
         <v>43</v>
       </c>
-      <c r="H6">
-        <f>IF(G6&gt;0,G6-2,"")</f>
+      <c r="S6" s="25">
+        <f>IF(R6&gt;0,R6-2,"")</f>
         <v>41</v>
       </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="T6" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7">
+        <v>204</v>
+      </c>
+      <c r="D7" s="27">
+        <v>43660</v>
+      </c>
+      <c r="E7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="I7" s="25">
         <v>30</v>
       </c>
-      <c r="F7">
+      <c r="J7">
+        <v>118.9</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>115.9</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>115.9</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="G7">
+      <c r="R7">
         <v>43</v>
       </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H8" si="1">IF(G7&gt;0,G7-2,"")</f>
+      <c r="S7" s="25">
+        <f t="shared" ref="S7:S8" si="1">IF(R7&gt;0,R7-2,"")</f>
         <v>41</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21">
-        <v>0</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="T7" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8">
+        <v>205</v>
+      </c>
+      <c r="D8" s="27">
+        <v>43661</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8">
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="I8" s="25">
         <v>30</v>
       </c>
-      <c r="F8">
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="21">
+        <v>10</v>
+      </c>
+      <c r="N8" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="O8" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>54</v>
+      </c>
+      <c r="P8" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>54</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="G8">
+      <c r="R8">
         <v>43</v>
       </c>
-      <c r="H8">
+      <c r="S8" s="25">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8" s="21">
-        <v>10</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>109</v>
-      </c>
+      <c r="T8" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="G9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="26">
+        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" t="str">
+        <f>IF(R9&gt;0,R9+3,"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="25" t="str">
+        <f>IF(R9&gt;0,R9-2,"")</f>
+        <v/>
+      </c>
+      <c r="T9" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
-    <hyperlink ref="K3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
-    <hyperlink ref="K7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
-    <hyperlink ref="K8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
-    <hyperlink ref="K6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+    <hyperlink ref="T2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
+    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
+    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
+    <hyperlink ref="T8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
+    <hyperlink ref="T6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId6"/>
   </tableParts>
@@ -2010,7 +2485,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2023,16 +2498,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -2040,13 +2515,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2055,7 +2530,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -2070,13 +2545,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>169</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -2085,13 +2560,13 @@
         <v>7.9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2100,13 +2575,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="F6" s="22"/>
     </row>
@@ -2115,13 +2590,13 @@
         <v>12.1</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="F7" s="22"/>
     </row>
@@ -2130,13 +2605,13 @@
         <v>24.6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -2145,13 +2620,13 @@
         <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="F9" s="22"/>
     </row>
@@ -2160,13 +2635,13 @@
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="F10" s="22"/>
     </row>
@@ -2175,13 +2650,13 @@
         <v>39.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -2190,13 +2665,13 @@
         <v>47.4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F12" s="22"/>
     </row>
@@ -2205,13 +2680,13 @@
         <v>55.7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F13" s="22"/>
     </row>
@@ -2220,13 +2695,13 @@
         <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F14" s="22"/>
     </row>
@@ -2235,13 +2710,13 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -2250,13 +2725,13 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F16" s="22"/>
     </row>
@@ -2265,13 +2740,13 @@
         <v>62.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F17" s="22"/>
     </row>
@@ -2280,13 +2755,13 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F18" s="22"/>
     </row>
@@ -2295,13 +2770,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>17</v>
+        <v>160</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="F19" s="22"/>
     </row>
@@ -2310,13 +2785,13 @@
         <v>77.5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F20" s="22"/>
     </row>
@@ -2325,13 +2800,13 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F21" s="22"/>
     </row>
@@ -2340,13 +2815,13 @@
         <v>92.5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="F22" s="22"/>
     </row>
@@ -2355,13 +2830,13 @@
         <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="F23" s="22"/>
     </row>
@@ -2370,13 +2845,13 @@
         <v>101.2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F24" s="22"/>
     </row>
@@ -2385,13 +2860,13 @@
         <v>101.7</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F25" s="22"/>
     </row>
@@ -2400,13 +2875,13 @@
         <v>104.1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>24</v>
+        <v>172</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F26" s="22"/>
     </row>
@@ -2415,13 +2890,13 @@
         <v>107.5</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F27" s="22"/>
     </row>
@@ -2430,7 +2905,7 @@
         <v>107.9</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -2445,13 +2920,13 @@
         <v>108</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F29" s="22"/>
     </row>
@@ -2460,7 +2935,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -2475,7 +2950,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -2490,7 +2965,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -2505,13 +2980,13 @@
         <v>109.15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F33" s="22"/>
     </row>
@@ -2520,7 +2995,7 @@
         <v>109.35</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>7</v>
@@ -2535,7 +3010,7 @@
         <v>109.75</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
@@ -2550,7 +3025,7 @@
         <v>110.15</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
@@ -2565,7 +3040,7 @@
         <v>110.7</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
@@ -2580,7 +3055,7 @@
         <v>110.75</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>3</v>
@@ -2595,13 +3070,13 @@
         <v>111.2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F39" s="22"/>
     </row>
@@ -2610,13 +3085,13 @@
         <v>114.4</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F40" s="22"/>
     </row>
@@ -2625,13 +3100,13 @@
         <v>117.6</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F41" s="22"/>
     </row>
@@ -2644,10 +3119,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2660,16 +3135,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -2677,13 +3152,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -2691,7 +3166,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -2705,13 +3180,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>169</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -2719,13 +3194,13 @@
         <v>7.9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -2733,13 +3208,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -2747,492 +3222,506 @@
         <v>12.1</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
-        <v>24.6</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>27</v>
+        <v>24.6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>169</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
         <v>35</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
         <v>39.5</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
+      <c r="B12" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
         <v>47.4</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
+      <c r="B13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
         <v>55.7</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="B14" s="7" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>45</v>
+      <c r="C14" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>61.3</v>
+        <v>61</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>61.8</v>
+        <v>61.3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>13</v>
+        <v>162</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>62.8</v>
+        <v>61.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>68</v>
+        <v>163</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
         <v>72.400000000000006</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B19" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="3">
+      <c r="D19" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
         <v>76.900000000000006</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="3">
-        <v>77.5</v>
-      </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>75</v>
+        <v>160</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
+        <v>77.5</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
         <v>77.8</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
+      <c r="B22" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
         <v>92.5</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="3">
-        <v>98</v>
-      </c>
       <c r="B23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>21</v>
+        <v>171</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>101.2</v>
+        <v>98</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>101.7</v>
+        <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>104.1</v>
+        <v>101.7</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
-        <v>107.5</v>
+        <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>107.9</v>
+        <v>107.5</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>108</v>
+        <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>108.2</v>
+        <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>108.4</v>
+        <v>108.2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
+        <v>108.4</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
         <v>109</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B33" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D33" s="15" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="9">
-        <v>109.15</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
-        <v>109.35</v>
+        <v>109.15</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>7</v>
+        <v>161</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
-        <v>109.75</v>
+        <v>109.35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="9">
+        <v>109.75</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A37" s="9">
         <v>110.15</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B37" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D37" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="3">
+    <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
         <v>110.7</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B38" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="9">
+    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A39" s="9">
         <v>110.75</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="3">
-        <v>111.2</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
+        <v>111.2</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A41" s="3">
         <v>114.4</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A41" s="3">
+      <c r="B41" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A42" s="3">
         <v>115</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="B42" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3244,7 +3733,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3257,16 +3746,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3274,13 +3763,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3288,13 +3777,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3302,13 +3791,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -3316,13 +3805,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3337,7 +3826,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3350,16 +3839,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -3367,13 +3856,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -3382,13 +3871,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -3397,13 +3886,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -3412,13 +3901,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -3686,7 +4175,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3699,16 +4188,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3716,13 +4205,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3730,13 +4219,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3744,13 +4233,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -3758,13 +4247,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
@@ -3995,7 +4484,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4008,16 +4497,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -4025,13 +4514,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -4040,13 +4529,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -4055,13 +4544,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -4070,13 +4559,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="F5" s="22"/>
     </row>

</xml_diff>

<commit_message>
Ajout idees parcours 2023
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AC3A51-4C7F-9846-A29B-B63BB8E927F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF517A12-CEF0-0D47-8493-FB3C7129D6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
     <sheet name="Lexique" sheetId="20" r:id="rId2"/>
     <sheet name="Details" sheetId="21" r:id="rId3"/>
-    <sheet name="Etape_1" sheetId="6" r:id="rId4"/>
-    <sheet name="Etape_2" sheetId="22" r:id="rId5"/>
-    <sheet name="Etape_3" sheetId="24" r:id="rId6"/>
-    <sheet name="Etape_4" sheetId="25" r:id="rId7"/>
-    <sheet name="Etape_5" sheetId="26" r:id="rId8"/>
-    <sheet name="Etape_6" sheetId="27" r:id="rId9"/>
-    <sheet name="Etape_7" sheetId="28" r:id="rId10"/>
+    <sheet name="Details2023" sheetId="29" r:id="rId4"/>
+    <sheet name="Etape_1" sheetId="6" r:id="rId5"/>
+    <sheet name="Etape_2" sheetId="22" r:id="rId6"/>
+    <sheet name="Etape_3" sheetId="24" r:id="rId7"/>
+    <sheet name="Etape_4" sheetId="25" r:id="rId8"/>
+    <sheet name="Etape_5" sheetId="26" r:id="rId9"/>
+    <sheet name="Etape_6" sheetId="27" r:id="rId10"/>
+    <sheet name="Etape_7" sheetId="28" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="211">
   <si>
     <t>GPM</t>
   </si>
@@ -690,6 +691,12 @@
   </si>
   <si>
     <t>Gouvernement du Québec</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/41813874</t>
+  </si>
+  <si>
+    <t>5 x 18.4 km + approches = 93,7 km</t>
   </si>
 </sst>
 </file>
@@ -900,7 +907,109 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1103,7 +1212,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
@@ -1125,28 +1234,67 @@
     <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
     <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="16"/>
     <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="KM_Route"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="15"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="13">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="3">
-      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</calculatedColumnFormula>
+    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="12">
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="11">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="9">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataCellStyle="Lien hypertexte"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58EED1FE-3653-0847-9EDE-8FA4564D716A}" name="Tableau24" displayName="Tableau24" ref="A1:T9" totalsRowShown="0">
+  <autoFilter ref="A1:T9" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{0A284ACC-6EDA-AF4C-B772-1C1B570B7A1B}" name="Etape"/>
+    <tableColumn id="19" xr3:uid="{AAE39FF3-3F24-A543-87FB-E807B6BECABD}" name="Jour"/>
+    <tableColumn id="18" xr3:uid="{9218298C-2AF9-3046-A2EE-FF3EB3B8AC01}" name="Day"/>
+    <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
+    <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
+    <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
+    <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
+    <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
+      <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
+      <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
+      <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
+      <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
+      <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1512,6 +1660,355 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>111.2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>114.4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>115</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="18"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="15"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="19"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="15"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="17"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="18"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="17"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="18"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="18"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A16" s="3"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="18"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="15"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="15"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A19" s="3"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="17"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A20" s="3"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="18"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="15"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="17"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="15"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A24" s="3"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="15"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A25" s="3"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="15"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A26" s="3"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="15"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A27" s="3"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="15"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="15"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A29" s="3"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="15"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A30" s="3"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="15"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="15"/>
+      <c r="F31" s="22"/>
+    </row>
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="15"/>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A33" s="9"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="19"/>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A34" s="9"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="15"/>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A35" s="9"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="15"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A36" s="9"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="15"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="15"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A38" s="9"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="15"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="15"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="15"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="17"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -1885,8 +2382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2026,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="25">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
         <v>131.69999999999999</v>
       </c>
       <c r="Q2">
@@ -2093,8 +2590,8 @@
         <v>21.6</v>
       </c>
       <c r="P3" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
-        <v>116.9</v>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
+        <v>95.3</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q8" si="0">IF(R3&gt;0,R3+3,"")</f>
@@ -2160,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
         <v>10</v>
       </c>
       <c r="Q4">
@@ -2225,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
         <v>57.4</v>
       </c>
       <c r="Q5">
@@ -2292,7 +2789,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="25">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
         <v>140</v>
       </c>
       <c r="Q6">
@@ -2359,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
         <v>115.9</v>
       </c>
       <c r="Q7">
@@ -2423,8 +2920,8 @@
         <v>54</v>
       </c>
       <c r="P8" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
-        <v>54</v>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
+        <v>0</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -2442,27 +2939,69 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="G9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="27">
+        <v>43660</v>
+      </c>
+      <c r="E9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9" s="25">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>96.7</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>93.7</v>
+      </c>
+      <c r="M9" s="21">
+        <v>5</v>
+      </c>
+      <c r="N9" s="21">
+        <v>18.399999999999999</v>
+      </c>
       <c r="O9" s="21">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="P9" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]+Tableau2[[#This Row],[Distance_en_circuit]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" t="str">
-        <f>IF(R9&gt;0,R9+3,"")</f>
-        <v/>
-      </c>
-      <c r="S9" s="25" t="str">
-        <f>IF(R9&gt;0,R9-2,"")</f>
-        <v/>
-      </c>
-      <c r="T9" s="20"/>
+        <f>Tableau2[[#This Row],[KM_Route]]</f>
+        <v>93.7</v>
+      </c>
+      <c r="Q9">
+        <v>46</v>
+      </c>
+      <c r="R9">
+        <v>43</v>
+      </c>
+      <c r="S9" s="25">
+        <v>41</v>
+      </c>
+      <c r="T9" s="20" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2471,6 +3010,584 @@
     <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
     <hyperlink ref="T8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
     <hyperlink ref="T6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+    <hyperlink ref="T9" r:id="rId6" xr:uid="{3F51F527-190F-9F47-AAE7-517DB2147C74}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D286032-E11B-2F4F-8B68-3808324E7B4A}">
+  <dimension ref="A1:T8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="27">
+        <v>43656</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2" s="25">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="25">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="Q2">
+        <f>IF(R2&gt;0,R2+3,"")</f>
+        <v>46</v>
+      </c>
+      <c r="R2">
+        <v>43</v>
+      </c>
+      <c r="S2" s="25">
+        <f>IF(R2&gt;0,R2-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="27">
+        <v>43657</v>
+      </c>
+      <c r="E3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3" s="25">
+        <v>45</v>
+      </c>
+      <c r="J3">
+        <v>98.3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>95.3</v>
+      </c>
+      <c r="M3" s="21">
+        <v>4</v>
+      </c>
+      <c r="N3" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="O3" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>21.6</v>
+      </c>
+      <c r="P3" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>95.3</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q7" si="0">IF(R3&gt;0,R3+3,"")</f>
+        <v>46</v>
+      </c>
+      <c r="R3">
+        <v>43</v>
+      </c>
+      <c r="S3" s="25">
+        <f>IF(R3&gt;0,R3-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D4" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>10</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>48</v>
+      </c>
+      <c r="R4">
+        <v>46</v>
+      </c>
+      <c r="S4" s="25">
+        <v>44</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5" s="25">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>59.4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>57.4</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>57.4</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="R5">
+        <v>46</v>
+      </c>
+      <c r="S5" s="25">
+        <f>IF(R5&gt;0,R5-2,"")</f>
+        <v>44</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" s="27">
+        <v>43659</v>
+      </c>
+      <c r="E6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>145</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>140</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="25">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>140</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="R6">
+        <v>43</v>
+      </c>
+      <c r="S6" s="25">
+        <f>IF(R6&gt;0,R6-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="27">
+        <v>43660</v>
+      </c>
+      <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7" s="25">
+        <v>30</v>
+      </c>
+      <c r="J7">
+        <v>118.9</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>115.9</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>115.9</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="R7">
+        <v>43</v>
+      </c>
+      <c r="S7" s="25">
+        <f t="shared" ref="S7" si="1">IF(R7&gt;0,R7-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="27">
+        <v>43661</v>
+      </c>
+      <c r="E8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8" s="25">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>96.7</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>93.7</v>
+      </c>
+      <c r="M8" s="21">
+        <v>5</v>
+      </c>
+      <c r="N8" s="21">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O8" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>92</v>
+      </c>
+      <c r="P8" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>93.7</v>
+      </c>
+      <c r="Q8">
+        <v>46</v>
+      </c>
+      <c r="R8">
+        <v>43</v>
+      </c>
+      <c r="S8" s="25">
+        <v>41</v>
+      </c>
+      <c r="T8" s="20" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" xr:uid="{27AC5D4C-3BC2-F545-B17F-1C5289CFF5CB}"/>
+    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{9BD66C34-9BC8-124D-9A01-D34D1D703557}"/>
+    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{C87D0144-957A-804A-AEB4-531610EB899D}"/>
+    <hyperlink ref="T6" r:id="rId4" xr:uid="{8420C6E5-6743-CB48-937E-CA00687573DE}"/>
+    <hyperlink ref="T8" r:id="rId5" xr:uid="{94B4D1BE-E2B6-BA4D-A834-AAAE6B904595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2480,7 +3597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
@@ -3117,7 +4234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D43"/>
   <sheetViews>
@@ -3728,7 +4845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F578A-E7BF-4EB0-BBD6-BC84A4E8AD52}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -3821,7 +4938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D617926-71C2-4A16-9C07-BDFAD50267E4}">
   <dimension ref="A1:F42"/>
   <sheetViews>
@@ -4170,7 +5287,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61388227-0C5A-4795-A5A0-4EE10C974F3C}">
   <dimension ref="A1:D42"/>
   <sheetViews>
@@ -4477,353 +5594,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
-  <dimension ref="A1:F42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>111.2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="15"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="17"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="17"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="18"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="15"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="17"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="15"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="15"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="15"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="15"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A26" s="3"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="15"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="15"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A28" s="3"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="15"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="15"/>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="15"/>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="15"/>
-      <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="15"/>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="19"/>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A34" s="9"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="15"/>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A35" s="9"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="15"/>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A36" s="9"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="15"/>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A37" s="3"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="15"/>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="15"/>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A39" s="3"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="15"/>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A40" s="3"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="15"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A41" s="3"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="17"/>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modification du calcul du temps avec lubridate
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF517A12-CEF0-0D47-8493-FB3C7129D6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5EC3D8-069E-4B41-B239-9D9233107A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
     <sheet name="Lexique" sheetId="20" r:id="rId2"/>
     <sheet name="Details" sheetId="21" r:id="rId3"/>
-    <sheet name="Details2023" sheetId="29" r:id="rId4"/>
+    <sheet name="Details_options" sheetId="29" r:id="rId4"/>
     <sheet name="Etape_1" sheetId="6" r:id="rId5"/>
     <sheet name="Etape_2" sheetId="22" r:id="rId6"/>
     <sheet name="Etape_3" sheetId="24" r:id="rId7"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="212">
   <si>
     <t>GPM</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Lac Malartic street</t>
   </si>
   <si>
-    <t>Rue  due Lac Malartic</t>
-  </si>
-  <si>
     <t>City of Cadillac</t>
   </si>
   <si>
@@ -303,12 +300,6 @@
     <t>Malartic - Malartic</t>
   </si>
   <si>
-    <t>138.4 km</t>
-  </si>
-  <si>
-    <t>52.7 km</t>
-  </si>
-  <si>
     <t>Amos -Preissac - RH - Amos</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>10 x 10.8 km = 108 km</t>
   </si>
   <si>
-    <t>116 km</t>
-  </si>
-  <si>
     <t>Liens</t>
   </si>
   <si>
@@ -438,15 +426,9 @@
     <t>U-turn</t>
   </si>
   <si>
-    <t>Arrivée&lt;br/&gt;Bonification en temps et points&lt;br/&gt;(10-6-4 sec; 30-24-20-16-12-10-8-6-4-2 pts)</t>
-  </si>
-  <si>
     <t>Finish&lt;br/&gt;Time and points bonus&lt;br/&gt;(10-6-4 sec; 30-24-20-16-12-10-8-6-4-2 pts)</t>
   </si>
   <si>
-    <t>115.6 km</t>
-  </si>
-  <si>
     <t>Virage gauche</t>
   </si>
   <si>
@@ -697,6 +679,27 @@
   </si>
   <si>
     <t>5 x 18.4 km + approches = 93,7 km</t>
+  </si>
+  <si>
+    <t>Distance_Route</t>
+  </si>
+  <si>
+    <t>131.7 km</t>
+  </si>
+  <si>
+    <t>57.4 km</t>
+  </si>
+  <si>
+    <t>140 km</t>
+  </si>
+  <si>
+    <t>115.9 km</t>
+  </si>
+  <si>
+    <t>Rue  du Lac Malartic</t>
+  </si>
+  <si>
+    <t>Arrivée&lt;br/&gt;Bonification en temps et points</t>
   </si>
 </sst>
 </file>
@@ -775,7 +778,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -791,6 +794,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -902,12 +911,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1049,18 +1060,16 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="double">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1068,7 +1077,16 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1212,7 +1230,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
@@ -1225,8 +1243,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:T9" totalsRowShown="0">
-  <autoFilter ref="A1:T9" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:T8" totalsRowShown="0">
+  <autoFilter ref="A1:T8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{F159CC0E-186F-4E03-998F-71303E6AFF37}" name="Etape"/>
     <tableColumn id="19" xr3:uid="{3543EB43-316C-0F44-B3AA-B931646E7365}" name="Jour"/>
@@ -1234,19 +1252,21 @@
     <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
     <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="17"/>
     <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
-    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="KM_Route"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="14">
+      <calculatedColumnFormula>P2-O2</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="13">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="12">
-      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Route]]</calculatedColumnFormula>
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="11">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
@@ -1262,8 +1282,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58EED1FE-3653-0847-9EDE-8FA4564D716A}" name="Tableau24" displayName="Tableau24" ref="A1:T9" totalsRowShown="0">
-  <autoFilter ref="A1:T9" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58EED1FE-3653-0847-9EDE-8FA4564D716A}" name="Tableau24" displayName="Tableau24" ref="A1:T3" totalsRowShown="0">
+  <autoFilter ref="A1:T3" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{0A284ACC-6EDA-AF4C-B772-1C1B570B7A1B}" name="Etape"/>
     <tableColumn id="19" xr3:uid="{AAE39FF3-3F24-A543-87FB-E807B6BECABD}" name="Jour"/>
@@ -1634,17 +1654,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
@@ -1677,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -1694,13 +1714,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -1709,7 +1729,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -1724,7 +1744,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1739,13 +1759,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2026,7 +2046,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2043,13 +2063,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2058,7 +2078,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2073,7 +2093,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2087,13 +2107,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2125,80 +2145,80 @@
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -2206,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2217,156 +2237,156 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" t="s">
         <v>168</v>
-      </c>
-      <c r="B18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2380,10 +2400,582 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.83203125" customWidth="1"/>
+    <col min="24" max="24" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" t="s">
+        <v>205</v>
+      </c>
+      <c r="O1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="27">
+        <v>43656</v>
+      </c>
+      <c r="E2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2" s="25">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="28">
+        <f t="shared" ref="N2:N8" si="0">P2-O2</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="O2" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>131.69999999999999</v>
+      </c>
+      <c r="Q2">
+        <v>46</v>
+      </c>
+      <c r="R2">
+        <v>44</v>
+      </c>
+      <c r="S2" s="25">
+        <f>IF(R2&gt;0,R2-2,"")</f>
+        <v>42</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="27">
+        <v>43657</v>
+      </c>
+      <c r="E3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3" s="25">
+        <v>45</v>
+      </c>
+      <c r="J3">
+        <v>119.9</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="21">
+        <v>4</v>
+      </c>
+      <c r="M3" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="N3" s="28">
+        <f t="shared" si="0"/>
+        <v>95.300000000000011</v>
+      </c>
+      <c r="O3" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>21.6</v>
+      </c>
+      <c r="P3" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>116.9</v>
+      </c>
+      <c r="Q3">
+        <v>46</v>
+      </c>
+      <c r="R3">
+        <v>44</v>
+      </c>
+      <c r="S3" s="25">
+        <f>IF(R3&gt;0,R3-2,"")</f>
+        <v>42</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0</v>
+      </c>
+      <c r="N4" s="28">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O4" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>47</v>
+      </c>
+      <c r="R4">
+        <v>45</v>
+      </c>
+      <c r="S4" s="25">
+        <v>42</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="27">
+        <v>43658</v>
+      </c>
+      <c r="E5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5" s="25">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>59.4</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="21">
+        <v>0</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0</v>
+      </c>
+      <c r="N5" s="28">
+        <f t="shared" si="0"/>
+        <v>57.4</v>
+      </c>
+      <c r="O5" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>57.4</v>
+      </c>
+      <c r="Q5">
+        <v>48</v>
+      </c>
+      <c r="R5">
+        <v>46</v>
+      </c>
+      <c r="S5" s="25">
+        <f>IF(R5&gt;0,R5-2,"")</f>
+        <v>44</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="27">
+        <v>43659</v>
+      </c>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>145</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="28">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="O6" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>140</v>
+      </c>
+      <c r="Q6">
+        <v>45</v>
+      </c>
+      <c r="R6">
+        <v>43</v>
+      </c>
+      <c r="S6" s="25">
+        <f>IF(R6&gt;0,R6-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="27">
+        <v>43660</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7" s="25">
+        <v>30</v>
+      </c>
+      <c r="J7">
+        <v>118.9</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" si="0"/>
+        <v>115.9</v>
+      </c>
+      <c r="O7" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>115.9</v>
+      </c>
+      <c r="Q7">
+        <v>45</v>
+      </c>
+      <c r="R7">
+        <v>43</v>
+      </c>
+      <c r="S7" s="25">
+        <f t="shared" ref="S7:S8" si="1">IF(R7&gt;0,R7-2,"")</f>
+        <v>41</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="27">
+        <v>43661</v>
+      </c>
+      <c r="E8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8" s="25">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>108</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="21">
+        <v>10</v>
+      </c>
+      <c r="M8" s="21">
+        <v>10.8</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="28">
+        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
+        <v>108</v>
+      </c>
+      <c r="P8" s="29">
+        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
+        <v>108</v>
+      </c>
+      <c r="Q8">
+        <v>45</v>
+      </c>
+      <c r="R8">
+        <v>43</v>
+      </c>
+      <c r="S8" s="25">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="T8" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
+    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
+    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
+    <hyperlink ref="T8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
+    <hyperlink ref="T6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D286032-E11B-2F4F-8B68-3808324E7B4A}">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2414,1185 +3006,139 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" t="s">
-        <v>184</v>
-      </c>
-      <c r="L1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O1" t="s">
-        <v>187</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>66</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="25" t="s">
-        <v>68</v>
-      </c>
       <c r="T1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="27">
-        <v>43656</v>
+        <v>43661</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="H2">
         <v>16</v>
       </c>
       <c r="I2" s="25">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J2">
-        <v>136.69999999999999</v>
+        <v>96.7</v>
       </c>
       <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
+        <v>93.7</v>
+      </c>
+      <c r="M2" s="21">
         <v>5</v>
       </c>
-      <c r="L2">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>131.69999999999999</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="25">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>131.69999999999999</v>
+      <c r="N2" s="21">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="O2" s="21">
+        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
+        <v>92</v>
+      </c>
+      <c r="P2" s="26">
+        <f>Tableau24[[#This Row],[KM_Route]]</f>
+        <v>93.7</v>
       </c>
       <c r="Q2">
-        <f>IF(R2&gt;0,R2+3,"")</f>
         <v>46</v>
       </c>
       <c r="R2">
         <v>43</v>
       </c>
       <c r="S2" s="25">
-        <f>IF(R2&gt;0,R2-2,"")</f>
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="27">
-        <v>43657</v>
-      </c>
-      <c r="E3" t="s">
-        <v>208</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3" s="25">
-        <v>45</v>
-      </c>
-      <c r="J3">
-        <v>98.3</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>95.3</v>
-      </c>
-      <c r="M3" s="21">
-        <v>4</v>
-      </c>
-      <c r="N3" s="21">
-        <v>5.4</v>
-      </c>
-      <c r="O3" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>21.6</v>
-      </c>
-      <c r="P3" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>95.3</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q8" si="0">IF(R3&gt;0,R3+3,"")</f>
-        <v>46</v>
-      </c>
-      <c r="R3">
-        <v>43</v>
-      </c>
-      <c r="S3" s="25">
-        <f>IF(R3&gt;0,R3-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="27">
-        <v>43658</v>
-      </c>
-      <c r="E4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4" s="25">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>10</v>
-      </c>
-      <c r="M4" s="21">
-        <v>0</v>
-      </c>
-      <c r="N4" s="21">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <v>48</v>
-      </c>
-      <c r="R4">
-        <v>46</v>
-      </c>
-      <c r="S4" s="25">
-        <v>44</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="27">
-        <v>43658</v>
-      </c>
-      <c r="E5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5">
-        <v>18</v>
-      </c>
-      <c r="I5" s="25">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>59.4</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>57.4</v>
-      </c>
-      <c r="M5" s="21">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>57.4</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="R5">
-        <v>46</v>
-      </c>
-      <c r="S5" s="25">
-        <f>IF(R5&gt;0,R5-2,"")</f>
-        <v>44</v>
-      </c>
-      <c r="T5" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="27">
-        <v>43659</v>
-      </c>
-      <c r="E6" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6" s="25">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>145</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>140</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="25">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>140</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R6">
-        <v>43</v>
-      </c>
-      <c r="S6" s="25">
-        <f>IF(R6&gt;0,R6-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" t="s">
         <v>203</v>
-      </c>
-      <c r="D7" s="27">
-        <v>43660</v>
-      </c>
-      <c r="E7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7">
-        <v>16</v>
-      </c>
-      <c r="I7" s="25">
-        <v>30</v>
-      </c>
-      <c r="J7">
-        <v>118.9</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>115.9</v>
-      </c>
-      <c r="M7" s="21">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>115.9</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R7">
-        <v>43</v>
-      </c>
-      <c r="S7" s="25">
-        <f t="shared" ref="S7:S8" si="1">IF(R7&gt;0,R7-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T7" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D8" s="27">
-        <v>43661</v>
-      </c>
-      <c r="E8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8">
-        <v>14</v>
-      </c>
-      <c r="I8" s="25">
-        <v>30</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
-        <v>10</v>
-      </c>
-      <c r="N8" s="21">
-        <v>5.4</v>
-      </c>
-      <c r="O8" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>54</v>
-      </c>
-      <c r="P8" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R8">
-        <v>43</v>
-      </c>
-      <c r="S8" s="25">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="T8" s="20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D9" s="27">
-        <v>43660</v>
-      </c>
-      <c r="E9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="H9">
-        <v>16</v>
-      </c>
-      <c r="I9" s="25">
-        <v>30</v>
-      </c>
-      <c r="J9">
-        <v>96.7</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>93.7</v>
-      </c>
-      <c r="M9" s="21">
-        <v>5</v>
-      </c>
-      <c r="N9" s="21">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="O9" s="21">
-        <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>92</v>
-      </c>
-      <c r="P9" s="26">
-        <f>Tableau2[[#This Row],[KM_Route]]</f>
-        <v>93.7</v>
-      </c>
-      <c r="Q9">
-        <v>46</v>
-      </c>
-      <c r="R9">
-        <v>43</v>
-      </c>
-      <c r="S9" s="25">
-        <v>41</v>
-      </c>
-      <c r="T9" s="20" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
-    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
-    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
-    <hyperlink ref="T8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
-    <hyperlink ref="T6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
-    <hyperlink ref="T9" r:id="rId6" xr:uid="{3F51F527-190F-9F47-AAE7-517DB2147C74}"/>
+    <hyperlink ref="T2" r:id="rId1" xr:uid="{94B4D1BE-E2B6-BA4D-A834-AAAE6B904595}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D286032-E11B-2F4F-8B68-3808324E7B4A}">
-  <dimension ref="A1:T8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.83203125" customWidth="1"/>
-    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" t="s">
-        <v>184</v>
-      </c>
-      <c r="L1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O1" t="s">
-        <v>187</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="27">
-        <v>43656</v>
-      </c>
-      <c r="E2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
-      </c>
-      <c r="I2" s="25">
-        <v>15</v>
-      </c>
-      <c r="J2">
-        <v>136.69999999999999</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>131.69999999999999</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="25">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>131.69999999999999</v>
-      </c>
-      <c r="Q2">
-        <f>IF(R2&gt;0,R2+3,"")</f>
-        <v>46</v>
-      </c>
-      <c r="R2">
-        <v>43</v>
-      </c>
-      <c r="S2" s="25">
-        <f>IF(R2&gt;0,R2-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T2" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="27">
-        <v>43657</v>
-      </c>
-      <c r="E3" t="s">
-        <v>208</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3">
-        <v>16</v>
-      </c>
-      <c r="I3" s="25">
-        <v>45</v>
-      </c>
-      <c r="J3">
-        <v>98.3</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>95.3</v>
-      </c>
-      <c r="M3" s="21">
-        <v>4</v>
-      </c>
-      <c r="N3" s="21">
-        <v>5.4</v>
-      </c>
-      <c r="O3" s="21">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>21.6</v>
-      </c>
-      <c r="P3" s="26">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>95.3</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q7" si="0">IF(R3&gt;0,R3+3,"")</f>
-        <v>46</v>
-      </c>
-      <c r="R3">
-        <v>43</v>
-      </c>
-      <c r="S3" s="25">
-        <f>IF(R3&gt;0,R3-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T3" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="27">
-        <v>43658</v>
-      </c>
-      <c r="E4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4" s="25">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>10</v>
-      </c>
-      <c r="M4" s="21">
-        <v>0</v>
-      </c>
-      <c r="N4" s="21">
-        <v>0</v>
-      </c>
-      <c r="O4" s="21">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="26">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <v>48</v>
-      </c>
-      <c r="R4">
-        <v>46</v>
-      </c>
-      <c r="S4" s="25">
-        <v>44</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="27">
-        <v>43658</v>
-      </c>
-      <c r="E5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5">
-        <v>18</v>
-      </c>
-      <c r="I5" s="25">
-        <v>15</v>
-      </c>
-      <c r="J5">
-        <v>59.4</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>57.4</v>
-      </c>
-      <c r="M5" s="21">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="26">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>57.4</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="R5">
-        <v>46</v>
-      </c>
-      <c r="S5" s="25">
-        <f>IF(R5&gt;0,R5-2,"")</f>
-        <v>44</v>
-      </c>
-      <c r="T5" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="27">
-        <v>43659</v>
-      </c>
-      <c r="E6" t="s">
-        <v>180</v>
-      </c>
-      <c r="F6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6">
-        <v>14</v>
-      </c>
-      <c r="I6" s="25">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>145</v>
-      </c>
-      <c r="K6">
-        <v>5</v>
-      </c>
-      <c r="L6">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>140</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="25">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>140</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R6">
-        <v>43</v>
-      </c>
-      <c r="S6" s="25">
-        <f>IF(R6&gt;0,R6-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D7" s="27">
-        <v>43660</v>
-      </c>
-      <c r="E7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7">
-        <v>16</v>
-      </c>
-      <c r="I7" s="25">
-        <v>30</v>
-      </c>
-      <c r="J7">
-        <v>118.9</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>115.9</v>
-      </c>
-      <c r="M7" s="21">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="26">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>115.9</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="R7">
-        <v>43</v>
-      </c>
-      <c r="S7" s="25">
-        <f t="shared" ref="S7" si="1">IF(R7&gt;0,R7-2,"")</f>
-        <v>41</v>
-      </c>
-      <c r="T7" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>195</v>
-      </c>
-      <c r="C8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" s="27">
-        <v>43661</v>
-      </c>
-      <c r="E8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="H8">
-        <v>16</v>
-      </c>
-      <c r="I8" s="25">
-        <v>30</v>
-      </c>
-      <c r="J8">
-        <v>96.7</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
-        <f>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</f>
-        <v>93.7</v>
-      </c>
-      <c r="M8" s="21">
-        <v>5</v>
-      </c>
-      <c r="N8" s="21">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="O8" s="21">
-        <f>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</f>
-        <v>92</v>
-      </c>
-      <c r="P8" s="26">
-        <f>Tableau24[[#This Row],[KM_Route]]</f>
-        <v>93.7</v>
-      </c>
-      <c r="Q8">
-        <v>46</v>
-      </c>
-      <c r="R8">
-        <v>43</v>
-      </c>
-      <c r="S8" s="25">
-        <v>41</v>
-      </c>
-      <c r="T8" s="20" t="s">
-        <v>209</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{27AC5D4C-3BC2-F545-B17F-1C5289CFF5CB}"/>
-    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{9BD66C34-9BC8-124D-9A01-D34D1D703557}"/>
-    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{C87D0144-957A-804A-AEB4-531610EB899D}"/>
-    <hyperlink ref="T6" r:id="rId4" xr:uid="{8420C6E5-6743-CB48-937E-CA00687573DE}"/>
-    <hyperlink ref="T8" r:id="rId5" xr:uid="{94B4D1BE-E2B6-BA4D-A834-AAAE6B904595}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3601,8 +3147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3615,7 +3161,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3632,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -3647,7 +3193,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3659,10 +3205,10 @@
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3677,7 +3223,7 @@
         <v>7.9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>28</v>
@@ -3698,7 +3244,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="22"/>
     </row>
@@ -3707,7 +3253,7 @@
         <v>12.1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -3722,7 +3268,7 @@
         <v>24.6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>28</v>
@@ -3737,13 +3283,13 @@
         <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F9" s="22"/>
     </row>
@@ -3752,7 +3298,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
@@ -3767,13 +3313,13 @@
         <v>39.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -3788,7 +3334,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12" s="22"/>
     </row>
@@ -3797,13 +3343,13 @@
         <v>55.7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="22"/>
     </row>
@@ -3827,7 +3373,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -3842,10 +3388,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -3857,7 +3403,7 @@
         <v>62.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>52</v>
@@ -3872,13 +3418,13 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="22"/>
     </row>
@@ -3887,13 +3433,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F19" s="22"/>
     </row>
@@ -3908,7 +3454,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="22"/>
     </row>
@@ -3917,7 +3463,7 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -3932,13 +3478,13 @@
         <v>92.5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F22" s="22"/>
     </row>
@@ -3947,7 +3493,7 @@
         <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
@@ -3962,7 +3508,7 @@
         <v>101.2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>50</v>
@@ -3977,7 +3523,7 @@
         <v>101.7</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>49</v>
@@ -3992,7 +3538,7 @@
         <v>104.1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>16</v>
@@ -4007,7 +3553,7 @@
         <v>107.5</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>49</v>
@@ -4022,7 +3568,7 @@
         <v>107.9</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -4037,7 +3583,7 @@
         <v>108</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -4052,7 +3598,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4067,7 +3613,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -4082,7 +3628,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -4097,13 +3643,13 @@
         <v>109.15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F33" s="22"/>
     </row>
@@ -4112,7 +3658,7 @@
         <v>109.35</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>7</v>
@@ -4127,7 +3673,7 @@
         <v>109.75</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
@@ -4142,7 +3688,7 @@
         <v>110.15</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
@@ -4157,7 +3703,7 @@
         <v>110.7</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
@@ -4172,7 +3718,7 @@
         <v>110.75</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>3</v>
@@ -4187,7 +3733,7 @@
         <v>111.2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>41</v>
@@ -4202,7 +3748,7 @@
         <v>114.4</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>42</v>
@@ -4212,18 +3758,18 @@
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>117.6</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F41" s="22"/>
     </row>
@@ -4239,7 +3785,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4252,7 +3798,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4269,13 +3815,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4283,7 +3829,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -4294,10 +3840,10 @@
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4311,7 +3857,7 @@
         <v>7.9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>28</v>
@@ -4331,7 +3877,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4339,7 +3885,7 @@
         <v>12.1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -4353,13 +3899,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4367,7 +3913,7 @@
         <v>24.6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>28</v>
@@ -4381,13 +3927,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4395,7 +3941,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
@@ -4409,13 +3955,13 @@
         <v>39.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4429,7 +3975,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -4437,13 +3983,13 @@
         <v>55.7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4465,7 +4011,7 @@
         <v>61.3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>2</v>
@@ -4479,10 +4025,10 @@
         <v>61.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>54</v>
@@ -4493,7 +4039,7 @@
         <v>62.8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>52</v>
@@ -4507,13 +4053,13 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -4521,13 +4067,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4541,7 +4087,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4549,7 +4095,7 @@
         <v>77.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>16</v>
@@ -4563,13 +4109,13 @@
         <v>92.5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4577,7 +4123,7 @@
         <v>98</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>13</v>
@@ -4591,7 +4137,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4605,7 +4151,7 @@
         <v>101.7</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>49</v>
@@ -4619,7 +4165,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4633,7 +4179,7 @@
         <v>107.5</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>49</v>
@@ -4647,7 +4193,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4661,7 +4207,7 @@
         <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>47</v>
@@ -4675,7 +4221,7 @@
         <v>108.2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
@@ -4689,7 +4235,7 @@
         <v>108.4</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
@@ -4703,7 +4249,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
@@ -4717,13 +4263,13 @@
         <v>109.15</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4731,7 +4277,7 @@
         <v>109.35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>7</v>
@@ -4745,7 +4291,7 @@
         <v>109.75</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>8</v>
@@ -4759,7 +4305,7 @@
         <v>110.15</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -4773,7 +4319,7 @@
         <v>110.7</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
@@ -4787,7 +4333,7 @@
         <v>110.75</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>3</v>
@@ -4801,7 +4347,7 @@
         <v>111.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>41</v>
@@ -4815,7 +4361,7 @@
         <v>114.4</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>42</v>
@@ -4829,13 +4375,13 @@
         <v>115</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4863,7 +4409,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4880,13 +4426,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4894,7 +4440,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4908,7 +4454,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4922,13 +4468,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4956,7 +4502,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4973,13 +4519,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -4988,7 +4534,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -5003,7 +4549,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -5018,13 +4564,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -5305,7 +4851,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -5322,13 +4868,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5336,7 +4882,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -5350,7 +4896,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -5364,13 +4910,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ajout code pour importElevation, maj code et RMD Etape démos
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5EC3D8-069E-4B41-B239-9D9233107A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA9F921-AF26-3B4D-BFAF-43D0A2A87DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -291,9 +291,6 @@
     <t>10.0 km</t>
   </si>
   <si>
-    <t>Val-d'OR - Amos</t>
-  </si>
-  <si>
     <t>95.3 km + (4 x 5.4 km) = 116.9 km</t>
   </si>
   <si>
@@ -700,6 +697,9 @@
   </si>
   <si>
     <t>Arrivée&lt;br/&gt;Bonification en temps et points</t>
+  </si>
+  <si>
+    <t>Val-d'Or - Amos</t>
   </si>
 </sst>
 </file>
@@ -1654,17 +1654,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
@@ -1697,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -1714,13 +1714,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -1729,7 +1729,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -1744,7 +1744,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1759,13 +1759,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2046,7 +2046,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2063,13 +2063,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2078,7 +2078,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2093,7 +2093,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2107,13 +2107,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2145,66 +2145,66 @@
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2212,7 +2212,7 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>62</v>
@@ -2226,7 +2226,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2237,156 +2237,156 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" t="s">
         <v>167</v>
-      </c>
-      <c r="D18" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2436,16 +2436,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2460,25 +2460,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
         <v>177</v>
       </c>
-      <c r="K1" t="s">
-        <v>178</v>
-      </c>
       <c r="L1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" t="s">
         <v>180</v>
       </c>
-      <c r="N1" t="s">
-        <v>205</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -2490,7 +2490,7 @@
         <v>67</v>
       </c>
       <c r="T1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
@@ -2498,22 +2498,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -2556,7 +2556,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
@@ -2564,22 +2564,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>76</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -2622,7 +2622,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
@@ -2630,16 +2630,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s">
         <v>73</v>
@@ -2687,7 +2687,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
@@ -2695,22 +2695,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -2753,7 +2753,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
@@ -2761,22 +2761,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -2819,7 +2819,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
@@ -2827,22 +2827,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -2885,7 +2885,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
@@ -2893,22 +2893,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>80</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>81</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -2951,7 +2951,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3009,16 +3009,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -3033,25 +3033,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
         <v>177</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>178</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
         <v>179</v>
       </c>
-      <c r="M1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>180</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>182</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -3063,7 +3063,7 @@
         <v>67</v>
       </c>
       <c r="T1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
@@ -3071,22 +3071,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="27">
         <v>43661</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3128,7 +3128,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3147,7 +3147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -3161,7 +3161,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3178,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -3193,7 +3193,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3208,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3283,13 +3283,13 @@
         <v>27</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="F9" s="22"/>
     </row>
@@ -3313,13 +3313,13 @@
         <v>39.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -3343,7 +3343,7 @@
         <v>55.7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
@@ -3373,7 +3373,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -3388,10 +3388,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -3418,7 +3418,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -3433,13 +3433,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="F19" s="22"/>
     </row>
@@ -3463,7 +3463,7 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -3478,13 +3478,13 @@
         <v>92.5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="F22" s="22"/>
     </row>
@@ -3508,7 +3508,7 @@
         <v>101.2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>50</v>
@@ -3538,7 +3538,7 @@
         <v>104.1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>16</v>
@@ -3568,7 +3568,7 @@
         <v>107.9</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -3583,7 +3583,7 @@
         <v>108</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -3598,7 +3598,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -3613,7 +3613,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -3628,7 +3628,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -3643,13 +3643,13 @@
         <v>109.15</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="F33" s="22"/>
     </row>
@@ -3658,7 +3658,7 @@
         <v>109.35</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>7</v>
@@ -3673,7 +3673,7 @@
         <v>109.75</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
@@ -3688,7 +3688,7 @@
         <v>110.15</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
@@ -3703,7 +3703,7 @@
         <v>110.7</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
@@ -3718,7 +3718,7 @@
         <v>110.75</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>3</v>
@@ -3733,7 +3733,7 @@
         <v>111.2</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>41</v>
@@ -3748,7 +3748,7 @@
         <v>114.4</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>42</v>
@@ -3763,13 +3763,13 @@
         <v>117.6</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F41" s="22"/>
     </row>
@@ -3798,7 +3798,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -3829,7 +3829,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3843,7 +3843,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3899,13 +3899,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3927,13 +3927,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3955,13 +3955,13 @@
         <v>39.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3983,13 +3983,13 @@
         <v>55.7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4011,7 +4011,7 @@
         <v>61.3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>2</v>
@@ -4025,10 +4025,10 @@
         <v>61.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>54</v>
@@ -4053,7 +4053,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4067,13 +4067,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4095,7 +4095,7 @@
         <v>77.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>16</v>
@@ -4109,13 +4109,13 @@
         <v>92.5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4137,7 +4137,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4165,7 +4165,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4193,7 +4193,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4207,7 +4207,7 @@
         <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>47</v>
@@ -4221,7 +4221,7 @@
         <v>108.2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
@@ -4235,7 +4235,7 @@
         <v>108.4</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
@@ -4249,7 +4249,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
@@ -4263,13 +4263,13 @@
         <v>109.15</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C34" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4277,7 +4277,7 @@
         <v>109.35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>7</v>
@@ -4291,7 +4291,7 @@
         <v>109.75</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>8</v>
@@ -4305,7 +4305,7 @@
         <v>110.15</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -4319,7 +4319,7 @@
         <v>110.7</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
@@ -4333,7 +4333,7 @@
         <v>110.75</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>3</v>
@@ -4347,7 +4347,7 @@
         <v>111.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>41</v>
@@ -4361,7 +4361,7 @@
         <v>114.4</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>42</v>
@@ -4375,13 +4375,13 @@
         <v>115</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4409,7 +4409,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4426,13 +4426,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4440,7 +4440,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4454,7 +4454,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4468,13 +4468,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4502,7 +4502,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4519,13 +4519,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -4534,7 +4534,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4549,7 +4549,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4564,13 +4564,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -4851,7 +4851,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4868,13 +4868,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4882,7 +4882,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4896,7 +4896,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4910,13 +4910,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ajstement etape1 pour avoir info 2022
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA9F921-AF26-3B4D-BFAF-43D0A2A87DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2889E53-3910-1940-A885-D743702B07B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="560" windowWidth="51100" windowHeight="28180" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="208">
   <si>
     <t>GPM</t>
   </si>
@@ -342,36 +342,12 @@
     <t>Utiliser '&lt;br/&gt;' pour indiquer un saut de ligne dans le tableau des détails</t>
   </si>
   <si>
-    <t>Bonus sprint time and points&lt;br/&gt;(3-2-1 sec; 6-4-2 pts)&lt;br/&gt;(Chemin Lac Normand)</t>
-  </si>
-  <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;(3-2-1 sec; 6-4-2 pts)&lt;br/&gt;(Chemin Lac Normand)</t>
-  </si>
-  <si>
-    <t>GPM Points (5-3-2)&lt;br/&gt;(Chemin Bousquet)</t>
-  </si>
-  <si>
-    <t>KOM Points (5-3-2)&lt;br/&gt;(Chemin Bousquet)</t>
-  </si>
-  <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;(3-2-1 sec; 6-4-2 pts) (km 544)</t>
-  </si>
-  <si>
-    <t>Bonus sprint time and points&lt;br/&gt;(3-2-1 sec; 6-4-2 pts) (km 544)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sprint du maire de Rouyn-Noranda - $250&lt;br/&gt;(École St-Philippe sur la traverse piétons) </t>
   </si>
   <si>
     <t xml:space="preserve">Mayor's sprint - $250&lt;br/&gt;(École St-Philippe sur la traverse piétons) </t>
   </si>
   <si>
-    <t>GPM Points (5-3-2)&lt;br/&gt;(Rue Brébeuf)</t>
-  </si>
-  <si>
-    <t>KOM Points (5-3-2)&lt;br/&gt;(Rue Brébeuf)</t>
-  </si>
-  <si>
     <t>Info_FR</t>
   </si>
   <si>
@@ -700,6 +676,18 @@
   </si>
   <si>
     <t>Val-d'Or - Amos</t>
+  </si>
+  <si>
+    <t>GPM Points&lt;br/&gt;(Sortie Cléricy)</t>
+  </si>
+  <si>
+    <t>GPM Points&lt;br/&gt;(Côte Lac Dufault)</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Halte Trecesson)</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Halte Trécesson)</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1652,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
@@ -1697,7 +1685,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -1714,13 +1702,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -1729,7 +1717,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -1744,7 +1732,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1759,13 +1747,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2046,7 +2034,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2063,13 +2051,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2078,7 +2066,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2093,7 +2081,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2107,13 +2095,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2145,66 +2133,66 @@
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2212,7 +2200,7 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>62</v>
@@ -2226,7 +2214,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2237,156 +2225,156 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -2436,16 +2424,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
         <v>182</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>190</v>
       </c>
-      <c r="D1" t="s">
-        <v>198</v>
-      </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2460,25 +2448,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="L1" t="s">
         <v>89</v>
       </c>
       <c r="M1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="O1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -2498,22 +2486,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
         <v>183</v>
-      </c>
-      <c r="C2" t="s">
-        <v>191</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -2564,19 +2552,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" t="s">
         <v>184</v>
-      </c>
-      <c r="C3" t="s">
-        <v>192</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>75</v>
@@ -2630,16 +2618,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" t="s">
         <v>185</v>
-      </c>
-      <c r="C4" t="s">
-        <v>193</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F4" t="s">
         <v>73</v>
@@ -2695,22 +2683,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" t="s">
         <v>186</v>
-      </c>
-      <c r="C5" t="s">
-        <v>194</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -2761,22 +2749,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
         <v>187</v>
-      </c>
-      <c r="C6" t="s">
-        <v>195</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F6" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -2827,22 +2815,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
         <v>188</v>
-      </c>
-      <c r="C7" t="s">
-        <v>196</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -2893,16 +2881,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
         <v>189</v>
-      </c>
-      <c r="C8" t="s">
-        <v>197</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F8" t="s">
         <v>79</v>
@@ -3009,16 +2997,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
         <v>182</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>190</v>
       </c>
-      <c r="D1" t="s">
-        <v>198</v>
-      </c>
       <c r="E1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -3033,25 +3021,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="K1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="L1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="M1" t="s">
         <v>89</v>
       </c>
       <c r="N1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="O1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -3071,22 +3059,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
         <v>188</v>
-      </c>
-      <c r="C2" t="s">
-        <v>196</v>
       </c>
       <c r="D2" s="27">
         <v>43661</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F2" t="s">
         <v>79</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3128,7 +3116,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3145,10 +3133,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3161,7 +3149,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3178,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -3193,7 +3181,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3208,7 +3196,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3265,7 +3253,7 @@
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
-        <v>24.6</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>62</v>
@@ -3280,46 +3268,46 @@
     </row>
     <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
-        <v>27</v>
+        <v>13.4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>95</v>
+        <v>205</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>205</v>
       </c>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>35</v>
+        <v>34.6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>14</v>
+        <v>146</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>204</v>
       </c>
       <c r="F10" s="22"/>
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
-        <v>39.5</v>
+        <v>45.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>92</v>
+        <v>132</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -3340,10 +3328,10 @@
     </row>
     <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
-        <v>55.7</v>
+        <v>62.8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
@@ -3373,7 +3361,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -3388,10 +3376,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -3418,7 +3406,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -3428,129 +3416,130 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>76.900000000000006</v>
+        <v>77.5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>97</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>77.5</v>
+        <v>77.8</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>59</v>
+        <v>157</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>77.8</v>
+        <v>98</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>92.5</v>
+        <v>101.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>98</v>
+        <v>101.2</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
-        <v>101.2</v>
+        <v>101.7</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>160</v>
+        <v>62</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F24" s="22"/>
     </row>
     <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
-        <v>101.7</v>
+        <v>104.1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
-        <v>104.1</v>
+        <v>119</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>17</v>
+        <v>145</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
-        <v>107.5</v>
+        <f>A26+1</f>
+        <v>120</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>62</v>
@@ -3565,10 +3554,11 @@
     </row>
     <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
-        <v>107.9</v>
+        <f t="shared" ref="A28:A39" si="0">A27+1</f>
+        <v>121</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -3580,10 +3570,11 @@
     </row>
     <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
-        <v>108</v>
+        <f t="shared" si="0"/>
+        <v>122</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -3595,10 +3586,11 @@
     </row>
     <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>108.2</v>
+        <f t="shared" si="0"/>
+        <v>123</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -3610,10 +3602,11 @@
     </row>
     <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>108.4</v>
+        <f t="shared" si="0"/>
+        <v>124</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -3625,10 +3618,11 @@
     </row>
     <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>109</v>
+        <f t="shared" si="0"/>
+        <v>125</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -3639,141 +3633,133 @@
       <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="9">
-        <v>109.15</v>
+      <c r="A33" s="3">
+        <f t="shared" si="0"/>
+        <v>126</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>101</v>
+        <v>151</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="9">
-        <v>109.35</v>
+      <c r="A34" s="3">
+        <f t="shared" si="0"/>
+        <v>127</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="9">
-        <v>109.75</v>
+      <c r="A35" s="3">
+        <f t="shared" si="0"/>
+        <v>128</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="9">
-        <v>110.15</v>
+      <c r="A36" s="3">
+        <f t="shared" si="0"/>
+        <v>129</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
-        <v>110.7</v>
+        <f t="shared" si="0"/>
+        <v>130</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F37" s="22"/>
     </row>
     <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="9">
-        <v>110.75</v>
+      <c r="A38" s="3">
+        <f t="shared" si="0"/>
+        <v>131</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
-        <v>111.2</v>
+        <f t="shared" si="0"/>
+        <v>132</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>44</v>
+        <v>136.69999999999999</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A41" s="3">
-        <v>117.6</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3798,7 +3784,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3815,7 +3801,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -3829,7 +3815,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3843,7 +3829,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3899,13 +3885,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3927,13 +3913,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3955,13 +3941,13 @@
         <v>39.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3983,13 +3969,13 @@
         <v>55.7</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4011,7 +3997,7 @@
         <v>61.3</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>2</v>
@@ -4025,10 +4011,10 @@
         <v>61.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>54</v>
@@ -4053,7 +4039,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4067,13 +4053,13 @@
         <v>76.900000000000006</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4095,7 +4081,7 @@
         <v>77.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>16</v>
@@ -4109,13 +4095,13 @@
         <v>92.5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4137,7 +4123,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4165,7 +4151,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4193,7 +4179,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4207,7 +4193,7 @@
         <v>108</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>47</v>
@@ -4221,7 +4207,7 @@
         <v>108.2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
@@ -4235,7 +4221,7 @@
         <v>108.4</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
@@ -4249,7 +4235,7 @@
         <v>109</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
@@ -4263,13 +4249,13 @@
         <v>109.15</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4277,7 +4263,7 @@
         <v>109.35</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>7</v>
@@ -4291,7 +4277,7 @@
         <v>109.75</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>8</v>
@@ -4305,7 +4291,7 @@
         <v>110.15</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
@@ -4319,7 +4305,7 @@
         <v>110.7</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>9</v>
@@ -4333,7 +4319,7 @@
         <v>110.75</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>3</v>
@@ -4347,7 +4333,7 @@
         <v>111.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>41</v>
@@ -4361,7 +4347,7 @@
         <v>114.4</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>42</v>
@@ -4375,13 +4361,13 @@
         <v>115</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4409,7 +4395,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4426,13 +4412,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4440,7 +4426,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4454,7 +4440,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4468,13 +4454,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4502,7 +4488,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4519,13 +4505,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -4534,7 +4520,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4549,7 +4535,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4564,13 +4550,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -4851,7 +4837,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4868,13 +4854,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4882,7 +4868,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4896,7 +4882,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4910,13 +4896,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Finalisation des graphiques d'élévation
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2889E53-3910-1940-A885-D743702B07B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB607404-4335-174F-819C-CEB8CA5DD90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="560" windowWidth="51100" windowHeight="28180" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="214">
   <si>
     <t>GPM</t>
   </si>
@@ -444,12 +444,6 @@
     <t>Points GPM (Chemin Bousquet)</t>
   </si>
   <si>
-    <t>Points GPM - Rue Brébeuf</t>
-  </si>
-  <si>
-    <t>KOM points- Rue Brébeuf</t>
-  </si>
-  <si>
     <t>Arrivée Finale&lt;br/&gt;Bonification temps et points</t>
   </si>
   <si>
@@ -471,12 +465,6 @@
     <t>KOM Points (Chemin Bousquet)</t>
   </si>
   <si>
-    <t>Sprint du maire de Rouyn-Noranda - $250&lt;br/&gt;(mine Lapa)</t>
-  </si>
-  <si>
-    <t>Mayor's sprint - $250&lt;br/&gt;(mine Lapa)</t>
-  </si>
-  <si>
     <t>Départ</t>
   </si>
   <si>
@@ -688,6 +676,36 @@
   </si>
   <si>
     <t>Sprint bonification temps et points&lt;br/&gt;(Halte Trécesson)</t>
+  </si>
+  <si>
+    <t>GPM - Flat de Landirenne</t>
+  </si>
+  <si>
+    <t>KOM - Landrienne's flat</t>
+  </si>
+  <si>
+    <t>Bypass</t>
+  </si>
+  <si>
+    <t>Caravan bypass on the right</t>
+  </si>
+  <si>
+    <t>Déviation Caravane</t>
+  </si>
+  <si>
+    <t>Caravan Bypass</t>
+  </si>
+  <si>
+    <t>&amp;#9936;</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Rouyn-Noranda - $250&lt;br/&gt;Début du 2e tour</t>
+  </si>
+  <si>
+    <t>Mayor's sprint - $250&lt;br/&gt;Start of 2nd lap</t>
+  </si>
+  <si>
+    <t>Déviation de la caravane sur la droite</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1650,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1702,13 +1720,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -1717,7 +1735,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -1732,7 +1750,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1750,10 +1768,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2051,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2066,7 +2084,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2081,7 +2099,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2098,10 +2116,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2112,10 +2130,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2141,7 +2159,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
@@ -2155,7 +2173,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
         <v>118</v>
@@ -2169,7 +2187,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
         <v>119</v>
@@ -2214,7 +2232,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2225,7 +2243,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
         <v>121</v>
@@ -2239,7 +2257,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>120</v>
@@ -2253,7 +2271,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>115</v>
@@ -2267,10 +2285,10 @@
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
@@ -2281,10 +2299,10 @@
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>112</v>
@@ -2295,10 +2313,10 @@
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>113</v>
@@ -2309,10 +2327,10 @@
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
@@ -2323,10 +2341,10 @@
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
@@ -2337,7 +2355,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
         <v>114</v>
@@ -2351,7 +2369,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
         <v>114</v>
@@ -2365,16 +2383,30 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2391,7 +2423,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2424,16 +2456,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2448,25 +2480,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
         <v>89</v>
       </c>
       <c r="M1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="N1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="O1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -2486,22 +2518,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -2552,19 +2584,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>75</v>
@@ -2618,16 +2650,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
         <v>73</v>
@@ -2683,22 +2715,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -2749,22 +2781,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F6" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -2815,22 +2847,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -2881,16 +2913,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
         <v>79</v>
@@ -2997,16 +3029,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -3021,25 +3053,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="K1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M1" t="s">
         <v>89</v>
       </c>
       <c r="N1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -3059,22 +3091,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D2" s="27">
         <v>43661</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>79</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3116,7 +3148,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3135,8 +3167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3166,7 +3198,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -3181,7 +3213,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3196,7 +3228,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3271,28 +3303,28 @@
         <v>13.4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F9" s="22"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>34.6</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F10" s="22"/>
     </row>
@@ -3301,13 +3333,13 @@
         <v>45.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -3331,7 +3363,7 @@
         <v>62.8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
@@ -3361,7 +3393,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -3376,10 +3408,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -3406,7 +3438,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -3436,7 +3468,7 @@
         <v>77.8</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
@@ -3466,7 +3498,7 @@
         <v>101.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>92</v>
@@ -3481,7 +3513,7 @@
         <v>101.2</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>50</v>
@@ -3511,7 +3543,7 @@
         <v>104.1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>16</v>
@@ -3526,13 +3558,13 @@
         <v>119</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F26" s="22"/>
     </row>
@@ -3558,7 +3590,7 @@
         <v>121</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -3574,7 +3606,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -3590,7 +3622,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -3606,7 +3638,7 @@
         <v>124</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -3622,7 +3654,7 @@
         <v>125</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -3638,7 +3670,7 @@
         <v>126</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -3654,7 +3686,7 @@
         <v>127</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -3670,7 +3702,7 @@
         <v>128</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -3686,7 +3718,7 @@
         <v>129</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -3702,7 +3734,7 @@
         <v>130</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -3718,7 +3750,7 @@
         <v>131</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>41</v>
@@ -3734,7 +3766,7 @@
         <v>132</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>42</v>
@@ -3752,7 +3784,7 @@
         <v>100</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>111</v>
@@ -3768,10 +3800,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3801,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -3815,7 +3847,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3829,7 +3861,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3885,13 +3917,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3910,16 +3942,16 @@
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>125</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3938,16 +3970,16 @@
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
-        <v>39.5</v>
+        <v>47.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -3964,82 +3996,82 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>55.7</v>
+        <v>61</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>136</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
-        <v>61</v>
+        <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>61.3</v>
+        <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
-        <v>61.8</v>
+        <v>62.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
-        <v>62.8</v>
+        <v>72.7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>53</v>
+        <v>142</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>72.400000000000006</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4048,74 +4080,75 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
-        <v>76.900000000000006</v>
+        <v>77.5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>130</v>
+        <v>19</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
-        <v>77.5</v>
+        <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
-        <v>77.8</v>
+        <v>81.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
-        <v>92.5</v>
+        <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <f>A38-3.2</f>
+        <v>108</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D24" s="17" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="3">
-        <v>98</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4123,7 +4156,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4151,7 +4184,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4179,7 +4212,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4190,187 +4223,173 @@
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
-        <v>108</v>
+        <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
-        <v>108.2</v>
+        <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
-        <v>108.4</v>
+        <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="3">
-        <v>109</v>
+      <c r="A33" s="9">
+        <v>109.35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
-        <v>109.15</v>
+        <v>109.75</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>127</v>
+        <v>147</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
-        <v>109.35</v>
+        <v>110.15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="9">
-        <v>109.75</v>
+      <c r="A36" s="3">
+        <v>110.7</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="9">
-        <v>110.15</v>
+        <v>110.75</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
-        <v>110.7</v>
+        <v>111.2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="9">
-        <v>110.75</v>
+      <c r="A39" s="3">
+        <v>114.4</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
-        <v>111.2</v>
+        <v>118.7</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>41</v>
+        <v>213</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A42" s="3">
-        <v>115</v>
-      </c>
-      <c r="B42" s="13" t="s">
+        <v>119.9</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="C41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4412,13 +4431,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4426,7 +4445,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4440,7 +4459,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4457,10 +4476,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4505,13 +4524,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -4520,7 +4539,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4535,7 +4554,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4553,10 +4572,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -4854,13 +4873,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4868,7 +4887,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4882,7 +4901,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4899,10 +4918,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ajout organisation Snakefile, closes #2
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB607404-4335-174F-819C-CEB8CA5DD90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3E2739-E74D-BC47-BBED-175DD5854908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="215">
   <si>
     <t>GPM</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>Déviation de la caravane sur la droite</t>
+  </si>
+  <si>
+    <t>Pont de bois en feu</t>
   </si>
 </sst>
 </file>
@@ -3167,8 +3170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3426,7 +3429,7 @@
         <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>214</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>53</v>
@@ -3802,7 +3805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modif liens entre fichier Excel pour horaire, ref issue #7
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\guide2023\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3E2739-E74D-BC47-BBED-175DD5854908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F7CB8-B79D-44CA-9859-ECE766B597D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33075" yWindow="660" windowWidth="35910" windowHeight="19680" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="221">
   <si>
     <t>GPM</t>
   </si>
@@ -710,13 +710,32 @@
   <si>
     <t>Pont de bois en feu</t>
   </si>
+  <si>
+    <t>Delai Signature</t>
+  </si>
+  <si>
+    <t>Heure_Navette</t>
+  </si>
+  <si>
+    <t>Delai Preparation</t>
+  </si>
+  <si>
+    <t>Temps Transport</t>
+  </si>
+  <si>
+    <t>Heure Signature</t>
+  </si>
+  <si>
+    <t>Heure Arrivee</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -813,7 +832,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -856,12 +875,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -922,12 +950,21 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1022,6 +1059,32 @@
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="double">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <right style="thin">
           <color indexed="64"/>
         </right>
         <top/>
@@ -1239,7 +1302,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
@@ -1252,39 +1315,54 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:T8" totalsRowShown="0">
-  <autoFilter ref="A1:T8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:AA8" totalsRowShown="0">
+  <autoFilter ref="A1:AA8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+  <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{F159CC0E-186F-4E03-998F-71303E6AFF37}" name="Etape"/>
     <tableColumn id="19" xr3:uid="{3543EB43-316C-0F44-B3AA-B931646E7365}" name="Jour"/>
     <tableColumn id="18" xr3:uid="{0D4EFF62-DD86-2240-BAFF-EEDA66BC4B15}" name="Day"/>
     <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
     <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="25"/>
     <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="14">
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="22">
       <calculatedColumnFormula>P2-O2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="13">
+    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="21">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="12">
+    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="20">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="11">
+    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="19">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="17">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataDxfId="16" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="21" xr3:uid="{F2204A86-7E8B-4F1F-89A0-9523DD2193D9}" name="Départ" dataDxfId="15">
+      <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{2B5A63D9-26DC-4A28-8248-6E6EA5709678}" name="Temps Transport" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{F7C0E5F3-60BA-4A5C-949D-A330E373C447}" name="Delai Preparation" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{B5478C0D-EFC2-4CDA-831C-0997C386A960}" name="Delai Signature" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="11">
+      <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="1">
+      <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="Heure Arrivee" dataDxfId="0">
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1300,27 +1378,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="6">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="5">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="4">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="2">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -1332,7 +1410,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1370,7 +1448,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1476,7 +1554,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1656,30 +1734,30 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
     </row>
   </sheetData>
@@ -1696,15 +1774,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -1718,7 +1796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -1733,7 +1811,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -1748,7 +1826,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -1763,7 +1841,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -1778,259 +1856,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2045,15 +2123,15 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -2067,7 +2145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2082,7 +2160,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -2111,7 +2189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -2139,14 +2217,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
@@ -2160,7 +2238,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2174,7 +2252,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -2188,7 +2266,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -2202,7 +2280,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -2216,7 +2294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -2230,7 +2308,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2244,7 +2322,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -2258,7 +2336,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2272,7 +2350,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -2286,7 +2364,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -2300,7 +2378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -2314,7 +2392,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2328,7 +2406,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -2342,7 +2420,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -2356,7 +2434,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -2370,7 +2448,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -2384,7 +2462,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -2398,7 +2476,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>206</v>
       </c>
@@ -2423,38 +2501,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="14.83203125" customWidth="1"/>
-    <col min="24" max="24" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="39" customWidth="1"/>
+    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.125" style="30" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -2512,11 +2593,32 @@
       <c r="S1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="30" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V1" t="s">
+        <v>218</v>
+      </c>
+      <c r="W1" t="s">
+        <v>217</v>
+      </c>
+      <c r="X1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2578,11 +2680,36 @@
         <f>IF(R2&gt;0,R2-2,"")</f>
         <v>42</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="31" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U2" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>16:15</v>
+      </c>
+      <c r="V2" s="32">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="W2" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="X2" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y2" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="Z2" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="AA2" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.80653409090909089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2644,11 +2771,36 @@
         <f>IF(R3&gt;0,R3-2,"")</f>
         <v>42</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U3" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>16:45</v>
+      </c>
+      <c r="V3" s="32">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="W3" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="X3" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y3" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.59374999999999989</v>
+      </c>
+      <c r="Z3" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AA3" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.81145833333333328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2709,11 +2861,34 @@
       <c r="S4" s="25">
         <v>42</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="T4" s="31" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>9:0</v>
+      </c>
+      <c r="V4" s="32">
+        <v>0</v>
+      </c>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="Y4" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="Z4" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="AA4" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.38425925925925924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2775,11 +2950,36 @@
         <f>IF(R5&gt;0,R5-2,"")</f>
         <v>44</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="T5" s="31" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U5" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>18:15</v>
+      </c>
+      <c r="V5" s="32">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W5" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="X5" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y5" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.65625</v>
+      </c>
+      <c r="Z5" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="AA5" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.81422101449275353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2841,11 +3041,36 @@
         <f>IF(R6&gt;0,R6-2,"")</f>
         <v>41</v>
       </c>
-      <c r="T6" s="20" t="s">
+      <c r="T6" s="31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U6" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>14:0</v>
+      </c>
+      <c r="V6" s="32">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="W6" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="X6" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y6" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.45833333333333343</v>
+      </c>
+      <c r="Z6" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="AA6" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.72383720930232565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2907,11 +3132,36 @@
         <f t="shared" ref="S7:S8" si="1">IF(R7&gt;0,R7-2,"")</f>
         <v>41</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="U7" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>16:30</v>
+      </c>
+      <c r="V7" s="32">
+        <v>0</v>
+      </c>
+      <c r="W7" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="X7" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y7" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="Z7" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.65625</v>
+      </c>
+      <c r="AA7" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.80271317829457367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2973,8 +3223,33 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="31" t="s">
         <v>88</v>
+      </c>
+      <c r="U8" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <v>14:30</v>
+      </c>
+      <c r="V8" s="32">
+        <v>0</v>
+      </c>
+      <c r="W8" s="32">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="X8" s="32">
+        <v>3.125E-2</v>
+      </c>
+      <c r="Y8" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <v>0.55208333333333326</v>
+      </c>
+      <c r="Z8" s="32">
+        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="AA8" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
+        <v>0.70881782945736427</v>
       </c>
     </row>
   </sheetData>
@@ -3001,33 +3276,33 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.83203125" customWidth="1"/>
-    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.875" customWidth="1"/>
+    <col min="23" max="23" width="38.125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -3089,7 +3364,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>8</v>
       </c>
@@ -3170,19 +3445,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -3196,7 +3471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3211,7 +3486,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -3226,7 +3501,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>5</v>
       </c>
@@ -3241,7 +3516,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -3256,7 +3531,7 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -3271,7 +3546,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -3286,7 +3561,7 @@
       </c>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -3301,7 +3576,7 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>13.4</v>
       </c>
@@ -3316,7 +3591,7 @@
       </c>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>34.700000000000003</v>
       </c>
@@ -3331,7 +3606,7 @@
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>45.5</v>
       </c>
@@ -3346,7 +3621,7 @@
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.4</v>
       </c>
@@ -3361,7 +3636,7 @@
       </c>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>62.8</v>
       </c>
@@ -3376,7 +3651,7 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -3391,7 +3666,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -3406,7 +3681,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -3421,7 +3696,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -3436,7 +3711,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -3451,7 +3726,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>77.5</v>
       </c>
@@ -3466,7 +3741,7 @@
       </c>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.8</v>
       </c>
@@ -3481,7 +3756,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>98</v>
       </c>
@@ -3496,7 +3771,7 @@
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>101.1</v>
       </c>
@@ -3511,7 +3786,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>101.2</v>
       </c>
@@ -3526,7 +3801,7 @@
       </c>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>101.7</v>
       </c>
@@ -3541,7 +3816,7 @@
       </c>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>104.1</v>
       </c>
@@ -3556,7 +3831,7 @@
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>119</v>
       </c>
@@ -3571,7 +3846,7 @@
       </c>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <f>A26+1</f>
         <v>120</v>
@@ -3587,7 +3862,7 @@
       </c>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <f t="shared" ref="A28:A39" si="0">A27+1</f>
         <v>121</v>
@@ -3603,7 +3878,7 @@
       </c>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -3619,7 +3894,7 @@
       </c>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -3635,7 +3910,7 @@
       </c>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -3651,7 +3926,7 @@
       </c>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -3667,7 +3942,7 @@
       </c>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -3683,7 +3958,7 @@
       </c>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>127</v>
@@ -3699,7 +3974,7 @@
       </c>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3715,7 +3990,7 @@
       </c>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>129</v>
@@ -3731,7 +4006,7 @@
       </c>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>130</v>
@@ -3747,7 +4022,7 @@
       </c>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -3763,7 +4038,7 @@
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>132</v>
@@ -3779,7 +4054,7 @@
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>136.69999999999999</v>
       </c>
@@ -3794,7 +4069,7 @@
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3809,15 +4084,15 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -3831,7 +4106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3845,7 +4120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -3859,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3873,7 +4148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -3887,7 +4162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -3901,7 +4176,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -3915,7 +4190,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -3929,7 +4204,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>24.6</v>
       </c>
@@ -3943,7 +4218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -3957,7 +4232,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -3971,7 +4246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.5</v>
       </c>
@@ -3985,7 +4260,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>47.4</v>
       </c>
@@ -3999,7 +4274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -4013,7 +4288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -4027,7 +4302,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -4041,7 +4316,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -4055,7 +4330,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.7</v>
       </c>
@@ -4069,7 +4344,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>74.400000000000006</v>
       </c>
@@ -4083,7 +4358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.5</v>
       </c>
@@ -4097,7 +4372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>77.8</v>
       </c>
@@ -4111,7 +4386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>81.8</v>
       </c>
@@ -4125,7 +4400,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>98</v>
       </c>
@@ -4139,7 +4414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <f>A38-3.2</f>
         <v>108</v>
@@ -4154,7 +4429,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>101.2</v>
       </c>
@@ -4168,7 +4443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>101.7</v>
       </c>
@@ -4182,7 +4457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>104.1</v>
       </c>
@@ -4196,7 +4471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>107.5</v>
       </c>
@@ -4210,7 +4485,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>107.9</v>
       </c>
@@ -4224,7 +4499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>108.2</v>
       </c>
@@ -4238,7 +4513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>108.4</v>
       </c>
@@ -4252,7 +4527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>109</v>
       </c>
@@ -4266,7 +4541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>109.35</v>
       </c>
@@ -4280,7 +4555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>109.75</v>
       </c>
@@ -4294,7 +4569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>110.15</v>
       </c>
@@ -4308,7 +4583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>110.7</v>
       </c>
@@ -4322,7 +4597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="9">
         <v>110.75</v>
       </c>
@@ -4336,7 +4611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>111.2</v>
       </c>
@@ -4350,7 +4625,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>114.4</v>
       </c>
@@ -4364,7 +4639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>118.7</v>
       </c>
@@ -4378,7 +4653,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>119.9</v>
       </c>
@@ -4392,7 +4667,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4407,15 +4682,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4429,7 +4704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4443,7 +4718,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4457,7 +4732,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4471,7 +4746,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4485,7 +4760,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4500,15 +4775,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4522,7 +4797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4537,7 +4812,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4552,7 +4827,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4567,7 +4842,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4582,259 +4857,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4849,15 +5124,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4871,7 +5146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4885,7 +5160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4899,7 +5174,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4913,7 +5188,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4927,223 +5202,223 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
     </row>
-    <row r="34" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modif excel pour lier heures a feuille de route, pour issu #7
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\guide2023\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508F7CB8-B79D-44CA-9859-ECE766B597D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB84429-71D6-9C4C-B6E0-2E7C53C5644C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33075" yWindow="660" windowWidth="35910" windowHeight="19680" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -960,12 +960,6 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1066,6 +1060,12 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1357,10 +1357,10 @@
     <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="11">
       <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="1">
+    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="10">
       <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="Heure Arrivee" dataDxfId="0">
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="Heure Arrivee" dataDxfId="9">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1378,27 +1378,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="5">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -1410,7 +1410,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1448,7 +1448,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1554,7 +1554,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1734,30 +1734,30 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="24"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="24"/>
     </row>
   </sheetData>
@@ -1774,15 +1774,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -1856,259 +1856,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2123,15 +2123,15 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -2217,14 +2217,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>151</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>147</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>206</v>
       </c>
@@ -2503,39 +2503,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.125" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" style="30" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>0.80653409090909089</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0.81145833333333328</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0.38425925925925924</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>0.81422101449275353</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0.72383720930232565</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0.80271317829457367</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3276,33 +3276,33 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.875" customWidth="1"/>
-    <col min="23" max="23" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>8</v>
       </c>
@@ -3449,15 +3449,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>5</v>
       </c>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -3546,7 +3546,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>13.4</v>
       </c>
@@ -3591,7 +3591,7 @@
       </c>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>34.700000000000003</v>
       </c>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>45.5</v>
       </c>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.4</v>
       </c>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>62.8</v>
       </c>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -3696,7 +3696,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>77.5</v>
       </c>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.8</v>
       </c>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>98</v>
       </c>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>101.1</v>
       </c>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>101.2</v>
       </c>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>101.7</v>
       </c>
@@ -3816,7 +3816,7 @@
       </c>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>104.1</v>
       </c>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>119</v>
       </c>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <f>A26+1</f>
         <v>120</v>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <f t="shared" ref="A28:A39" si="0">A27+1</f>
         <v>121</v>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>122</v>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>123</v>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>124</v>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>125</v>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>126</v>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>127</v>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>129</v>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>130</v>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>131</v>
@@ -4038,7 +4038,7 @@
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>132</v>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>136.69999999999999</v>
       </c>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4084,15 +4084,15 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>24.6</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.5</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>47.4</v>
       </c>
@@ -4274,7 +4274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
@@ -4316,7 +4316,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.7</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>74.400000000000006</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.5</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>77.8</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>81.8</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>98</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <f>A38-3.2</f>
         <v>108</v>
@@ -4429,7 +4429,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>101.2</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>101.7</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>104.1</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>107.5</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>107.9</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>108.2</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>108.4</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>109</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>109.35</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>109.75</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>110.15</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>110.7</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="9">
         <v>110.75</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>111.2</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>114.4</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>118.7</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>119.9</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4682,15 +4682,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4775,15 +4775,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -4827,7 +4827,7 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -4842,7 +4842,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -4857,259 +4857,259 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5124,15 +5124,15 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>124</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
@@ -5202,223 +5202,223 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fin modification feuilles de route, closes #7
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB84429-71D6-9C4C-B6E0-2E7C53C5644C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238BAEB5-2D9C-2B46-8704-37AD33883475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2503,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2826,7 +2826,7 @@
         <v>9</v>
       </c>
       <c r="I4" s="25">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="U4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
-        <v>9:0</v>
+        <v>9:30</v>
       </c>
       <c r="V4" s="32">
         <v>0</v>
@@ -2877,15 +2877,15 @@
       </c>
       <c r="Y4" s="32">
         <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
-        <v>0.36458333333333331</v>
+        <v>0.38541666666666663</v>
       </c>
       <c r="Z4" s="32">
         <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
-        <v>0.36458333333333331</v>
+        <v>0.38541666666666663</v>
       </c>
       <c r="AA4" s="32">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.38425925925925924</v>
+        <v>0.40509259259259256</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ajout page resume et modificatio homepage, closes #10
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238BAEB5-2D9C-2B46-8704-37AD33883475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A439C2-D375-6640-900A-48F7689D1373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2504,7 +2504,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Modification étape La Sarre
- Ajout d'un GPX temporaire pour une étape La Sarre
- Changement heurers itinéraires et feuille de route.
- MAJ sites web
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\guide2023\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357808ED-2D23-4ED8-A0A6-B9B474E6E96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C75BA-1AAF-5642-B4AA-A0868E369E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38115" yWindow="975" windowWidth="35910" windowHeight="19680" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="224">
   <si>
     <t>GPM</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Circuit - Amos</t>
   </si>
   <si>
-    <t>10 x 10.8 km = 108 km</t>
-  </si>
-  <si>
     <t>Liens</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t xml:space="preserve">https://ridewithgps.com/routes/39650118   </t>
   </si>
   <si>
-    <t xml:space="preserve">https://ridewithgps.com/routes/39650511 </t>
-  </si>
-  <si>
     <t>Nb_tours</t>
   </si>
   <si>
@@ -730,6 +724,18 @@
   </si>
   <si>
     <t>Ouverture du ravito : maintenant à 30 km, pas 50km</t>
+  </si>
+  <si>
+    <t>La Sarre - Amos</t>
+  </si>
+  <si>
+    <t>96.4 km + ( 5 x 5.4 km) = 123.4 km</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/41972181</t>
+  </si>
+  <si>
+    <t>Preissac - Amos</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1419,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1451,7 +1457,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1557,7 +1563,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1733,36 +1739,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="24"/>
     </row>
   </sheetData>
@@ -1779,17 +1785,17 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -1801,27 +1807,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -1831,12 +1837,12 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1846,274 +1852,274 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2128,17 +2134,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2150,27 +2156,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2185,7 +2191,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2194,18 +2200,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2222,14 +2228,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>40</v>
       </c>
@@ -2237,74 +2243,74 @@
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D2" s="16" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>62</v>
@@ -2313,12 +2319,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2327,172 +2333,172 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="23" t="s">
+    <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>136</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>138</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" t="s">
         <v>206</v>
       </c>
-      <c r="B19" t="s">
-        <v>210</v>
-      </c>
-      <c r="C19" t="s">
-        <v>208</v>
-      </c>
       <c r="D19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2508,53 +2514,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.125" style="30" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" style="30" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2569,25 +2575,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K1" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
         <v>165</v>
       </c>
-      <c r="L1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="N1" t="s">
-        <v>192</v>
-      </c>
-      <c r="O1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>169</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -2599,51 +2605,51 @@
         <v>67</v>
       </c>
       <c r="T1" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="V1" t="s">
+        <v>216</v>
+      </c>
+      <c r="W1" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA1" t="s">
         <v>218</v>
       </c>
-      <c r="W1" t="s">
-        <v>217</v>
-      </c>
-      <c r="X1" t="s">
-        <v>215</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -2686,7 +2692,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U2" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -2714,24 +2720,24 @@
         <v>0.80653409090909089</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>75</v>
@@ -2777,7 +2783,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U3" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -2805,21 +2811,21 @@
         <v>0.81145833333333328</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
         <v>73</v>
@@ -2867,7 +2873,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -2893,27 +2899,27 @@
         <v>0.40509259259259256</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -2956,7 +2962,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U5" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -2984,27 +2990,27 @@
         <v>0.81422101449275353</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F6" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -3047,7 +3053,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U6" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -3075,27 +3081,27 @@
         <v>0.72383720930232565</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -3138,7 +3144,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U7" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
@@ -3166,57 +3172,58 @@
         <v>0.80271317829457367</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>220</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>80</v>
+        <v>221</v>
       </c>
       <c r="H8">
         <v>14</v>
       </c>
       <c r="I8" s="25">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>108</v>
+        <f>99.4+Tableau2[[#This Row],[Nb_tours]]*Tableau2[[#This Row],[KM_par_tours]]</f>
+        <v>126.4</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L8" s="21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M8" s="21">
-        <v>10.8</v>
+        <v>5.4</v>
       </c>
       <c r="N8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="N8" si="2">P8-O8</f>
+        <v>96.4</v>
       </c>
       <c r="O8" s="28">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="P8" s="29">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>108</v>
+        <v>123.4</v>
       </c>
       <c r="Q8">
         <v>45</v>
@@ -3229,14 +3236,14 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>88</v>
+        <v>222</v>
       </c>
       <c r="U8" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
-        <v>14:30</v>
+        <v>14:0</v>
       </c>
       <c r="V8" s="32">
-        <v>0</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="W8" s="32">
         <v>2.0833333333333332E-2</v>
@@ -3246,15 +3253,15 @@
       </c>
       <c r="Y8" s="32">
         <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
-        <v>0.55208333333333326</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="Z8" s="32">
         <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
-        <v>0.57291666666666663</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="AA8" s="32">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.70881782945736427</v>
+        <v>0.70581395348837217</v>
       </c>
     </row>
   </sheetData>
@@ -3262,66 +3269,65 @@
     <hyperlink ref="T2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
     <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
     <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
-    <hyperlink ref="T8" r:id="rId4" display="https://ridewithgps.com/routes/39650511" xr:uid="{67B71125-04A3-4187-889F-1635E044BB03}"/>
-    <hyperlink ref="T6" r:id="rId5" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+    <hyperlink ref="T6" r:id="rId4" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D286032-E11B-2F4F-8B68-3808324E7B4A}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.875" customWidth="1"/>
-    <col min="23" max="23" width="38.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -3336,25 +3342,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" t="s">
+        <v>163</v>
+      </c>
+      <c r="L1" t="s">
         <v>164</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
         <v>165</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>166</v>
       </c>
-      <c r="M1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="O1" t="s">
-        <v>168</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>169</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -3366,30 +3372,30 @@
         <v>67</v>
       </c>
       <c r="T1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D2" s="27">
-        <v>43661</v>
+        <v>43660</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
         <v>79</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3431,7 +3437,24 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="27">
+        <v>43661</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -3454,17 +3477,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3476,12 +3499,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -3491,12 +3514,12 @@
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3506,12 +3529,12 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -3521,7 +3544,7 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -3536,7 +3559,7 @@
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -3551,7 +3574,7 @@
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -3566,7 +3589,7 @@
       </c>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
@@ -3581,52 +3604,52 @@
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>13.4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>34.700000000000003</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>45.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.4</v>
       </c>
@@ -3641,12 +3664,12 @@
       </c>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>62.8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
@@ -3656,7 +3679,7 @@
       </c>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -3671,12 +3694,12 @@
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -3686,22 +3709,22 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -3709,19 +3732,19 @@
         <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -3731,7 +3754,7 @@
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>77.5</v>
       </c>
@@ -3746,12 +3769,12 @@
       </c>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.8</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
@@ -3761,7 +3784,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>98</v>
       </c>
@@ -3776,27 +3799,27 @@
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>101.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>101.2</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>50</v>
@@ -3806,7 +3829,7 @@
       </c>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>101.7</v>
       </c>
@@ -3821,12 +3844,12 @@
       </c>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>104.1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>16</v>
@@ -3836,22 +3859,22 @@
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>119</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <f>A26+1</f>
         <v>120</v>
@@ -3867,13 +3890,13 @@
       </c>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <f t="shared" ref="A28:A39" si="0">A27+1</f>
         <v>121</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -3883,13 +3906,13 @@
       </c>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -3899,13 +3922,13 @@
       </c>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>123</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -3915,13 +3938,13 @@
       </c>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -3931,13 +3954,13 @@
       </c>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -3947,13 +3970,13 @@
       </c>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -3963,13 +3986,13 @@
       </c>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -3979,13 +4002,13 @@
       </c>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -3995,13 +4018,13 @@
       </c>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -4011,13 +4034,13 @@
       </c>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -4027,13 +4050,13 @@
       </c>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>41</v>
@@ -4043,13 +4066,13 @@
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>42</v>
@@ -4059,22 +4082,22 @@
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>136.69999999999999</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4089,17 +4112,17 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4111,12 +4134,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -4125,12 +4148,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -4139,12 +4162,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4153,7 +4176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>7.9</v>
       </c>
@@ -4167,7 +4190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>8</v>
       </c>
@@ -4181,7 +4204,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>12.1</v>
       </c>
@@ -4195,21 +4218,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>24.6</v>
       </c>
@@ -4223,21 +4246,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -4251,21 +4274,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>47.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>47.4</v>
       </c>
@@ -4279,7 +4302,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>61</v>
       </c>
@@ -4293,12 +4316,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -4307,21 +4330,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>62.8</v>
       </c>
@@ -4335,26 +4358,26 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>72.7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>74.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4363,7 +4386,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>77.5</v>
       </c>
@@ -4377,12 +4400,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -4391,21 +4414,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>81.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>98</v>
       </c>
@@ -4419,27 +4442,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <f>A38-3.2</f>
         <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4448,7 +4471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>101.7</v>
       </c>
@@ -4462,12 +4485,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4476,7 +4499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>107.5</v>
       </c>
@@ -4490,12 +4513,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4504,12 +4527,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4518,12 +4541,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -4532,12 +4555,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -4546,12 +4569,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="9">
         <v>109.35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -4560,12 +4583,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="9">
         <v>109.75</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -4574,12 +4597,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="9">
         <v>110.15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -4588,12 +4611,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>110.7</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -4602,12 +4625,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="9">
         <v>110.75</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -4616,26 +4639,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>111.2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="3">
         <v>114.4</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>42</v>
@@ -4644,35 +4667,35 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>118.7</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>119.9</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4687,17 +4710,17 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4709,26 +4732,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4737,12 +4760,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4751,21 +4774,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4780,17 +4803,17 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4802,27 +4825,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -4832,12 +4855,12 @@
       </c>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -4847,274 +4870,274 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5129,17 +5152,17 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -5151,26 +5174,26 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -5179,12 +5202,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -5193,237 +5216,237 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="10"/>
       <c r="D9" s="19"/>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="4"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="4"/>
       <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="17"/>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5"/>
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" s="10"/>
       <c r="D33" s="19"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5"/>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="13"/>
       <c r="C41" s="4"/>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification liens iframe - page programmation préliminaire
- id de *Ride wtih GPS* mis dans le lien général iframe grâce èa Regex
- Affichage de la map seulement
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1C75BA-1AAF-5642-B4AA-A0868E369E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380D581-0330-624A-A09E-27054E41B9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2514,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="N2" s="28">
-        <f t="shared" ref="N2:N8" si="0">P2-O2</f>
+        <f t="shared" ref="N2:N7" si="0">P2-O2</f>
         <v>131.69999999999999</v>
       </c>
       <c r="O2" s="28">

</xml_diff>

<commit_message>
Ajout page programmation - 1 à 4
- Création d'un nouvelle page de programmation - résumé de la semaine
- Tableau en html pour être en mesure d'ajouter les images du commanditaires
- Utilisation glue pour passer les variables qui viennent de `itineraires.xlsx`
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D380D581-0330-624A-A09E-27054E41B9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F477710-77DE-6C42-8FF0-7C46125ED9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="261">
   <si>
     <t>GPM</t>
   </si>
@@ -720,9 +720,6 @@
     <t>Heure Signature</t>
   </si>
   <si>
-    <t>Heure Arrivee</t>
-  </si>
-  <si>
     <t>Ouverture du ravito : maintenant à 30 km, pas 50km</t>
   </si>
   <si>
@@ -736,6 +733,120 @@
   </si>
   <si>
     <t>Preissac - Amos</t>
+  </si>
+  <si>
+    <t>HeureEntreeVille</t>
+  </si>
+  <si>
+    <t>VilleDep</t>
+  </si>
+  <si>
+    <t>VilleArr</t>
+  </si>
+  <si>
+    <t>Rouyn-Noranda</t>
+  </si>
+  <si>
+    <t>Amos</t>
+  </si>
+  <si>
+    <t>LieuDepFR</t>
+  </si>
+  <si>
+    <t>LieuArrFR</t>
+  </si>
+  <si>
+    <t>Cathédrale</t>
+  </si>
+  <si>
+    <t>LieuDepEN</t>
+  </si>
+  <si>
+    <t>LieuArrEN</t>
+  </si>
+  <si>
+    <t>CEGEP</t>
+  </si>
+  <si>
+    <t>Cathedral</t>
+  </si>
+  <si>
+    <t>Val-d'Or</t>
+  </si>
+  <si>
+    <t>Place Agnico-Eagle</t>
+  </si>
+  <si>
+    <t>La Sarre</t>
+  </si>
+  <si>
+    <t>Aréna Nicol Auto</t>
+  </si>
+  <si>
+    <t>Nicol Auto Arena</t>
+  </si>
+  <si>
+    <t>Malartic</t>
+  </si>
+  <si>
+    <t>École secondaire le Tremplin</t>
+  </si>
+  <si>
+    <t>Le Tremplin High School</t>
+  </si>
+  <si>
+    <t>Senneterre</t>
+  </si>
+  <si>
+    <t>Hôtel de Ville</t>
+  </si>
+  <si>
+    <t>Mont Bell</t>
+  </si>
+  <si>
+    <t>Agnico-Eagle Public Market</t>
+  </si>
+  <si>
+    <t>City Hall</t>
+  </si>
+  <si>
+    <t>HeureArrivee</t>
+  </si>
+  <si>
+    <t>Depart</t>
+  </si>
+  <si>
+    <t>Via</t>
+  </si>
+  <si>
+    <t>(via Aiguebelle)</t>
+  </si>
+  <si>
+    <t>(via Barraute)</t>
+  </si>
+  <si>
+    <t>(sens horaire)</t>
+  </si>
+  <si>
+    <t>(via Poularie)</t>
+  </si>
+  <si>
+    <t>Nb_Coureurs</t>
+  </si>
+  <si>
+    <t>DerArr</t>
+  </si>
+  <si>
+    <t>DerDep</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Saint-Maurice</t>
+  </si>
+  <si>
+    <t>Cadillac</t>
   </si>
 </sst>
 </file>
@@ -746,7 +857,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -812,6 +923,11 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -898,7 +1014,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -962,12 +1078,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="38">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1069,6 +1188,52 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1311,7 +1476,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
@@ -1324,54 +1489,68 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:AA8" totalsRowShown="0">
-  <autoFilter ref="A1:AA8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
-  <tableColumns count="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:AK8" totalsRowShown="0">
+  <autoFilter ref="A1:AK8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+  <tableColumns count="37">
     <tableColumn id="1" xr3:uid="{F159CC0E-186F-4E03-998F-71303E6AFF37}" name="Etape"/>
     <tableColumn id="19" xr3:uid="{3543EB43-316C-0F44-B3AA-B931646E7365}" name="Jour"/>
     <tableColumn id="18" xr3:uid="{0D4EFF62-DD86-2240-BAFF-EEDA66BC4B15}" name="Day"/>
     <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
     <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="36"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="35"/>
     <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="22">
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="34"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="32">
       <calculatedColumnFormula>P2-O2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="21">
+    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="31">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="20">
+    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="30">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="19">
+    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="29">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="27">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataDxfId="16" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="21" xr3:uid="{F2204A86-7E8B-4F1F-89A0-9523DD2193D9}" name="Départ" dataDxfId="15">
-      <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataDxfId="26" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="21" xr3:uid="{F2204A86-7E8B-4F1F-89A0-9523DD2193D9}" name="Depart" dataDxfId="25">
+      <calculatedColumnFormula>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2B5A63D9-26DC-4A28-8248-6E6EA5709678}" name="Temps Transport" dataDxfId="14"/>
-    <tableColumn id="25" xr3:uid="{F7C0E5F3-60BA-4A5C-949D-A330E373C447}" name="Delai Preparation" dataDxfId="13"/>
-    <tableColumn id="23" xr3:uid="{B5478C0D-EFC2-4CDA-831C-0997C386A960}" name="Delai Signature" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="11">
-      <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</calculatedColumnFormula>
+    <tableColumn id="22" xr3:uid="{2B5A63D9-26DC-4A28-8248-6E6EA5709678}" name="Temps Transport" dataDxfId="24"/>
+    <tableColumn id="25" xr3:uid="{F7C0E5F3-60BA-4A5C-949D-A330E373C447}" name="Delai Preparation" dataDxfId="23"/>
+    <tableColumn id="23" xr3:uid="{B5478C0D-EFC2-4CDA-831C-0997C386A960}" name="Delai Signature" dataDxfId="22"/>
+    <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="21">
+      <calculatedColumnFormula>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="10">
-      <calculatedColumnFormula>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</calculatedColumnFormula>
+    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="20">
+      <calculatedColumnFormula>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="Heure Arrivee" dataDxfId="9">
-      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</calculatedColumnFormula>
+    <tableColumn id="28" xr3:uid="{87DB48BA-40E9-2842-81A9-7C28757A794A}" name="HeureEntreeVille" dataDxfId="19">
+      <calculatedColumnFormula>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="18">
+      <calculatedColumnFormula>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="17"/>
+    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="16"/>
+    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="14"/>
+    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="13"/>
+    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="12">
+      <calculatedColumnFormula>Tableau2[[#This Row],[LieuDepFR]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="11"/>
+    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="10"/>
+    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1737,38 +1916,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B1" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B2">
+        <f>20*6</f>
+        <v>120</v>
+      </c>
+      <c r="C2" s="35">
+        <v>6.9444444444444447E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="24"/>
     </row>
   </sheetData>
@@ -2512,10 +2705,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2544,9 +2737,18 @@
     <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.83203125" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.6640625" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -2607,8 +2809,8 @@
       <c r="T1" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="U1" t="s">
-        <v>131</v>
+      <c r="U1" s="16" t="s">
+        <v>249</v>
       </c>
       <c r="V1" t="s">
         <v>216</v>
@@ -2625,11 +2827,41 @@
       <c r="Z1" t="s">
         <v>217</v>
       </c>
-      <c r="AA1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA1" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2695,7 +2927,7 @@
         <v>81</v>
       </c>
       <c r="U2" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>16:15</v>
       </c>
       <c r="V2" s="32">
@@ -2708,19 +2940,47 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y2" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.55208333333333337</v>
       </c>
       <c r="Z2" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.64583333333333337</v>
       </c>
-      <c r="AA2" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.80653409090909089</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA2" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:21</v>
+      </c>
+      <c r="AB2" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:21</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD2" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF2" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG2" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH2" s="33" t="str">
+        <f>Tableau2[[#This Row],[LieuDepFR]]</f>
+        <v>CEGEP</v>
+      </c>
+      <c r="AI2" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2786,7 +3046,7 @@
         <v>82</v>
       </c>
       <c r="U3" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>16:45</v>
       </c>
       <c r="V3" s="32">
@@ -2799,19 +3059,46 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y3" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.59374999999999989</v>
       </c>
       <c r="Z3" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AA3" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.81145833333333328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA3" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>18:59</v>
+      </c>
+      <c r="AB3" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:28</v>
+      </c>
+      <c r="AC3" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD3" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE3" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF3" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG3" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH3" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI3" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="32"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2876,30 +3163,65 @@
         <v>83</v>
       </c>
       <c r="U4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
-        <v>9:30</v>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
+        <v>09:30</v>
       </c>
       <c r="V4" s="32">
         <v>0</v>
       </c>
-      <c r="W4" s="32"/>
+      <c r="W4" s="32">
+        <v>0</v>
+      </c>
       <c r="X4" s="32">
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="Y4" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.38541666666666663</v>
       </c>
       <c r="Z4" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.38541666666666663</v>
       </c>
-      <c r="AA4" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.40509259259259256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA4" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>09:43</v>
+      </c>
+      <c r="AB4" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>09:43</v>
+      </c>
+      <c r="AC4" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD4" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE4" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="AF4" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AG4" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH4" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AI4" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ4" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
+        <v>11:40</v>
+      </c>
+      <c r="AK4" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[DerDep]],"HH:MM")</f>
+        <v>11:53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" ht="14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2965,7 +3287,7 @@
         <v>84</v>
       </c>
       <c r="U5" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>18:15</v>
       </c>
       <c r="V5" s="32">
@@ -2978,19 +3300,48 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y5" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.65625</v>
       </c>
       <c r="Z5" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.72916666666666663</v>
       </c>
-      <c r="AA5" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.81422101449275353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA5" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:32</v>
+      </c>
+      <c r="AB5" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:32</v>
+      </c>
+      <c r="AC5" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD5" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE5" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="AF5" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="AG5" s="33" t="str">
+        <f>Tableau2[[#This Row],[LieuDepFR]]</f>
+        <v>École secondaire le Tremplin</v>
+      </c>
+      <c r="AH5" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI5" s="32" t="str">
+        <f>Tableau2[[#This Row],[LieuDepEN]]</f>
+        <v>Le Tremplin High School</v>
+      </c>
+      <c r="AJ5" s="32"/>
+      <c r="AK5" s="32"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3056,8 +3407,8 @@
         <v>85</v>
       </c>
       <c r="U6" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
-        <v>14:0</v>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
+        <v>14:00</v>
       </c>
       <c r="V6" s="32">
         <v>7.2916666666666671E-2</v>
@@ -3069,19 +3420,47 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y6" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.45833333333333343</v>
       </c>
       <c r="Z6" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.55208333333333337</v>
       </c>
-      <c r="AA6" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.72383720930232565</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA6" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>17:22</v>
+      </c>
+      <c r="AB6" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>17:22</v>
+      </c>
+      <c r="AC6" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="AD6" s="32" t="str">
+        <f>Tableau2[[#This Row],[VilleDep]]</f>
+        <v>Senneterre</v>
+      </c>
+      <c r="AE6" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF6" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="AG6" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH6" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI6" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ6" s="32"/>
+      <c r="AK6" s="32"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3147,7 +3526,7 @@
         <v>86</v>
       </c>
       <c r="U7" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>16:30</v>
       </c>
       <c r="V7" s="32">
@@ -3160,19 +3539,46 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y7" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.63541666666666663</v>
       </c>
       <c r="Z7" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.65625</v>
       </c>
-      <c r="AA7" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.80271317829457367</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+      <c r="AA7" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:15</v>
+      </c>
+      <c r="AB7" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>19:15</v>
+      </c>
+      <c r="AC7" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD7" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE7" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="AF7" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AG7" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH7" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AI7" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ7" s="32"/>
+      <c r="AK7" s="32"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3189,10 +3595,10 @@
         <v>161</v>
       </c>
       <c r="F8" t="s">
+        <v>219</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>220</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>221</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3236,11 +3642,11 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U8" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]])</f>
-        <v>14:0</v>
+        <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
+        <v>14:00</v>
       </c>
       <c r="V8" s="32">
         <v>5.2083333333333336E-2</v>
@@ -3252,17 +3658,47 @@
         <v>3.125E-2</v>
       </c>
       <c r="Y8" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
         <v>0.47916666666666669</v>
       </c>
       <c r="Z8" s="32">
-        <f>Tableau2[[#This Row],[Départ]]-Tableau2[[#This Row],[Delai Signature]]</f>
+        <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
         <v>0.55208333333333337</v>
       </c>
-      <c r="AA8" s="32">
-        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Départ]]</f>
-        <v>0.70581395348837217</v>
-      </c>
+      <c r="AA8" s="32" t="str">
+        <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>16:18</v>
+      </c>
+      <c r="AB8" s="32" t="str">
+        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
+        <v>16:56</v>
+      </c>
+      <c r="AC8" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD8" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE8" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF8" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG8" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AH8" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI8" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ8" s="32"/>
+      <c r="AK8" s="32"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="Z14" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3273,6 +3709,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="AH4" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>
@@ -3454,7 +3893,7 @@
         <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin de la programmation
- Fin des étapes programmation
- Ajout de la programmation anglaise
- Modification pour utilisation des logos 0 à 7
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F477710-77DE-6C42-8FF0-7C46125ED9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C47C3E5-5EC8-FB4E-87BA-B68DFEA48666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="262">
   <si>
     <t>GPM</t>
   </si>
@@ -825,9 +825,6 @@
     <t>(via Barraute)</t>
   </si>
   <si>
-    <t>(sens horaire)</t>
-  </si>
-  <si>
     <t>(via Poularie)</t>
   </si>
   <si>
@@ -847,6 +844,12 @@
   </si>
   <si>
     <t>Cadillac</t>
+  </si>
+  <si>
+    <t>(via Rivière-Héva &amp; Preissac )</t>
+  </si>
+  <si>
+    <t>(via Val-d'Or)</t>
   </si>
 </sst>
 </file>
@@ -1933,10 +1936,10 @@
         <v>88</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2855,10 +2858,10 @@
         <v>232</v>
       </c>
       <c r="AJ1" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AK1" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.15">
@@ -3198,7 +3201,7 @@
         <v>227</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AF4" s="33" t="s">
         <v>230</v>
@@ -3322,7 +3325,7 @@
         <v>240</v>
       </c>
       <c r="AE5" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AF5" s="34" t="s">
         <v>241</v>
@@ -3443,7 +3446,7 @@
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="AF6" s="33" t="s">
         <v>244</v>
@@ -3561,7 +3564,7 @@
         <v>227</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="AF7" s="33" t="s">
         <v>230</v>
@@ -3680,7 +3683,7 @@
         <v>227</v>
       </c>
       <c r="AE8" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AF8" s="33" t="s">
         <v>238</v>

</xml_diff>

<commit_message>
Modification étape 7 et maj feuille de route en conséquence
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C47C3E5-5EC8-FB4E-87BA-B68DFEA48666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F878D9-F38D-DE4B-95C1-46C0F893ABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,9 +726,6 @@
     <t>La Sarre - Amos</t>
   </si>
   <si>
-    <t>96.4 km + ( 5 x 5.4 km) = 123.4 km</t>
-  </si>
-  <si>
     <t>https://ridewithgps.com/routes/41972181</t>
   </si>
   <si>
@@ -825,9 +822,6 @@
     <t>(via Barraute)</t>
   </si>
   <si>
-    <t>(via Poularie)</t>
-  </si>
-  <si>
     <t>Nb_Coureurs</t>
   </si>
   <si>
@@ -850,6 +844,12 @@
   </si>
   <si>
     <t>(via Val-d'Or)</t>
+  </si>
+  <si>
+    <t>98,6 km + ( 5 x 5.4 km) = 125.6 km</t>
+  </si>
+  <si>
+    <t>(via Palmarolle)</t>
   </si>
 </sst>
 </file>
@@ -1091,6 +1091,9 @@
   </cellStyles>
   <dxfs count="38">
     <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1227,9 +1230,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
@@ -1540,20 +1540,20 @@
     <tableColumn id="28" xr3:uid="{87DB48BA-40E9-2842-81A9-7C28757A794A}" name="HeureEntreeVille" dataDxfId="19">
       <calculatedColumnFormula>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="18">
-      <calculatedColumnFormula>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="0">
+      <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="17"/>
-    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="16"/>
-    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="15"/>
-    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="14"/>
-    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="13"/>
-    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="12">
+    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="18"/>
+    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="17"/>
+    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="16"/>
+    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="15"/>
+    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="14"/>
+    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="13">
       <calculatedColumnFormula>Tableau2[[#This Row],[LieuDepFR]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="11"/>
-    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="10"/>
-    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="9"/>
+    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="11"/>
+    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1569,27 +1569,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="8"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="5">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="4">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="3">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="1">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -1936,10 +1936,10 @@
         <v>88</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2813,7 +2813,7 @@
         <v>80</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V1" t="s">
         <v>216</v>
@@ -2831,37 +2831,37 @@
         <v>217</v>
       </c>
       <c r="AA1" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC1" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="AB1" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="AD1" s="16" t="s">
-        <v>225</v>
-      </c>
       <c r="AE1" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AF1" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="AG1" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="AG1" s="16" t="s">
-        <v>229</v>
-      </c>
       <c r="AH1" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="AI1" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="AI1" s="33" t="s">
-        <v>232</v>
-      </c>
       <c r="AJ1" s="16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AK1" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.15">
@@ -2954,31 +2954,31 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>19:21</v>
       </c>
-      <c r="AB2" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:21</v>
+      <c r="AB2" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.80653409090909089</v>
       </c>
       <c r="AC2" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD2" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="AD2" s="33" t="s">
-        <v>227</v>
-      </c>
       <c r="AE2" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AG2" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH2" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI2" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ2" s="32"/>
       <c r="AK2" s="32"/>
@@ -3073,30 +3073,30 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>18:59</v>
       </c>
-      <c r="AB3" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:28</v>
+      <c r="AB3" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.81145833333333328</v>
       </c>
       <c r="AC3" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="AD3" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE3" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="AF3" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="AD3" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE3" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>236</v>
-      </c>
       <c r="AG3" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH3" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AI3" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ3" s="32"/>
       <c r="AK3" s="32"/>
@@ -3190,30 +3190,30 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>09:43</v>
       </c>
-      <c r="AB4" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>09:43</v>
+      <c r="AB4" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AD4" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AF4" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AG4" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH4" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AI4" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ4" s="32" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -3314,28 +3314,28 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>19:32</v>
       </c>
-      <c r="AB5" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:32</v>
+      <c r="AB5" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD5" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE5" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF5" s="34" t="s">
         <v>240</v>
-      </c>
-      <c r="AD5" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="AE5" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="AF5" s="34" t="s">
-        <v>241</v>
       </c>
       <c r="AG5" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AI5" s="32" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -3434,31 +3434,31 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>17:22</v>
       </c>
-      <c r="AB6" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>17:22</v>
+      <c r="AB6" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AD6" s="32" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AF6" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG6" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="AG6" s="33" t="s">
-        <v>245</v>
-      </c>
       <c r="AH6" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AI6" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AJ6" s="32"/>
       <c r="AK6" s="32"/>
@@ -3553,30 +3553,30 @@
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
         <v>19:15</v>
       </c>
-      <c r="AB7" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:15</v>
+      <c r="AB7" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AD7" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AF7" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AG7" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH7" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AI7" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ7" s="32"/>
       <c r="AK7" s="32"/>
@@ -3601,7 +3601,7 @@
         <v>219</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3610,8 +3610,8 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <f>99.4+Tableau2[[#This Row],[Nb_tours]]*Tableau2[[#This Row],[KM_par_tours]]</f>
-        <v>126.4</v>
+        <f>101.6+Tableau2[[#This Row],[Nb_tours]]*Tableau2[[#This Row],[KM_par_tours]]</f>
+        <v>128.6</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -3624,7 +3624,7 @@
       </c>
       <c r="N8" s="28">
         <f t="shared" ref="N8" si="2">P8-O8</f>
-        <v>96.4</v>
+        <v>98.6</v>
       </c>
       <c r="O8" s="28">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="P8" s="29">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>123.4</v>
+        <v>125.6</v>
       </c>
       <c r="Q8">
         <v>45</v>
@@ -3645,7 +3645,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3670,32 +3670,32 @@
       </c>
       <c r="AA8" s="32" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>16:18</v>
-      </c>
-      <c r="AB8" s="32" t="str">
-        <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>16:56</v>
+        <v>16:21</v>
+      </c>
+      <c r="AB8" s="32">
+        <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
+        <v>0.70794573643410852</v>
       </c>
       <c r="AC8" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD8" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE8" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="AF8" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="AD8" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE8" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="AF8" s="33" t="s">
+      <c r="AG8" s="33" t="s">
+        <v>229</v>
+      </c>
+      <c r="AH8" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="AG8" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="AH8" s="33" t="s">
-        <v>239</v>
-      </c>
       <c r="AI8" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ8" s="32"/>
       <c r="AK8" s="32"/>
@@ -3709,6 +3709,7 @@
     <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
     <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
     <hyperlink ref="T6" r:id="rId4" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+    <hyperlink ref="T8" r:id="rId5" xr:uid="{6ADD1D3E-718C-764E-8FDE-6A84C5E1F896}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3716,7 +3717,7 @@
     <ignoredError sqref="AH4" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3896,7 +3897,7 @@
         <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Création des graphiques d'Élévation en .pgn, ref à #16
- Pour éviter de recréer les graphique à chaque fois sur le site web
- Pour faciliter l'intégration dans le guide papier en pdf

Modifications :

- Modification Snakefile
- Ajout de fonctions pour créer tous les graphs, en FR et EN directement dans le fichier qui dévrit les fonctions : `graphique_denivele.R`
- Modification des pages EtapeX.Rmd pour import du fichier .png plutôt que de recréer le graphique à chaque fois.
- Arrêt d'importer ce fichier dans `index.Rmd` pour création du git_book.
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F878D9-F38D-DE4B-95C1-46C0F893ABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA58820-FCE9-4248-815C-80AB5D98BBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="7280" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="263">
   <si>
     <t>GPM</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>(via Palmarolle)</t>
+  </si>
+  <si>
+    <t>Demi tour</t>
   </si>
 </sst>
 </file>
@@ -1091,9 +1094,6 @@
   </cellStyles>
   <dxfs count="38">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1230,6 +1230,9 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
@@ -1540,20 +1543,20 @@
     <tableColumn id="28" xr3:uid="{87DB48BA-40E9-2842-81A9-7C28757A794A}" name="HeureEntreeVille" dataDxfId="19">
       <calculatedColumnFormula>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="0">
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="18">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="18"/>
-    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="17"/>
-    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="16"/>
-    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="15"/>
-    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="14"/>
-    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="13">
+    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="17"/>
+    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="16"/>
+    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="14"/>
+    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="13"/>
+    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="12">
       <calculatedColumnFormula>Tableau2[[#This Row],[LieuDepFR]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="12"/>
-    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="11"/>
-    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="10"/>
+    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="11"/>
+    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="10"/>
+    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1569,27 +1572,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="4">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -1978,7 +1981,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2008,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>131</v>
@@ -2327,7 +2330,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -2357,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>131</v>
@@ -2421,7 +2424,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2710,7 +2713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
@@ -4552,7 +4555,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -5147,10 +5150,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F578A-E7BF-4EB0-BBD6-BC84A4E8AD52}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -5180,58 +5183,43 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>68</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
-        <v>111.2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5243,7 +5231,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -5273,7 +5261,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>131</v>
@@ -5592,7 +5580,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -5622,7 +5610,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Modification fichiers excel et code pour inversion RN-VD, ref #25
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA58820-FCE9-4248-815C-80AB5D98BBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B0ACAF-317C-4B42-A861-DC5C526B9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="7280" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
     <sheet name="Lexique" sheetId="20" r:id="rId2"/>
     <sheet name="Details" sheetId="21" r:id="rId3"/>
     <sheet name="Details_options" sheetId="29" r:id="rId4"/>
-    <sheet name="Etape_1" sheetId="6" r:id="rId5"/>
-    <sheet name="Etape_2" sheetId="22" r:id="rId6"/>
+    <sheet name="Etape_1" sheetId="22" r:id="rId5"/>
+    <sheet name="Etape_2" sheetId="6" r:id="rId6"/>
     <sheet name="Etape_3" sheetId="24" r:id="rId7"/>
     <sheet name="Etape_4" sheetId="25" r:id="rId8"/>
     <sheet name="Etape_5" sheetId="26" r:id="rId9"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="262">
   <si>
     <t>GPM</t>
   </si>
@@ -799,9 +799,6 @@
   </si>
   <si>
     <t>Mont Bell</t>
-  </si>
-  <si>
-    <t>Agnico-Eagle Public Market</t>
   </si>
   <si>
     <t>City Hall</t>
@@ -1939,10 +1936,10 @@
         <v>88</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2713,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AK14"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC32" sqref="AC32"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2816,7 +2813,7 @@
         <v>80</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V1" t="s">
         <v>216</v>
@@ -2837,7 +2834,7 @@
         <v>222</v>
       </c>
       <c r="AB1" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AC1" s="16" t="s">
         <v>223</v>
@@ -2846,7 +2843,7 @@
         <v>224</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="16" t="s">
         <v>227</v>
@@ -2861,10 +2858,10 @@
         <v>231</v>
       </c>
       <c r="AJ1" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AK1" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.15">
@@ -2884,40 +2881,40 @@
         <v>156</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>197</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>191</v>
+        <v>75</v>
       </c>
       <c r="H2">
         <v>16</v>
       </c>
       <c r="I2" s="25">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="J2">
-        <v>136.69999999999999</v>
+        <v>119.9</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="N2" s="28">
         <f t="shared" ref="N2:N7" si="0">P2-O2</f>
-        <v>131.69999999999999</v>
+        <v>95.300000000000011</v>
       </c>
       <c r="O2" s="28">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>0</v>
+        <v>21.6</v>
       </c>
       <c r="P2" s="29">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>131.69999999999999</v>
+        <v>116.9</v>
       </c>
       <c r="Q2">
         <v>46</v>
@@ -2930,14 +2927,14 @@
         <v>42</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
-        <v>16:15</v>
+        <v>16:45</v>
       </c>
       <c r="V2" s="32">
-        <v>7.2916666666666671E-2</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="W2" s="32">
         <v>2.0833333333333332E-2</v>
@@ -2947,22 +2944,22 @@
       </c>
       <c r="Y2" s="32">
         <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
-        <v>0.55208333333333337</v>
+        <v>0.59374999999999989</v>
       </c>
       <c r="Z2" s="32">
         <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
-        <v>0.64583333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AA2" s="32" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:21</v>
+        <v>18:59</v>
       </c>
       <c r="AB2" s="32">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.80653409090909089</v>
+        <v>0.81145833333333328</v>
       </c>
       <c r="AC2" s="33" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="AD2" s="33" t="s">
         <v>226</v>
@@ -2971,14 +2968,14 @@
         <v>250</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AG2" s="33" t="s">
         <v>229</v>
       </c>
       <c r="AH2" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
-        <v>CEGEP</v>
+        <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="33" t="s">
         <v>233</v>
@@ -3003,40 +3000,40 @@
         <v>187</v>
       </c>
       <c r="F3" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="H3">
         <v>16</v>
       </c>
       <c r="I3" s="25">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="J3">
-        <v>119.9</v>
+        <v>136.69999999999999</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L3" s="21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3" s="21">
-        <v>5.4</v>
+        <v>0</v>
       </c>
       <c r="N3" s="28">
         <f t="shared" si="0"/>
-        <v>95.300000000000011</v>
+        <v>131.69999999999999</v>
       </c>
       <c r="O3" s="28">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
-        <v>21.6</v>
+        <v>0</v>
       </c>
       <c r="P3" s="29">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>116.9</v>
+        <v>131.69999999999999</v>
       </c>
       <c r="Q3">
         <v>46</v>
@@ -3049,14 +3046,14 @@
         <v>42</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
-        <v>16:45</v>
+        <v>16:15</v>
       </c>
       <c r="V3" s="32">
-        <v>5.2083333333333336E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="W3" s="32">
         <v>2.0833333333333332E-2</v>
@@ -3066,37 +3063,38 @@
       </c>
       <c r="Y3" s="32">
         <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</f>
-        <v>0.59374999999999989</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="Z3" s="32">
         <f>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</f>
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="AA3" s="32" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>18:59</v>
+        <v>19:21</v>
       </c>
       <c r="AB3" s="32">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.81145833333333328</v>
+        <v>0.80653409090909089</v>
       </c>
       <c r="AC3" s="33" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="AD3" s="33" t="s">
         <v>226</v>
       </c>
       <c r="AE3" s="33" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AF3" s="33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="AG3" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="AH3" s="33" t="s">
-        <v>245</v>
+      <c r="AH3" s="33" t="str">
+        <f>Tableau2[[#This Row],[LieuDepFR]]</f>
+        <v>CEGEP</v>
       </c>
       <c r="AI3" s="33" t="s">
         <v>233</v>
@@ -3204,7 +3202,7 @@
         <v>226</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AF4" s="33" t="s">
         <v>229</v>
@@ -3328,7 +3326,7 @@
         <v>239</v>
       </c>
       <c r="AE5" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AF5" s="34" t="s">
         <v>240</v>
@@ -3449,7 +3447,7 @@
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AF6" s="33" t="s">
         <v>243</v>
@@ -3458,7 +3456,7 @@
         <v>244</v>
       </c>
       <c r="AH6" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AI6" s="33" t="s">
         <v>244</v>
@@ -3567,7 +3565,7 @@
         <v>226</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF7" s="33" t="s">
         <v>229</v>
@@ -3604,7 +3602,7 @@
         <v>219</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3686,7 +3684,7 @@
         <v>226</v>
       </c>
       <c r="AE8" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AF8" s="33" t="s">
         <v>237</v>
@@ -3708,11 +3706,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{42F24162-7D5A-460C-B9A5-A15ADD968CF5}"/>
-    <hyperlink ref="T3" r:id="rId2" display="https://ridewithgps.com/routes/39641884" xr:uid="{DA268459-A33B-4E5F-A020-38440DCEA8B3}"/>
-    <hyperlink ref="T7" r:id="rId3" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
-    <hyperlink ref="T6" r:id="rId4" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
-    <hyperlink ref="T8" r:id="rId5" xr:uid="{6ADD1D3E-718C-764E-8FDE-6A84C5E1F896}"/>
+    <hyperlink ref="T7" r:id="rId1" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
+    <hyperlink ref="T6" r:id="rId2" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
+    <hyperlink ref="T8" r:id="rId3" xr:uid="{6ADD1D3E-718C-764E-8FDE-6A84C5E1F896}"/>
+    <hyperlink ref="T2" r:id="rId4" display="https://ridewithgps.com/routes/39641884" xr:uid="{6E809109-7436-EF40-BB42-B9AF199BF12E}"/>
+    <hyperlink ref="T3" r:id="rId5" xr:uid="{9DB439FE-3F18-9946-8B24-CE9C2E8957D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3916,645 +3914,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
-        <v>45.5</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
-        <v>47.4</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
-        <v>62.8</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="3">
-        <v>61.3</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="3">
-        <v>61.8</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="3">
-        <v>62.8</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="3">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="3">
-        <v>77.5</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="3">
-        <v>77.8</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="3">
-        <v>98</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
-        <v>101.1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="3">
-        <v>101.2</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="3">
-        <v>101.7</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="3">
-        <v>104.1</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A26" s="3">
-        <v>119</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
-        <f>A26+1</f>
-        <v>120</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="3">
-        <f t="shared" ref="A28:A39" si="0">A27+1</f>
-        <v>121</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="3">
-        <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="3">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A31" s="3">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="3">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="3">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="3">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="3">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="3">
-        <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="3">
-        <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="3">
-        <f t="shared" si="0"/>
-        <v>131</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="3">
-        <f t="shared" si="0"/>
-        <v>132</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A40" s="3">
-        <v>136.69999999999999</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -5148,11 +4511,646 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="3">
+        <v>5</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="3">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="3">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="3">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" s="3">
+        <v>45.5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="3">
+        <v>47.4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A13" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="3">
+        <v>61</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="3">
+        <v>61.3</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="3">
+        <v>61.8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="3">
+        <v>62.8</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="3">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="3">
+        <v>77.5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>77.8</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>98</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>101.1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>101.2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="3">
+        <v>101.7</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="3">
+        <v>104.1</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>119</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
+        <f>A26+1</f>
+        <v>120</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
+        <f t="shared" ref="A28:A39" si="0">A27+1</f>
+        <v>121</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A30" s="3">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="22"/>
+    </row>
+    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A36" s="3">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="3">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A40" s="3">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F578A-E7BF-4EB0-BBD6-BC84A4E8AD52}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -5200,7 +5198,7 @@
         <v>146</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Correction lecture fichier GPX, ref @#30
- Création d'une liste des numéros d'étape `gpx_files_stages` pour boucler sur ceux-ci plutôt que sur une série de 1 à nrow, pour permettre le travail sur GPX partiel
- Création colonne Nom_Courts_xx dans le fichier excel `intineraires.xlsx` pour le petit nom de l'étape qui sert de nom de parcours et qui est afficher dans la carte dynamique
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B0ACAF-317C-4B42-A861-DC5C526B9705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB601549-C83A-3E4C-B87E-764ACCEF4D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="7520" windowWidth="61460" windowHeight="20600" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="278">
   <si>
     <t>GPM</t>
   </si>
@@ -312,21 +312,6 @@
     <t>https://ridewithgps.com/routes/39641737</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ridewithgps.com/routes/39641884 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ridewithgps.com/routes/39642105 </t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/39889304</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/39569524</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ridewithgps.com/routes/39650118   </t>
-  </si>
-  <si>
     <t>Nb_tours</t>
   </si>
   <si>
@@ -726,9 +711,6 @@
     <t>La Sarre - Amos</t>
   </si>
   <si>
-    <t>https://ridewithgps.com/routes/41972181</t>
-  </si>
-  <si>
     <t>Preissac - Amos</t>
   </si>
   <si>
@@ -850,6 +832,72 @@
   </si>
   <si>
     <t>Demi tour</t>
+  </si>
+  <si>
+    <t>Étape 1 - Val-d'Or</t>
+  </si>
+  <si>
+    <t>Étape 2 - Rouyn-Noranda</t>
+  </si>
+  <si>
+    <t>Nom_Courts_FR</t>
+  </si>
+  <si>
+    <t>Nom_Courts_EN</t>
+  </si>
+  <si>
+    <t>Étape 3 - CLMI</t>
+  </si>
+  <si>
+    <t>Étape 4 - Malartic</t>
+  </si>
+  <si>
+    <t>Étape 5 - Senneterre</t>
+  </si>
+  <si>
+    <t>Étape 6 - Boucle Preissac</t>
+  </si>
+  <si>
+    <t>Étape 7 - La Sarre</t>
+  </si>
+  <si>
+    <t>Stage 1 - Val-d'Or</t>
+  </si>
+  <si>
+    <t>Stage 2 - Rouyn-Noranda</t>
+  </si>
+  <si>
+    <t>Stage 4 - Malartic</t>
+  </si>
+  <si>
+    <t>Stage 5 - Senneterre</t>
+  </si>
+  <si>
+    <t>Stage 7 - La Sarre</t>
+  </si>
+  <si>
+    <t>Stage 3 - ITT</t>
+  </si>
+  <si>
+    <t>Stage 6 - Preissac Loop</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268563</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268538</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268527</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268509</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268449</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42183412</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1137,45 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1479,7 +1565,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}" name="Tableau1" displayName="Tableau1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A1:D24" xr:uid="{6D69E1BF-D563-4383-B16C-77CF4F7B3AFC}"/>
   <tableColumns count="4">
     <tableColumn id="5" xr3:uid="{F0FFBF15-FEDF-C643-982D-FCACCA7549C7}" name="Symbol"/>
@@ -1492,68 +1578,70 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:AK8" totalsRowShown="0">
-  <autoFilter ref="A1:AK8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
-  <tableColumns count="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}" name="Tableau2" displayName="Tableau2" ref="A1:AM8" totalsRowShown="0">
+  <autoFilter ref="A1:AM8" xr:uid="{8DFF6054-52E9-474A-8B81-4940D285ED76}"/>
+  <tableColumns count="39">
     <tableColumn id="1" xr3:uid="{F159CC0E-186F-4E03-998F-71303E6AFF37}" name="Etape"/>
     <tableColumn id="19" xr3:uid="{3543EB43-316C-0F44-B3AA-B931646E7365}" name="Jour"/>
     <tableColumn id="18" xr3:uid="{0D4EFF62-DD86-2240-BAFF-EEDA66BC4B15}" name="Day"/>
     <tableColumn id="20" xr3:uid="{E33C33BE-64A9-E544-83BB-0D75EE75CE41}" name="Date"/>
     <tableColumn id="12" xr3:uid="{ED5642DA-8113-0E4E-82A6-3C75E9265A97}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{F00D4F6E-C90E-46EE-A909-314DE697FD94}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{8354F9C0-AD0A-4AD3-9848-4F4943024BA4}" name="Descr_km" dataDxfId="38"/>
     <tableColumn id="2" xr3:uid="{B450C706-68CE-4E8A-AFDB-4B447D80EDA8}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{9E140560-130D-4628-86EE-1A55F160D78B}" name="min_dep" dataDxfId="37"/>
     <tableColumn id="14" xr3:uid="{405A50AD-C717-BD44-8CF4-3A381A4A382E}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{526CBEFC-EC9F-A544-BB03-D1A4FE46FA3B}" name="KM_Neutres"/>
-    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="34"/>
-    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="32">
+    <tableColumn id="11" xr3:uid="{0DFDFB6D-3AD3-41A7-8166-655572AFBECE}" name="Nb_tours" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{0F6AA147-5F2C-7844-AA70-39BA69D17822}" name="KM_par_tours" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{D427D8CB-CD24-494C-8C89-5C11E9AD38F5}" name="Distance_Route" dataDxfId="34">
       <calculatedColumnFormula>P2-O2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="31">
+    <tableColumn id="17" xr3:uid="{017DA8AC-0426-3748-9B31-2FBF5A4A71CC}" name="Distance_en_circuit" dataDxfId="33">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="30">
+    <tableColumn id="15" xr3:uid="{45950B2C-FA23-0C41-BD9A-2B87B2F2A583}" name="Distance_totale" dataDxfId="32">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="29">
+    <tableColumn id="4" xr3:uid="{B6A83BA6-1D6C-4B6F-AEB9-C659AC6292AB}" name="Vit_rapide" dataDxfId="31">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="27">
+    <tableColumn id="5" xr3:uid="{7644F403-E43B-41CD-AA3D-80D9B7BE282A}" name="Vit_moy" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{D6AC70F3-4051-4632-820E-D8AF8DE14301}" name="Vit_lent" dataDxfId="29">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataDxfId="26" dataCellStyle="Lien hypertexte"/>
-    <tableColumn id="21" xr3:uid="{F2204A86-7E8B-4F1F-89A0-9523DD2193D9}" name="Depart" dataDxfId="25">
+    <tableColumn id="10" xr3:uid="{94F4814B-ACC3-42BB-BE44-22DD4EEFAAC9}" name="Liens" dataDxfId="28" dataCellStyle="Lien hypertexte"/>
+    <tableColumn id="21" xr3:uid="{F2204A86-7E8B-4F1F-89A0-9523DD2193D9}" name="Depart" dataDxfId="27">
       <calculatedColumnFormula>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{2B5A63D9-26DC-4A28-8248-6E6EA5709678}" name="Temps Transport" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{F7C0E5F3-60BA-4A5C-949D-A330E373C447}" name="Delai Preparation" dataDxfId="23"/>
-    <tableColumn id="23" xr3:uid="{B5478C0D-EFC2-4CDA-831C-0997C386A960}" name="Delai Signature" dataDxfId="22"/>
-    <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="21">
+    <tableColumn id="22" xr3:uid="{2B5A63D9-26DC-4A28-8248-6E6EA5709678}" name="Temps Transport" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{F7C0E5F3-60BA-4A5C-949D-A330E373C447}" name="Delai Preparation" dataDxfId="25"/>
+    <tableColumn id="23" xr3:uid="{B5478C0D-EFC2-4CDA-831C-0997C386A960}" name="Delai Signature" dataDxfId="24"/>
+    <tableColumn id="24" xr3:uid="{A09046F5-0413-4C19-909F-C542FD5D89A5}" name="Heure_Navette" dataDxfId="23">
       <calculatedColumnFormula>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Temps Transport]]-Tableau2[[#This Row],[Delai Signature]]-Tableau2[[#This Row],[Delai Preparation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="20">
+    <tableColumn id="26" xr3:uid="{3FF438BF-A8F9-410C-9EE8-149BE535DB34}" name="Heure Signature" dataDxfId="22">
       <calculatedColumnFormula>Tableau2[[#This Row],[Depart]]-Tableau2[[#This Row],[Delai Signature]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{87DB48BA-40E9-2842-81A9-7C28757A794A}" name="HeureEntreeVille" dataDxfId="19">
+    <tableColumn id="28" xr3:uid="{87DB48BA-40E9-2842-81A9-7C28757A794A}" name="HeureEntreeVille" dataDxfId="21">
       <calculatedColumnFormula>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="18">
+    <tableColumn id="27" xr3:uid="{C742E3EE-A1EA-443B-8ED2-262CF7394F0A}" name="HeureArrivee" dataDxfId="20">
       <calculatedColumnFormula>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="17"/>
-    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="16"/>
-    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="15"/>
-    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="14"/>
-    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="13"/>
-    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="12">
+    <tableColumn id="29" xr3:uid="{296D98CC-9B61-3A4A-982E-D4453705D813}" name="VilleDep" dataDxfId="19"/>
+    <tableColumn id="31" xr3:uid="{61A48D43-59DF-1742-BF95-701B35EFFC5E}" name="VilleArr" dataDxfId="18"/>
+    <tableColumn id="35" xr3:uid="{FD0EAC1B-5177-134B-962E-7B34C06B11D4}" name="Via" dataDxfId="17"/>
+    <tableColumn id="30" xr3:uid="{85765C9D-3E63-A446-9E4D-6F43565FE723}" name="LieuDepFR" dataDxfId="16"/>
+    <tableColumn id="32" xr3:uid="{6F69E33C-23AD-0742-9451-C7620F744115}" name="LieuArrFR" dataDxfId="15"/>
+    <tableColumn id="33" xr3:uid="{3B628602-BF9E-5047-A829-1312DF11D0D1}" name="LieuDepEN" dataDxfId="14">
       <calculatedColumnFormula>Tableau2[[#This Row],[LieuDepFR]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="11"/>
-    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="10"/>
-    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="9"/>
+    <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="13"/>
+    <tableColumn id="39" xr3:uid="{5A66E4EC-1F67-9D41-BAB2-97579B33260B}" name="Nom_Courts_FR" dataDxfId="0"/>
+    <tableColumn id="38" xr3:uid="{28AFF566-5CAF-CE4B-BC1C-EB69DC8F2BED}" name="Nom_Courts_EN" dataDxfId="1"/>
+    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="12"/>
+    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1569,27 +1657,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="6">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="5">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="4">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="2">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -1933,18 +2021,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <f>20*6</f>
@@ -1956,12 +2044,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -1991,7 +2079,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2008,13 +2096,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2023,7 +2111,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2038,7 +2126,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2053,13 +2141,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2340,7 +2428,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -2357,13 +2445,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2372,7 +2460,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -2387,7 +2475,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -2401,13 +2489,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2439,66 +2527,66 @@
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2506,7 +2594,7 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>62</v>
@@ -2520,7 +2608,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2531,170 +2619,170 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s">
         <v>147</v>
       </c>
-      <c r="B18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" t="s">
-        <v>152</v>
-      </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C19" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2708,10 +2796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
-  <dimension ref="A1:AK14"/>
+  <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2720,52 +2808,54 @@
     <col min="2" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.83203125" customWidth="1"/>
-    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.6640625" customWidth="1"/>
-    <col min="32" max="32" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
+    <col min="23" max="23" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.83203125" customWidth="1"/>
+    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.6640625" customWidth="1"/>
+    <col min="33" max="33" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.1640625" customWidth="1"/>
+    <col min="37" max="37" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -2780,25 +2870,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
+        <v>185</v>
+      </c>
+      <c r="O1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>165</v>
-      </c>
-      <c r="N1" t="s">
-        <v>190</v>
-      </c>
-      <c r="O1" t="s">
-        <v>166</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>167</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -2813,75 +2903,81 @@
         <v>80</v>
       </c>
       <c r="U1" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="V1" t="s">
+        <v>211</v>
+      </c>
+      <c r="W1" t="s">
+        <v>210</v>
+      </c>
+      <c r="X1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AL1" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="V1" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" t="s">
-        <v>215</v>
-      </c>
-      <c r="X1" t="s">
-        <v>213</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>217</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="AC1" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="AI1" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>75</v>
@@ -2927,7 +3023,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>82</v>
+        <v>275</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -2959,51 +3055,57 @@
         <v>0.81145833333333328</v>
       </c>
       <c r="AC2" s="33" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AD2" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AE2" s="33" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AG2" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AH2" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>265</v>
+      </c>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F3" t="s">
         <v>72</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -3078,45 +3180,51 @@
         <v>0.80653409090909089</v>
       </c>
       <c r="AC3" s="33" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="AD3" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="AE3" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF3" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="AE3" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="AF3" s="33" t="s">
-        <v>232</v>
-      </c>
       <c r="AG3" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AH3" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ3" s="32"/>
-      <c r="AK3" s="32"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AL3" s="32"/>
+      <c r="AM3" s="32"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F4" t="s">
         <v>73</v>
@@ -3164,7 +3272,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="31" t="s">
-        <v>83</v>
+        <v>272</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3196,56 +3304,62 @@
         <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AD4" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="AF4" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AG4" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AH4" s="33" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AI4" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ4" s="32" t="str">
+        <v>227</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>260</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL4" s="32" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
         <v>11:40</v>
       </c>
-      <c r="AK4" s="32" t="str">
+      <c r="AM4" s="32" t="str">
         <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[DerDep]],"HH:MM")</f>
         <v>11:53</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -3288,7 +3402,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="31" t="s">
-        <v>84</v>
+        <v>274</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3320,52 +3434,58 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="33" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AD5" s="33" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AE5" s="33" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="AF5" s="34" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="AG5" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="33" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="AI5" s="32" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
-      <c r="AJ5" s="32"/>
-      <c r="AK5" s="32"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.15">
+      <c r="AJ5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AL5" s="32"/>
+      <c r="AM5" s="32"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F6" t="s">
         <v>78</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -3408,7 +3528,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>85</v>
+        <v>276</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3440,51 +3560,57 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="33" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD6" s="32" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="AF6" s="33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AG6" s="33" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AH6" s="33" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AI6" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ6" s="32"/>
-      <c r="AK6" s="32"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>262</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>268</v>
+      </c>
+      <c r="AL6" s="32"/>
+      <c r="AM6" s="32"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F7" t="s">
         <v>77</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -3527,7 +3653,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>86</v>
+        <v>273</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3559,50 +3685,56 @@
         <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AD7" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="AF7" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AG7" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AH7" s="33" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AI7" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ7" s="32"/>
-      <c r="AK7" s="32"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.15">
+        <v>227</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>271</v>
+      </c>
+      <c r="AL7" s="32"/>
+      <c r="AM7" s="32"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3646,7 +3778,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>220</v>
+        <v>277</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3678,39 +3810,41 @@
         <v>0.70794573643410852</v>
       </c>
       <c r="AC8" s="33" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="AD8" s="33" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="AE8" s="33" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AF8" s="33" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="AG8" s="33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="AH8" s="33" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="AI8" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="AJ8" s="32"/>
-      <c r="AK8" s="32"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="Z14" s="16"/>
+        <v>227</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>264</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="32"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AA14" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T7" r:id="rId1" display="https://ridewithgps.com/routes/39650118" xr:uid="{4E1B6279-72A5-4D7A-BF59-67AF4695779D}"/>
-    <hyperlink ref="T6" r:id="rId2" xr:uid="{5216C594-51D3-44FA-9793-C63BF8907F53}"/>
-    <hyperlink ref="T8" r:id="rId3" xr:uid="{6ADD1D3E-718C-764E-8FDE-6A84C5E1F896}"/>
-    <hyperlink ref="T2" r:id="rId4" display="https://ridewithgps.com/routes/39641884" xr:uid="{6E809109-7436-EF40-BB42-B9AF199BF12E}"/>
-    <hyperlink ref="T3" r:id="rId5" xr:uid="{9DB439FE-3F18-9946-8B24-CE9C2E8957D4}"/>
+    <hyperlink ref="T3" r:id="rId1" xr:uid="{9DB439FE-3F18-9946-8B24-CE9C2E8957D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3718,7 +3852,7 @@
     <ignoredError sqref="AH4" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3762,16 +3896,16 @@
         <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>70</v>
@@ -3786,25 +3920,25 @@
         <v>64</v>
       </c>
       <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" t="s">
+        <v>160</v>
+      </c>
+      <c r="O1" t="s">
+        <v>161</v>
+      </c>
+      <c r="P1" s="25" t="s">
         <v>162</v>
-      </c>
-      <c r="K1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L1" t="s">
-        <v>164</v>
-      </c>
-      <c r="M1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" t="s">
-        <v>165</v>
-      </c>
-      <c r="O1" t="s">
-        <v>166</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>167</v>
       </c>
       <c r="Q1" t="s">
         <v>65</v>
@@ -3824,22 +3958,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D2" s="27">
         <v>43660</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
         <v>79</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3881,7 +4015,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
@@ -3889,16 +4023,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D3" s="27">
         <v>43661</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3917,7 +4051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -3931,7 +4065,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -3948,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -3962,7 +4096,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -3976,7 +4110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4032,13 +4166,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4060,13 +4194,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4088,13 +4222,13 @@
         <v>47.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4130,7 +4264,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -4144,10 +4278,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -4172,13 +4306,13 @@
         <v>72.7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4186,7 +4320,7 @@
         <v>74.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4214,7 +4348,7 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -4228,13 +4362,13 @@
         <v>81.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4257,13 +4391,13 @@
         <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4271,7 +4405,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>50</v>
@@ -4299,7 +4433,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4327,7 +4461,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4341,7 +4475,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4355,7 +4489,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -4369,7 +4503,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -4383,7 +4517,7 @@
         <v>109.35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -4397,7 +4531,7 @@
         <v>109.75</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -4411,7 +4545,7 @@
         <v>110.15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -4425,7 +4559,7 @@
         <v>110.7</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -4439,7 +4573,7 @@
         <v>110.75</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -4453,13 +4587,13 @@
         <v>111.2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4467,7 +4601,7 @@
         <v>114.4</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>42</v>
@@ -4481,13 +4615,13 @@
         <v>118.7</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4495,13 +4629,13 @@
         <v>119.9</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4529,7 +4663,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -4546,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -4561,7 +4695,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -4576,7 +4710,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4651,13 +4785,13 @@
         <v>13.4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F9" s="22"/>
     </row>
@@ -4666,13 +4800,13 @@
         <v>34.700000000000003</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F10" s="22"/>
     </row>
@@ -4681,13 +4815,13 @@
         <v>45.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F11" s="22"/>
     </row>
@@ -4711,7 +4845,7 @@
         <v>62.8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>31</v>
@@ -4741,7 +4875,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -4756,10 +4890,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>54</v>
@@ -4774,7 +4908,7 @@
         <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>53</v>
@@ -4786,7 +4920,7 @@
         <v>72.400000000000006</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
@@ -4816,7 +4950,7 @@
         <v>77.8</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
@@ -4846,13 +4980,13 @@
         <v>101.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F22" s="22"/>
     </row>
@@ -4861,7 +4995,7 @@
         <v>101.2</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>50</v>
@@ -4891,7 +5025,7 @@
         <v>104.1</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>16</v>
@@ -4906,13 +5040,13 @@
         <v>119</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F26" s="22"/>
     </row>
@@ -4938,7 +5072,7 @@
         <v>121</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>3</v>
@@ -4954,7 +5088,7 @@
         <v>122</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>47</v>
@@ -4970,7 +5104,7 @@
         <v>123</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4986,7 +5120,7 @@
         <v>124</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -5002,7 +5136,7 @@
         <v>125</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -5018,7 +5152,7 @@
         <v>126</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -5034,7 +5168,7 @@
         <v>127</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -5050,7 +5184,7 @@
         <v>128</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -5066,7 +5200,7 @@
         <v>129</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -5082,7 +5216,7 @@
         <v>130</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -5098,7 +5232,7 @@
         <v>131</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>41</v>
@@ -5114,7 +5248,7 @@
         <v>132</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>42</v>
@@ -5129,13 +5263,13 @@
         <v>136.69999999999999</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F40" s="22"/>
     </row>
@@ -5164,7 +5298,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -5181,7 +5315,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>68</v>
@@ -5195,13 +5329,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -5209,13 +5343,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5242,7 +5376,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -5259,13 +5393,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -5274,7 +5408,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -5289,7 +5423,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -5304,13 +5438,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -5591,7 +5725,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>40</v>
@@ -5608,13 +5742,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5622,7 +5756,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>41</v>
@@ -5636,7 +5770,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -5650,13 +5784,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Correction tableau POIs signalisation et MAJ complète
- Modif identification SQ locale, ville départ, etc. dans le tableau
- Rouler MAJ site et PDF complète
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB601549-C83A-3E4C-B87E-764ACCEF4D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED55FC-9C0C-5348-9844-6CEC3EC58176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31920" yWindow="7520" windowWidth="61460" windowHeight="20600" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1139,44 +1139,6 @@
   </cellStyles>
   <dxfs count="40">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Verdana"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1282,6 +1244,44 @@
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Verdana"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
@@ -1638,10 +1638,10 @@
       <calculatedColumnFormula>Tableau2[[#This Row],[LieuDepFR]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="34" xr3:uid="{B0E21DC6-6191-EC41-B466-9EC0D03723A1}" name="LieuArrEN" dataDxfId="13"/>
-    <tableColumn id="39" xr3:uid="{5A66E4EC-1F67-9D41-BAB2-97579B33260B}" name="Nom_Courts_FR" dataDxfId="0"/>
-    <tableColumn id="38" xr3:uid="{28AFF566-5CAF-CE4B-BC1C-EB69DC8F2BED}" name="Nom_Courts_EN" dataDxfId="1"/>
-    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="12"/>
-    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="11"/>
+    <tableColumn id="39" xr3:uid="{5A66E4EC-1F67-9D41-BAB2-97579B33260B}" name="Nom_Courts_FR" dataDxfId="12"/>
+    <tableColumn id="38" xr3:uid="{28AFF566-5CAF-CE4B-BC1C-EB69DC8F2BED}" name="Nom_Courts_EN" dataDxfId="11"/>
+    <tableColumn id="36" xr3:uid="{FB7B8EE4-54EA-5141-899B-A705EB625FEF}" name="DerDep" dataDxfId="10"/>
+    <tableColumn id="37" xr3:uid="{F766DED6-C846-5F49-BB42-B60596160DD0}" name="DerArr" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1657,27 +1657,27 @@
     <tableColumn id="20" xr3:uid="{C58B5CB5-1055-E946-9174-9CFA1A9F8510}" name="Date"/>
     <tableColumn id="12" xr3:uid="{4DA263EE-9EC0-9142-87D5-E586E56C4A76}" name="Commanditaire"/>
     <tableColumn id="7" xr3:uid="{40EDD296-CC41-0F47-A1E5-1BA23B387446}" name="Descr_Villes"/>
-    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{8FF107E9-B80F-1543-9DB4-25AC43FEAC3E}" name="Descr_km" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{A56A105E-865C-F045-8CFB-93786B5EED14}" name="Heure_dep"/>
-    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{9665B96E-65A0-D74C-9BAC-B6FD984A5691}" name="min_dep" dataDxfId="7"/>
     <tableColumn id="14" xr3:uid="{F711B5B6-E1E2-014E-B099-F8BF32C9584C}" name="KM_Total"/>
     <tableColumn id="13" xr3:uid="{25339A76-1EC8-2A42-8875-D8C55022492F}" name="KM_Neutres"/>
     <tableColumn id="9" xr3:uid="{AAE07AFC-8616-254C-A6DB-E791AF77E841}" name="KM_Route">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Total]]-Tableau24[[#This Row],[KM_Neutres]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{2CD0635C-4E32-3144-B310-A053A714F7B2}" name="Nb_tours" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8BAF726B-764B-E048-82B7-CF9CE3069F74}" name="KM_par_tours" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F5504376-D823-E946-953E-C2E8F4207299}" name="Distance_en_circuit" dataDxfId="4">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_par_tours]]*Tableau24[[#This Row],[Nb_tours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="5">
+    <tableColumn id="15" xr3:uid="{33978460-C816-DB4B-943C-68325B247B09}" name="Distance_totale" dataDxfId="3">
       <calculatedColumnFormula>Tableau24[[#This Row],[KM_Route]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{E93341FB-DCFA-9C47-87D6-6EABB73E10CC}" name="Vit_rapide" dataDxfId="2">
       <calculatedColumnFormula>IF(R2&gt;0,R2+3,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{E0F24E83-4567-2B4F-B51F-F7467CB5F4BE}" name="Vit_moy" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7C611F16-7217-524F-8C1C-D79CEB38C02D}" name="Vit_lent" dataDxfId="0">
       <calculatedColumnFormula>IF(R2&gt;0,R2-2,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{9DEC91ED-8C76-674A-BFEB-DD00DFF6B1ED}" name="Liens" dataCellStyle="Lien hypertexte"/>
@@ -2798,8 +2798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2808,7 +2808,7 @@
     <col min="2" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Modification complète étape 2 RN Poularies Amos, ref #36
- Modifcation des gpx pour nouvelle routes
- Ajout des sprints et signalisation
- Correction des photos de signalisation
- Correction du détails et distances de l'étape
- Correction de la feuille de route (heure arrivée)
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BED55FC-9C0C-5348-9844-6CEC3EC58176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDBEE57-4B28-1B4D-B67B-AA9CDC879211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="7520" windowWidth="61460" windowHeight="20600" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17080" yWindow="4540" windowWidth="61460" windowHeight="20600" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="318">
   <si>
     <t>GPM</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Ville de Cadillac</t>
   </si>
   <si>
-    <t>Sprint du maire de Rouyn-Noranda - $250 (mine Lapa)</t>
-  </si>
-  <si>
     <t>Ville de Rivière-Héva</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>Dernier passage</t>
   </si>
   <si>
-    <t>Start of 1st lap</t>
-  </si>
-  <si>
-    <t>Début du 1er tour</t>
-  </si>
-  <si>
     <t>Railroad crossing</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>City of McWatters</t>
   </si>
   <si>
-    <t>Mayor's sprint - $250 (mine Lapa)</t>
-  </si>
-  <si>
     <t>Route 117 Sud / Highway 117 south</t>
   </si>
   <si>
@@ -309,9 +297,6 @@
     <t>Liens</t>
   </si>
   <si>
-    <t>https://ridewithgps.com/routes/39641737</t>
-  </si>
-  <si>
     <t>Nb_tours</t>
   </si>
   <si>
@@ -378,9 +363,6 @@
     <t>U-turn</t>
   </si>
   <si>
-    <t>Finish&lt;br/&gt;Time and points bonus&lt;br/&gt;(10-6-4 sec; 30-24-20-16-12-10-8-6-4-2 pts)</t>
-  </si>
-  <si>
     <t>Virage gauche</t>
   </si>
   <si>
@@ -528,9 +510,6 @@
     <t>Partenariat Canadian Malartic</t>
   </si>
   <si>
-    <t>Résolu Produits forestiers</t>
-  </si>
-  <si>
     <t>CSS Harricana</t>
   </si>
   <si>
@@ -624,9 +603,6 @@
     <t>Distance_Route</t>
   </si>
   <si>
-    <t>131.7 km</t>
-  </si>
-  <si>
     <t>57.4 km</t>
   </si>
   <si>
@@ -645,18 +621,9 @@
     <t>Val-d'Or - Amos</t>
   </si>
   <si>
-    <t>GPM Points&lt;br/&gt;(Sortie Cléricy)</t>
-  </si>
-  <si>
-    <t>GPM Points&lt;br/&gt;(Côte Lac Dufault)</t>
-  </si>
-  <si>
     <t>Sprint bonification temps et points&lt;br/&gt;(Halte Trecesson)</t>
   </si>
   <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;(Halte Trécesson)</t>
-  </si>
-  <si>
     <t>GPM - Flat de Landirenne</t>
   </si>
   <si>
@@ -687,9 +654,6 @@
     <t>Déviation de la caravane sur la droite</t>
   </si>
   <si>
-    <t>Pont de bois en feu</t>
-  </si>
-  <si>
     <t>Delai Signature</t>
   </si>
   <si>
@@ -795,9 +759,6 @@
     <t>Via</t>
   </si>
   <si>
-    <t>(via Aiguebelle)</t>
-  </si>
-  <si>
     <t>(via Barraute)</t>
   </si>
   <si>
@@ -828,9 +789,6 @@
     <t>98,6 km + ( 5 x 5.4 km) = 125.6 km</t>
   </si>
   <si>
-    <t>(via Palmarolle)</t>
-  </si>
-  <si>
     <t>Demi tour</t>
   </si>
   <si>
@@ -898,6 +856,168 @@
   </si>
   <si>
     <t>https://ridewithgps.com/routes/42183412</t>
+  </si>
+  <si>
+    <t>125.6 km</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42099075</t>
+  </si>
+  <si>
+    <t>(via Poularies)</t>
+  </si>
+  <si>
+    <t>(via Macamic)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Quartier D'Alembert</t>
+  </si>
+  <si>
+    <t>Finish&lt;br/&gt;Time and points bonus&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Boulevard du Collège</t>
+  </si>
+  <si>
+    <t>Rue Tardif</t>
+  </si>
+  <si>
+    <t>Avenue Laliberté</t>
+  </si>
+  <si>
+    <t>Rue Marie-Victorin</t>
+  </si>
+  <si>
+    <t>Rue Perreault Est</t>
+  </si>
+  <si>
+    <t>Rte 117 - Voie de contournement</t>
+  </si>
+  <si>
+    <t>Roundabout (use 1st exit)</t>
+  </si>
+  <si>
+    <t>KOM Points&lt;br/&gt;(Lac Dufault)</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt;(Côte Lac Dufault)</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt;(Intersection chemin forestier)</t>
+  </si>
+  <si>
+    <t>KOM Points&lt;br/&gt;(Intersection forest road)</t>
+  </si>
+  <si>
+    <t>Municipalité de Poularies</t>
+  </si>
+  <si>
+    <t>Municipality of Poularies</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Garage Tony Mercier)</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Tony Mercier Garage)</t>
+  </si>
+  <si>
+    <t>Chemin des Pionniers, route 390</t>
+  </si>
+  <si>
+    <t>Municipalité de Taschereau</t>
+  </si>
+  <si>
+    <t>Municipality of Taschereau</t>
+  </si>
+  <si>
+    <t>Zone déchêts</t>
+  </si>
+  <si>
+    <t>Trash zone</t>
+  </si>
+  <si>
+    <t>Rue Principale</t>
+  </si>
+  <si>
+    <t>Trash</t>
+  </si>
+  <si>
+    <t>&amp;#128465;</t>
+  </si>
+  <si>
+    <t>Route 111</t>
+  </si>
+  <si>
+    <t>Municipalité de Launay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Municipality of Launay </t>
+  </si>
+  <si>
+    <t>Municipalité de Trécesson</t>
+  </si>
+  <si>
+    <t>Municipality of Trécesson</t>
+  </si>
+  <si>
+    <t>Feed closed</t>
+  </si>
+  <si>
+    <t>Fin du ravitaillement</t>
+  </si>
+  <si>
+    <t>Début du ravitaillement</t>
+  </si>
+  <si>
+    <t>Feed open</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Trécesson rest stop)</t>
+  </si>
+  <si>
+    <t>City of Amos</t>
+  </si>
+  <si>
+    <t>Boulevard Mercier</t>
+  </si>
+  <si>
+    <t>2e Avenue Ouest</t>
+  </si>
+  <si>
+    <t>1re Rue Ouest</t>
+  </si>
+  <si>
+    <t>5e Avenue Ouest</t>
+  </si>
+  <si>
+    <t>Rue Principale Nord</t>
+  </si>
+  <si>
+    <t>Dérivation caravane sur la droite</t>
+  </si>
+  <si>
+    <t>Rond-point (prendre 1ère sortie)</t>
+  </si>
+  <si>
+    <t>Rte 117 - Bypass route</t>
+  </si>
+  <si>
+    <t>D'Alembert district</t>
+  </si>
+  <si>
+    <t>Rouyn-Noranda Mayor's sprint&lt;br/&gt;$250 (Reneault Parc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rouyn-Noranda Mayor's sprint&lt;br/&gt;$250 (Engoulevent municipal parc) </t>
+  </si>
+  <si>
+    <t>Sprint de la mairesse de Rouyn-Noranda&lt;br/&gt;$250 (Parc Renault)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint de la mairesse de Rouyn-Noranda&lt;br/&gt;$250 (Parc municipal Engoulevent) </t>
   </si>
 </sst>
 </file>
@@ -908,7 +1028,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -979,6 +1099,17 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1065,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1132,6 +1263,35 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2021,18 +2181,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <f>20*6</f>
@@ -2044,12 +2204,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2079,16 +2239,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -2096,13 +2256,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2111,13 +2271,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -2126,13 +2286,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -2141,13 +2301,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2428,16 +2588,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -2445,13 +2605,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2460,13 +2620,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -2475,13 +2635,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
@@ -2489,13 +2649,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2506,10 +2666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2521,86 +2681,86 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -2608,7 +2768,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2619,170 +2779,184 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" t="s">
         <v>142</v>
       </c>
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>199</v>
+      <c r="A19" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="B19" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2798,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2843,121 +3017,121 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="M1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="N1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="O1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="Q1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T1" s="30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="V1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="W1" t="s">
+        <v>198</v>
+      </c>
+      <c r="X1" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="AG1" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="X1" t="s">
-        <v>208</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>209</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AH1" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="AA1" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>224</v>
-      </c>
       <c r="AI1" s="33" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="AJ1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="AK1" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="AL1" s="16" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="AM1" s="16" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
@@ -2965,22 +3139,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -3023,7 +3197,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3055,32 +3229,32 @@
         <v>0.81145833333333328</v>
       </c>
       <c r="AC2" s="33" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="AD2" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AE2" s="33" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="AG2" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AH2" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AJ2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="AK2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="AL2" s="32"/>
       <c r="AM2" s="32"/>
@@ -3090,22 +3264,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>186</v>
+        <v>264</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -3114,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <v>136.69999999999999</v>
+        <v>130.6</v>
       </c>
       <c r="K3">
         <v>5</v>
@@ -3127,7 +3301,7 @@
       </c>
       <c r="N3" s="28">
         <f t="shared" si="0"/>
-        <v>131.69999999999999</v>
+        <v>125.6</v>
       </c>
       <c r="O3" s="28">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
@@ -3135,7 +3309,7 @@
       </c>
       <c r="P3" s="29">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>131.69999999999999</v>
+        <v>125.6</v>
       </c>
       <c r="Q3">
         <v>46</v>
@@ -3148,7 +3322,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>81</v>
+        <v>265</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3173,39 +3347,39 @@
       </c>
       <c r="AA3" s="32" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:21</v>
+        <v>19:13</v>
       </c>
       <c r="AB3" s="32">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.80653409090909089</v>
+        <v>0.80075757575757578</v>
       </c>
       <c r="AC3" s="33" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="AD3" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AE3" s="33" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="AF3" s="33" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="AG3" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AH3" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AJ3" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="AK3" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="AL3" s="32"/>
       <c r="AM3" s="32"/>
@@ -3215,22 +3389,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H4">
         <v>9</v>
@@ -3272,7 +3446,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="31" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3304,31 +3478,31 @@
         <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AD4" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="AF4" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AG4" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AH4" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AI4" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AJ4" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="AK4" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="AL4" s="32" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -3344,22 +3518,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -3402,7 +3576,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="31" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3434,33 +3608,33 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="33" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="AD5" s="33" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="AE5" s="33" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="AF5" s="34" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="AG5" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="33" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="AI5" s="32" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="AK5" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="AL5" s="32"/>
       <c r="AM5" s="32"/>
@@ -3470,22 +3644,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -3528,7 +3702,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3560,32 +3734,32 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="33" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="AD6" s="32" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="AF6" s="33" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="AG6" s="33" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="AH6" s="33" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="AI6" s="33" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="AJ6" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="AK6" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="AL6" s="32"/>
       <c r="AM6" s="32"/>
@@ -3595,22 +3769,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -3653,7 +3827,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3685,31 +3859,31 @@
         <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AD7" s="33" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="AF7" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AG7" s="33" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="AH7" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AI7" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AJ7" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="AK7" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="AL7" s="32"/>
       <c r="AM7" s="32"/>
@@ -3719,22 +3893,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3778,7 +3952,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3810,31 +3984,31 @@
         <v>0.70794573643410852</v>
       </c>
       <c r="AC8" s="33" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="AD8" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="AE8" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF8" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="AG8" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH8" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="AE8" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="AF8" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="AG8" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="AH8" s="33" t="s">
-        <v>232</v>
-      </c>
       <c r="AI8" s="33" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="AJ8" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="AK8" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="AL8" s="32"/>
       <c r="AM8" s="32"/>
@@ -3843,16 +4017,13 @@
       <c r="AA14" s="16"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="T3" r:id="rId1" xr:uid="{9DB439FE-3F18-9946-8B24-CE9C2E8957D4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="AH4" calculatedColumn="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3893,64 +4064,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="O1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="Q1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
@@ -3958,22 +4129,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D2" s="27">
         <v>43660</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -4015,7 +4186,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
@@ -4023,16 +4194,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D3" s="27">
         <v>43661</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -4065,16 +4236,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4082,13 +4253,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4096,7 +4267,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -4110,7 +4281,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4124,7 +4295,7 @@
         <v>7.9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>28</v>
@@ -4144,7 +4315,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4152,7 +4323,7 @@
         <v>12.1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -4166,13 +4337,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4180,7 +4351,7 @@
         <v>24.6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>28</v>
@@ -4194,13 +4365,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4208,7 +4379,7 @@
         <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
@@ -4222,13 +4393,13 @@
         <v>47.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4242,7 +4413,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4253,10 +4424,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4264,13 +4435,13 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4278,13 +4449,13 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4292,13 +4463,13 @@
         <v>62.8</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4306,13 +4477,13 @@
         <v>72.7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4320,13 +4491,13 @@
         <v>74.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4340,7 +4511,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4348,7 +4519,7 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -4362,13 +4533,13 @@
         <v>81.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4376,7 +4547,7 @@
         <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
@@ -4391,13 +4562,13 @@
         <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4405,13 +4576,13 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4419,13 +4590,13 @@
         <v>101.7</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4433,7 +4604,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4447,13 +4618,13 @@
         <v>107.5</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4461,7 +4632,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4475,7 +4646,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4489,7 +4660,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -4503,7 +4674,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -4517,7 +4688,7 @@
         <v>109.35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -4531,7 +4702,7 @@
         <v>109.75</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -4545,7 +4716,7 @@
         <v>110.15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -4559,7 +4730,7 @@
         <v>110.7</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -4573,7 +4744,7 @@
         <v>110.75</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -4587,13 +4758,13 @@
         <v>111.2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4601,13 +4772,13 @@
         <v>114.4</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4615,13 +4786,13 @@
         <v>118.7</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4629,13 +4800,13 @@
         <v>119.9</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4647,10 +4818,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4658,622 +4829,619 @@
     <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11" style="1"/>
+    <col min="5" max="6" width="11" style="1"/>
+    <col min="7" max="7" width="11" style="44"/>
+    <col min="8" max="8" width="11" style="45"/>
+    <col min="9" max="10" width="47.6640625" style="46" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+      <c r="K1" s="37"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="38">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="41" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="38">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="22"/>
+      <c r="K3" s="37"/>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="38">
+        <v>0.2</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
+        <v>8</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="K5" s="37"/>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="38">
+        <v>0.9</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="K6" s="37"/>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="38">
+        <v>2.7</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="K7" s="37"/>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="38">
+        <v>4</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="K8" s="37"/>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="38">
+        <v>5</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="K9" s="37"/>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="38">
+        <v>9.1</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="C10" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="K10" s="37"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="38">
+        <v>13.4</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="K11" s="37"/>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A12" s="38">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="K12" s="36"/>
+    </row>
+    <row r="13" spans="1:11" ht="26" x14ac:dyDescent="0.15">
+      <c r="A13" s="38">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="K13" s="36"/>
+    </row>
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="38">
+        <v>35</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="K14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="38">
+        <v>43.6</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="K15" s="37"/>
+    </row>
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="38">
+        <v>60.1</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" s="38">
+        <v>60.2</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="K17" s="37"/>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="38">
+        <v>60.4</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="K18" s="37"/>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="38">
+        <v>81.7</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>287</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="K19" s="37"/>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="38">
+        <v>82</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>290</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="K20" s="37"/>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="38">
+        <v>93</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="K21" s="37"/>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="38">
+        <v>83.1</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="K22" s="37"/>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="38">
+        <v>83.2</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="K23" s="37"/>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="38">
+        <v>86.8</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="K24" s="37"/>
+    </row>
+    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="38">
+        <v>94.5</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>296</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="K25" s="36"/>
+    </row>
+    <row r="26" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A26" s="38">
+        <v>95</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>315</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="K26" s="37"/>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="38">
+        <v>106.6</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D27" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="3">
-        <v>8</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="F27" s="22"/>
+      <c r="K27" s="37"/>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="38">
+        <v>108.3</v>
+      </c>
+      <c r="B28" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="3">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
-        <v>45.5</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="3">
-        <v>47.4</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="C28" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="F28" s="22"/>
+      <c r="K28" s="37"/>
+    </row>
+    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A29" s="38">
+        <v>110.6</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+      <c r="A30" s="38">
+        <v>112.9</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="F30" s="22"/>
+      <c r="K30" s="37"/>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="38">
+        <v>127.4</v>
+      </c>
+      <c r="B31" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="3">
-        <v>62.8</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="3">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="3">
-        <v>61.3</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="3">
-        <v>61.8</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="3">
-        <v>62.8</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="3">
-        <v>72.400000000000006</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="3">
-        <v>77.5</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="3">
-        <v>77.8</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="3">
-        <v>98</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
-        <v>101.1</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="3">
-        <v>101.2</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="3">
-        <v>101.7</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="3">
-        <v>104.1</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A26" s="3">
-        <v>119</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
-        <f>A26+1</f>
-        <v>120</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="3">
-        <f t="shared" ref="A28:A39" si="0">A27+1</f>
-        <v>121</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="3">
-        <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="3">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A31" s="3">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>5</v>
+      <c r="C31" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>304</v>
       </c>
       <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="3">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>6</v>
+      <c r="K31" s="37"/>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="38">
+        <v>129.4</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>305</v>
       </c>
       <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="3">
-        <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>7</v>
+      <c r="K32" s="37"/>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="38">
+        <v>129.5</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>306</v>
       </c>
       <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="3">
-        <f t="shared" si="0"/>
-        <v>127</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>8</v>
+      <c r="K33" s="37"/>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="38">
+        <v>129.69999999999999</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>307</v>
       </c>
       <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="3">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>5</v>
+      <c r="K34" s="37"/>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="38">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="B35" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>189</v>
       </c>
       <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="3">
-        <f t="shared" si="0"/>
-        <v>129</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>9</v>
+      <c r="K35" s="37"/>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="38">
+        <v>130.1</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>308</v>
       </c>
       <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="3">
-        <f t="shared" si="0"/>
+      <c r="K36" s="37"/>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="38">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="B37" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>3</v>
+      <c r="C37" s="39" t="s">
+        <v>309</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>309</v>
       </c>
       <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="3">
-        <f t="shared" si="0"/>
-        <v>131</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>43</v>
+      <c r="K37" s="37"/>
+    </row>
+    <row r="38" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A38" s="38">
+        <v>130.6</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>270</v>
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="3">
-        <f t="shared" si="0"/>
-        <v>132</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A40" s="3">
-        <v>136.69999999999999</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5298,16 +5466,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5315,13 +5483,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5329,13 +5497,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -5343,13 +5511,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -5376,16 +5544,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -5393,13 +5561,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -5408,13 +5576,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="22"/>
     </row>
@@ -5423,13 +5591,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="22"/>
     </row>
@@ -5438,13 +5606,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -5725,16 +5893,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5742,13 +5910,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5756,13 +5924,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5770,13 +5938,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -5784,13 +5952,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Compil et corrections étape 2, ref #36
- Compilation complète après modification étape 2
- Correction champs Étapex.rmd
- Correction unicode pour affichage web et pdf
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDBEE57-4B28-1B4D-B67B-AA9CDC879211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C06607F-05A5-4F41-801B-7240480AFF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="4540" windowWidth="61460" windowHeight="20600" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="3500" windowWidth="22440" windowHeight="20600" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="316">
   <si>
     <t>GPM</t>
   </si>
@@ -372,27 +372,15 @@
     <t>&amp;#8634;</t>
   </si>
   <si>
-    <t>&amp;#65284;</t>
-  </si>
-  <si>
-    <t>&amp;#127937;</t>
-  </si>
-  <si>
     <t>&amp;#9888;</t>
   </si>
   <si>
-    <t>&amp;#129001;</t>
-  </si>
-  <si>
     <t>&amp;#128276;</t>
   </si>
   <si>
     <t>&amp;#9968;</t>
   </si>
   <si>
-    <t>&amp;#127942;</t>
-  </si>
-  <si>
     <t>Source des unicodes pour Emoji : https://unicode-table.com/</t>
   </si>
   <si>
@@ -495,9 +483,6 @@
     <t>Feeding</t>
   </si>
   <si>
-    <t>&amp;#127868;</t>
-  </si>
-  <si>
     <t>Commanditaire</t>
   </si>
   <si>
@@ -945,9 +930,6 @@
     <t>Trash</t>
   </si>
   <si>
-    <t>&amp;#128465;</t>
-  </si>
-  <si>
     <t>Route 111</t>
   </si>
   <si>
@@ -1018,6 +1000,18 @@
   </si>
   <si>
     <t xml:space="preserve">Sprint de la mairesse de Rouyn-Noranda&lt;br/&gt;$250 (Parc municipal Engoulevent) </t>
+  </si>
+  <si>
+    <t>&amp;#9851;</t>
+  </si>
+  <si>
+    <t>&amp;#9873;</t>
+  </si>
+  <si>
+    <t>&amp;#36;</t>
+  </si>
+  <si>
+    <t>&amp;#9749;</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1265,33 +1259,34 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2184,10 +2179,10 @@
         <v>78</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2204,12 +2199,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2239,7 +2234,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -2256,13 +2251,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2271,7 +2266,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -2286,7 +2281,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>41</v>
@@ -2304,10 +2299,10 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -2588,7 +2583,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -2605,13 +2600,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -2620,7 +2615,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -2635,7 +2630,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>41</v>
@@ -2652,10 +2647,10 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +2664,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2695,10 +2690,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>84</v>
@@ -2709,10 +2704,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
+        <v>133</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>313</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
@@ -2723,10 +2718,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>44</v>
@@ -2739,8 +2734,8 @@
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
-        <v>103</v>
+      <c r="B5" s="16" t="s">
+        <v>313</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
@@ -2754,7 +2749,7 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>58</v>
@@ -2768,7 +2763,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2779,10 +2774,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>108</v>
+        <v>124</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>313</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
@@ -2793,10 +2788,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
@@ -2807,10 +2802,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>102</v>
+        <v>135</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>314</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
@@ -2821,10 +2816,10 @@
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>34</v>
@@ -2835,10 +2830,10 @@
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>99</v>
@@ -2849,10 +2844,10 @@
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>100</v>
@@ -2863,10 +2858,10 @@
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>35</v>
@@ -2877,10 +2872,10 @@
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>36</v>
@@ -2891,7 +2886,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>101</v>
@@ -2905,7 +2900,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
         <v>101</v>
@@ -2919,44 +2914,44 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" t="s">
-        <v>143</v>
+        <v>132</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>315</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2972,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3020,16 +3015,16 @@
         <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
@@ -3044,25 +3039,25 @@
         <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
         <v>77</v>
       </c>
       <c r="M1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="N1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O1" t="s">
-        <v>154</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>155</v>
+        <v>149</v>
+      </c>
+      <c r="P1" s="47" t="s">
+        <v>150</v>
       </c>
       <c r="Q1" t="s">
         <v>61</v>
@@ -3077,61 +3072,61 @@
         <v>76</v>
       </c>
       <c r="U1" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="V1" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" t="s">
+        <v>193</v>
+      </c>
+      <c r="X1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH1" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="AI1" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>240</v>
+      </c>
+      <c r="AL1" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="V1" t="s">
-        <v>199</v>
-      </c>
-      <c r="W1" t="s">
-        <v>198</v>
-      </c>
-      <c r="X1" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="AI1" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>244</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>245</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="AM1" s="16" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
@@ -3139,19 +3134,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D2" s="27">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>71</v>
@@ -3197,7 +3192,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3229,32 +3224,32 @@
         <v>0.81145833333333328</v>
       </c>
       <c r="AC2" s="33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="AD2" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE2" s="33" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AG2" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AH2" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AJ2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="AK2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="AL2" s="32"/>
       <c r="AM2" s="32"/>
@@ -3264,22 +3259,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D3" s="27">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
         <v>68</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -3322,7 +3317,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3354,32 +3349,32 @@
         <v>0.80075757575757578</v>
       </c>
       <c r="AC3" s="33" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="AD3" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE3" s="33" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AF3" s="33" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="AG3" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AH3" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AJ3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="AK3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="AL3" s="32"/>
       <c r="AM3" s="32"/>
@@ -3389,16 +3384,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D4" s="27">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
@@ -3446,7 +3441,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="31" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3478,31 +3473,31 @@
         <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AD4" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AF4" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AG4" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AH4" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AI4" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AJ4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AK4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="AL4" s="32" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -3518,22 +3513,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D5" s="27">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F5" t="s">
         <v>72</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -3576,7 +3571,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="31" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3608,33 +3603,33 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="33" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AD5" s="33" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AE5" s="33" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AF5" s="34" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="AG5" s="33" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="33" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="AI5" s="32" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="AK5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="AL5" s="32"/>
       <c r="AM5" s="32"/>
@@ -3644,22 +3639,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D6" s="27">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -3702,7 +3697,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3734,32 +3729,32 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="33" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AD6" s="32" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="33" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AF6" s="33" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AG6" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AH6" s="33" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AI6" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AJ6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="AK6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="AL6" s="32"/>
       <c r="AM6" s="32"/>
@@ -3769,22 +3764,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D7" s="27">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F7" t="s">
         <v>73</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -3827,7 +3822,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="31" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3859,31 +3854,31 @@
         <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AD7" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE7" s="33" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="AF7" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AG7" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AH7" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AI7" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AJ7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="AK7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AL7" s="32"/>
       <c r="AM7" s="32"/>
@@ -3893,22 +3888,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D8" s="27">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3952,7 +3947,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="31" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3984,31 +3979,31 @@
         <v>0.70794573643410852</v>
       </c>
       <c r="AC8" s="33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AD8" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="AE8" s="33" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AF8" s="33" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="AG8" s="33" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="AH8" s="33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="AI8" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AJ8" t="s">
+        <v>245</v>
+      </c>
+      <c r="AK8" t="s">
         <v>250</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>255</v>
       </c>
       <c r="AL8" s="32"/>
       <c r="AM8" s="32"/>
@@ -4067,16 +4062,16 @@
         <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
@@ -4091,25 +4086,25 @@
         <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M1" t="s">
         <v>77</v>
       </c>
       <c r="N1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="O1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Q1" t="s">
         <v>61</v>
@@ -4129,22 +4124,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D2" s="27">
         <v>43660</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>75</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -4186,7 +4181,7 @@
         <v>41</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
@@ -4194,16 +4189,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D3" s="27">
         <v>43661</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4223,7 +4218,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4236,7 +4231,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -4253,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>64</v>
@@ -4267,7 +4262,7 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -4281,7 +4276,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -4337,13 +4332,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4365,13 +4360,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4393,13 +4388,13 @@
         <v>47.5</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4435,7 +4430,7 @@
         <v>61.3</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>2</v>
@@ -4449,10 +4444,10 @@
         <v>61.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>51</v>
@@ -4477,13 +4472,13 @@
         <v>72.7</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4491,7 +4486,7 @@
         <v>74.400000000000006</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>10</v>
@@ -4519,7 +4514,7 @@
         <v>77.8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -4533,13 +4528,13 @@
         <v>81.8</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4562,7 +4557,7 @@
         <v>108</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>80</v>
@@ -4576,7 +4571,7 @@
         <v>101.2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>47</v>
@@ -4604,7 +4599,7 @@
         <v>104.1</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>16</v>
@@ -4632,7 +4627,7 @@
         <v>107.9</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>3</v>
@@ -4646,7 +4641,7 @@
         <v>108.2</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -4660,7 +4655,7 @@
         <v>108.4</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
@@ -4674,7 +4669,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>6</v>
@@ -4688,7 +4683,7 @@
         <v>109.35</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>7</v>
@@ -4702,7 +4697,7 @@
         <v>109.75</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -4716,7 +4711,7 @@
         <v>110.15</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
@@ -4730,7 +4725,7 @@
         <v>110.7</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>9</v>
@@ -4744,7 +4739,7 @@
         <v>110.75</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>3</v>
@@ -4758,13 +4753,13 @@
         <v>111.2</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4772,7 +4767,7 @@
         <v>114.4</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>41</v>
@@ -4786,13 +4781,13 @@
         <v>118.7</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -4803,10 +4798,10 @@
         <v>88</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4820,8 +4815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4838,7 +4833,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -4856,7 +4851,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="40" t="s">
         <v>24</v>
@@ -4872,13 +4867,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F3" s="22"/>
       <c r="K3" s="37"/>
@@ -4888,29 +4883,29 @@
         <v>0.2</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F4" s="22"/>
       <c r="K4" s="37"/>
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="38">
-        <v>8</v>
+        <v>0.8</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F5" s="22"/>
       <c r="K5" s="37"/>
@@ -4920,13 +4915,13 @@
         <v>0.9</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F6" s="22"/>
       <c r="K6" s="37"/>
@@ -4936,13 +4931,13 @@
         <v>2.7</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F7" s="22"/>
       <c r="K7" s="37"/>
@@ -4952,13 +4947,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F8" s="22"/>
       <c r="K8" s="37"/>
@@ -4968,7 +4963,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>26</v>
@@ -4984,13 +4979,13 @@
         <v>9.1</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F10" s="22"/>
       <c r="K10" s="37"/>
@@ -5000,13 +4995,13 @@
         <v>13.4</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F11" s="22"/>
       <c r="K11" s="37"/>
@@ -5019,10 +5014,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F12" s="22"/>
       <c r="K12" s="36"/>
@@ -5032,13 +5027,13 @@
         <v>34.700000000000003</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F13" s="22"/>
       <c r="K13" s="36"/>
@@ -5048,13 +5043,13 @@
         <v>35</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F14" s="22"/>
       <c r="K14" s="36"/>
@@ -5064,13 +5059,13 @@
         <v>43.6</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F15" s="22"/>
       <c r="K15" s="37"/>
@@ -5083,10 +5078,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F16" s="22"/>
       <c r="K16" s="36"/>
@@ -5096,13 +5091,13 @@
         <v>60.2</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F17" s="22"/>
       <c r="K17" s="37"/>
@@ -5112,13 +5107,13 @@
         <v>60.4</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F18" s="22"/>
       <c r="K18" s="37"/>
@@ -5131,10 +5126,10 @@
         <v>19</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F19" s="22"/>
       <c r="K19" s="37"/>
@@ -5144,29 +5139,29 @@
         <v>82</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F20" s="22"/>
       <c r="K20" s="37"/>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="38">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F21" s="22"/>
       <c r="K21" s="37"/>
@@ -5192,13 +5187,13 @@
         <v>83.2</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F23" s="22"/>
       <c r="K23" s="37"/>
@@ -5227,10 +5222,10 @@
         <v>19</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F25" s="22"/>
       <c r="K25" s="36"/>
@@ -5240,13 +5235,13 @@
         <v>95</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="F26" s="22"/>
       <c r="K26" s="37"/>
@@ -5275,10 +5270,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F28" s="22"/>
       <c r="K28" s="37"/>
@@ -5288,13 +5283,13 @@
         <v>110.6</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F29" s="22"/>
       <c r="K29" s="36"/>
@@ -5304,13 +5299,13 @@
         <v>112.9</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="F30" s="22"/>
       <c r="K30" s="37"/>
@@ -5323,10 +5318,10 @@
         <v>19</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="F31" s="22"/>
       <c r="K31" s="37"/>
@@ -5336,13 +5331,13 @@
         <v>129.4</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F32" s="22"/>
       <c r="K32" s="37"/>
@@ -5352,13 +5347,13 @@
         <v>129.5</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F33" s="22"/>
       <c r="K33" s="37"/>
@@ -5368,13 +5363,13 @@
         <v>129.69999999999999</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F34" s="22"/>
       <c r="K34" s="37"/>
@@ -5384,13 +5379,13 @@
         <v>129.80000000000001</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F35" s="22"/>
       <c r="K35" s="37"/>
@@ -5400,13 +5395,13 @@
         <v>130.1</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="F36" s="22"/>
       <c r="K36" s="37"/>
@@ -5416,13 +5411,13 @@
         <v>130.30000000000001</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F37" s="22"/>
       <c r="K37" s="37"/>
@@ -5435,10 +5430,10 @@
         <v>88</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F38" s="22"/>
     </row>
@@ -5466,7 +5461,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -5483,7 +5478,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>64</v>
@@ -5497,13 +5492,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -5514,10 +5509,10 @@
         <v>88</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -5544,7 +5539,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -5561,13 +5556,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F2" s="22"/>
     </row>
@@ -5576,7 +5571,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -5591,7 +5586,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>41</v>
@@ -5609,10 +5604,10 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F5" s="22"/>
     </row>
@@ -5893,7 +5888,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>39</v>
@@ -5910,13 +5905,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -5924,7 +5919,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>40</v>
@@ -5938,7 +5933,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>41</v>
@@ -5955,10 +5950,10 @@
         <v>88</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Ajout signalisation étape 7, ref #36
- GPX et cusheet pour signalisation étape 7 La Sarre
- Ajout photos de signalisation
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF90573F-2B4F-1D40-A94F-5517CEC1309B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12586A8-7953-EC4F-BE66-FD2B3D6D9337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="2020" windowWidth="22440" windowHeight="20600" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="2020" windowWidth="41460" windowHeight="20600" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="313">
   <si>
     <t>GPM</t>
   </si>
@@ -755,9 +755,6 @@
     <t>(via Val-d'Or)</t>
   </si>
   <si>
-    <t>98,6 km + ( 5 x 5.4 km) = 125.6 km</t>
-  </si>
-  <si>
     <t>Demi tour</t>
   </si>
   <si>
@@ -996,6 +993,15 @@
   </si>
   <si>
     <t>&amp;#9749;</t>
+  </si>
+  <si>
+    <t>93.5 km + ( 5 x 5.4 km) = 120.5 km</t>
+  </si>
+  <si>
+    <t>Départ - Stationnement Aréna Nicol Auto</t>
+  </si>
+  <si>
+    <t>Start - Nicol Auto Arena Parking</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1090,6 +1096,35 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1117,7 +1152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1169,12 +1204,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1269,6 +1317,35 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2061,89 +2138,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" style="46" customWidth="1"/>
+    <col min="4" max="4" width="54" style="46" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.15">
+      <c r="A1" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="48" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.15">
+      <c r="A2" s="49">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="50" t="s">
         <v>116</v>
       </c>
+      <c r="C2" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>312</v>
+      </c>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>111.2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>42</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56"/>
       <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>109</v>
-      </c>
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="53"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2199,7 +2253,7 @@
         <v>132</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
@@ -2227,7 +2281,7 @@
         <v>87</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
@@ -2269,7 +2323,7 @@
         <v>123</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
@@ -2297,7 +2351,7 @@
         <v>134</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
@@ -2409,7 +2463,7 @@
         <v>131</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C18" t="s">
         <v>136</v>
@@ -2434,16 +2488,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>279</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2459,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView topLeftCell="U1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2469,13 +2523,14 @@
     <col min="2" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" customWidth="1"/>
     <col min="8" max="8" width="33.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.5" bestFit="1" customWidth="1"/>
@@ -2609,10 +2664,10 @@
         <v>203</v>
       </c>
       <c r="AJ1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AK1" t="s">
         <v>234</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>235</v>
       </c>
       <c r="AL1" s="16" t="s">
         <v>224</v>
@@ -2684,7 +2739,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -2738,10 +2793,10 @@
         <v>205</v>
       </c>
       <c r="AJ2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AK2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -2766,7 +2821,7 @@
         <v>68</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -2809,7 +2864,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -2847,7 +2902,7 @@
         <v>198</v>
       </c>
       <c r="AE3" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AF3" s="31" t="s">
         <v>204</v>
@@ -2863,10 +2918,10 @@
         <v>205</v>
       </c>
       <c r="AJ3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AK3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -2933,7 +2988,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -2986,10 +3041,10 @@
         <v>205</v>
       </c>
       <c r="AJ4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AK4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -3063,7 +3118,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3118,10 +3173,10 @@
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AK5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AL5" s="30"/>
       <c r="AM5" s="30"/>
@@ -3140,7 +3195,7 @@
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
@@ -3189,7 +3244,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3243,10 +3298,10 @@
         <v>216</v>
       </c>
       <c r="AJ6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AK6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -3314,7 +3369,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3367,10 +3422,10 @@
         <v>205</v>
       </c>
       <c r="AJ7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AK7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -3395,7 +3450,7 @@
         <v>193</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>230</v>
+        <v>310</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -3404,8 +3459,8 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <f>101.6+Tableau2[[#This Row],[Nb_tours]]*Tableau2[[#This Row],[KM_par_tours]]</f>
-        <v>128.6</v>
+        <f>96.5+Tableau2[[#This Row],[Nb_tours]]*Tableau2[[#This Row],[KM_par_tours]]</f>
+        <v>123.5</v>
       </c>
       <c r="K8">
         <v>3</v>
@@ -3418,7 +3473,7 @@
       </c>
       <c r="N8" s="26">
         <f t="shared" ref="N8" si="2">P8-O8</f>
-        <v>98.6</v>
+        <v>93.5</v>
       </c>
       <c r="O8" s="26">
         <f>Tableau2[[#This Row],[KM_par_tours]]*Tableau2[[#This Row],[Nb_tours]]</f>
@@ -3426,7 +3481,7 @@
       </c>
       <c r="P8" s="27">
         <f>Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[KM_Neutres]]</f>
-        <v>125.6</v>
+        <v>120.5</v>
       </c>
       <c r="Q8">
         <v>45</v>
@@ -3439,7 +3494,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -3464,11 +3519,11 @@
       </c>
       <c r="AA8" s="30" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>16:21</v>
+        <v>16:14</v>
       </c>
       <c r="AB8" s="30">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.70794573643410852</v>
+        <v>0.70300387596899228</v>
       </c>
       <c r="AC8" s="31" t="s">
         <v>208</v>
@@ -3477,7 +3532,7 @@
         <v>198</v>
       </c>
       <c r="AE8" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AF8" s="31" t="s">
         <v>209</v>
@@ -3492,10 +3547,10 @@
         <v>205</v>
       </c>
       <c r="AJ8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AK8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -3519,7 +3574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -4172,10 +4227,10 @@
         <v>125</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="21"/>
       <c r="K3" s="35"/>
@@ -4188,10 +4243,10 @@
         <v>126</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F4" s="21"/>
       <c r="K4" s="35"/>
@@ -4204,10 +4259,10 @@
         <v>126</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F5" s="21"/>
       <c r="K5" s="35"/>
@@ -4220,10 +4275,10 @@
         <v>125</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F6" s="21"/>
       <c r="K6" s="35"/>
@@ -4236,10 +4291,10 @@
         <v>125</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F7" s="21"/>
       <c r="K7" s="35"/>
@@ -4252,10 +4307,10 @@
         <v>126</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
@@ -4284,10 +4339,10 @@
         <v>135</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -4300,10 +4355,10 @@
         <v>124</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -4316,10 +4371,10 @@
         <v>19</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F12" s="21"/>
       <c r="K12" s="34"/>
@@ -4332,10 +4387,10 @@
         <v>134</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -4348,10 +4403,10 @@
         <v>131</v>
       </c>
       <c r="C14" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="37" t="s">
         <v>290</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>291</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
@@ -4364,10 +4419,10 @@
         <v>124</v>
       </c>
       <c r="C15" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="38" t="s">
         <v>270</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>271</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -4380,10 +4435,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>272</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>273</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -4396,10 +4451,10 @@
         <v>123</v>
       </c>
       <c r="C17" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="D17" s="38" t="s">
         <v>274</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>275</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -4412,10 +4467,10 @@
         <v>125</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F18" s="21"/>
       <c r="K18" s="35"/>
@@ -4428,10 +4483,10 @@
         <v>19</v>
       </c>
       <c r="C19" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" s="37" t="s">
         <v>277</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>278</v>
       </c>
       <c r="F19" s="21"/>
       <c r="K19" s="35"/>
@@ -4441,13 +4496,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C20" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="37" t="s">
         <v>279</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>280</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -4460,10 +4515,10 @@
         <v>126</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -4492,10 +4547,10 @@
         <v>125</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -4524,10 +4579,10 @@
         <v>19</v>
       </c>
       <c r="C25" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="37" t="s">
         <v>284</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>285</v>
       </c>
       <c r="F25" s="21"/>
       <c r="K25" s="34"/>
@@ -4540,10 +4595,10 @@
         <v>134</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -4572,10 +4627,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="37" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>286</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>287</v>
       </c>
       <c r="F28" s="21"/>
       <c r="K28" s="35"/>
@@ -4588,10 +4643,10 @@
         <v>131</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -4607,7 +4662,7 @@
         <v>176</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -4623,7 +4678,7 @@
         <v>143</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -4636,10 +4691,10 @@
         <v>126</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -4652,10 +4707,10 @@
         <v>125</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -4668,10 +4723,10 @@
         <v>126</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
@@ -4684,7 +4739,7 @@
         <v>179</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D35" s="37" t="s">
         <v>180</v>
@@ -4700,10 +4755,10 @@
         <v>125</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -4716,10 +4771,10 @@
         <v>125</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
@@ -4735,7 +4790,7 @@
         <v>174</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F38" s="21"/>
     </row>
@@ -4797,7 +4852,7 @@
         <v>130</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Ajout course - étape 7, ref #36
- Ajout GPX
- Ajout onglets à itinéraire pour étape 7
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C31C58-F9E6-AB4E-9C0D-2AD8F0E1983D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B829A34-A651-DA49-9065-C6A7E19195C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="2320" windowWidth="41460" windowHeight="20600" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24300" yWindow="4560" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="351">
   <si>
     <t>GPM</t>
   </si>
@@ -842,9 +842,6 @@
     <t>Quartier D'Alembert</t>
   </si>
   <si>
-    <t>Finish&lt;br/&gt;Time and points bonus&lt;br/&gt;</t>
-  </si>
-  <si>
     <t>Boulevard du Collège</t>
   </si>
   <si>
@@ -872,12 +869,6 @@
     <t>Points GPM&lt;br/&gt;(Côte Lac Dufault)</t>
   </si>
   <si>
-    <t>Points GPM&lt;br/&gt;(Intersection chemin forestier)</t>
-  </si>
-  <si>
-    <t>KOM Points&lt;br/&gt;(Intersection forest road)</t>
-  </si>
-  <si>
     <t>Municipalité de Poularies</t>
   </si>
   <si>
@@ -887,9 +878,6 @@
     <t>Sprint bonification temps et points&lt;br/&gt;(Garage Tony Mercier)</t>
   </si>
   <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;(Tony Mercier Garage)</t>
-  </si>
-  <si>
     <t>Chemin des Pionniers, route 390</t>
   </si>
   <si>
@@ -938,9 +926,6 @@
     <t>Feed open</t>
   </si>
   <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;(Trécesson rest stop)</t>
-  </si>
-  <si>
     <t>City of Amos</t>
   </si>
   <si>
@@ -1002,6 +987,154 @@
   </si>
   <si>
     <t>Start - Nicol Auto Arena Parking</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt;(Intersection Chemin de l'Esker)</t>
+  </si>
+  <si>
+    <t>KOM Points&lt;br/&gt;(Intersection Chemin de l'Esker)</t>
+  </si>
+  <si>
+    <t>Bretelle vers Rte 111E</t>
+  </si>
+  <si>
+    <t>KOM Sprint</t>
+  </si>
+  <si>
+    <t>Pont en travaux - 1 voie</t>
+  </si>
+  <si>
+    <t>Municipalité d'Authier</t>
+  </si>
+  <si>
+    <t>Ponts - Travaux</t>
+  </si>
+  <si>
+    <t>Voie ferrée très oblique</t>
+  </si>
+  <si>
+    <t>11e Avenue Est</t>
+  </si>
+  <si>
+    <t>Route 111 Est</t>
+  </si>
+  <si>
+    <t>Ramp toward Rte 111E</t>
+  </si>
+  <si>
+    <t>La Sarre Mayor's sprint&lt;br/&gt;250$ (Postal Office Macamic)</t>
+  </si>
+  <si>
+    <t>Sprint du maire de La Sarre&lt;br/&gt;250$ (Bureau de Poste Macamic)</t>
+  </si>
+  <si>
+    <t>Municipality of Authier</t>
+  </si>
+  <si>
+    <t>Bridge - Roadwork  - 1 lane only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridge - Roadwork </t>
+  </si>
+  <si>
+    <t>Municipality of Launay</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Intersection Rtes 111/390)</t>
+  </si>
+  <si>
+    <t>Bonification sprint - times and points&lt;br/&gt;(Rte 111/390 intersections)</t>
+  </si>
+  <si>
+    <t>Sprint du maire de La Sarre&lt;br/&gt;250$ (Parc municipal Engoulevent)</t>
+  </si>
+  <si>
+    <t>La Sarre Mayor's sprint&lt;br/&gt;250$ (Engoulevent municipal parc)</t>
+  </si>
+  <si>
+    <t>Oblique Railroad crossing</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - time and  points&lt;br/&gt;(Trécesson rest stop)</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - times and points&lt;br/&gt;(Trécesson rest stop)</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">onification </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sprint - times and points&lt;br/&gt;(Tony Mercier Garage)</t>
+    </r>
+  </si>
+  <si>
+    <t>1re Avenue Est</t>
+  </si>
+  <si>
+    <t>1re Rue Est</t>
+  </si>
+  <si>
+    <t>4e Avenue Est</t>
+  </si>
+  <si>
+    <t>14e Avenue Est</t>
+  </si>
+  <si>
+    <t>Rue Principale Sud</t>
+  </si>
+  <si>
+    <t>10e Avenue Est</t>
+  </si>
+  <si>
+    <t>Début du 1er tour&lt;br/&gt;Sprint du Maire d'Amos (100$)</t>
+  </si>
+  <si>
+    <t>Start of 1st lap&lt;br/&gt;Amos Mayor's sprint (100$)</t>
+  </si>
+  <si>
+    <t>4e Rue Est</t>
+  </si>
+  <si>
+    <t>Début du 2e tour&lt;br/&gt;Sprint du Maire d'Amos (100$)</t>
+  </si>
+  <si>
+    <t>Start of 2nd lap&lt;br/&gt;Amos Mayor's sprint (100$)</t>
+  </si>
+  <si>
+    <t>Début du 3e tour&lt;br/&gt;Sprint du Maire d'Amos (100$)</t>
+  </si>
+  <si>
+    <t>Début du 4e tour&lt;br/&gt;Sprint du Maire d'Amos (100$)</t>
+  </si>
+  <si>
+    <t>Début du 5e tour&lt;br/&gt;Sprint du Maire d'Amos (100$)</t>
+  </si>
+  <si>
+    <t>Start of 3rd lap&lt;br/&gt;Amos Mayor's sprint (100$)</t>
+  </si>
+  <si>
+    <t>Start of 4th lap&lt;br/&gt;Amos Mayor's sprint (100$)</t>
+  </si>
+  <si>
+    <t>Start of 5th lap&lt;br/&gt;Amos Mayor's sprint (100$)</t>
+  </si>
+  <si>
+    <t>Finish&lt;br/&gt;Time and points bonus</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1145,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1115,14 +1248,41 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <name val="Verdana"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1222,7 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1317,35 +1477,44 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2136,72 +2305,987 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="46" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="59" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" style="46" customWidth="1"/>
     <col min="4" max="4" width="54" style="46" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.15">
-      <c r="A2" s="49">
+      <c r="A2" s="48">
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="57">
+        <v>0.1</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="35" t="str">
+        <f>C4</f>
+        <v>11e Avenue Est</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="57">
+        <v>0.4</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="35" t="str">
+        <f>C5</f>
+        <v>Route 111 Est</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="57">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>310</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="57">
+        <v>3</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="57">
+        <v>7.4</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="57">
+        <v>10.9</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="54" t="s">
         <v>311</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D9" s="54" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="57">
+        <v>18</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="57">
+        <v>18.7</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="57">
+        <v>28.4</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="54" t="s">
         <v>312</v>
       </c>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="53"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="53"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
+      <c r="D12" s="35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="57">
+        <v>30.3</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>313</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="57">
+        <v>31.3</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="57">
+        <v>33</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>285</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="57">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>314</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="57">
+        <v>44.9</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="57">
+        <v>47.3</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="57">
+        <v>49</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>325</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="57">
+        <v>49.5</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="57">
+        <v>52.7</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="57">
+        <v>60.6</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="57">
+        <v>60.9</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>327</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="57">
+        <v>72.5</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>315</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="57">
+        <v>74.2</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="57">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="60" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="57">
+        <v>95.2</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="35" t="str">
+        <f>C27</f>
+        <v>Boulevard Mercier</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="57">
+        <v>95.3</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="D28" s="35" t="str">
+        <f t="shared" ref="D28:D43" si="0">C28</f>
+        <v>2e Avenue Ouest</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="57">
+        <v>95.6</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>290</v>
+      </c>
+      <c r="D29" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>1re Rue Ouest</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="57">
+        <v>96</v>
+      </c>
+      <c r="B30" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="D30" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>5e Avenue Ouest</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="57">
+        <v>96.1</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>Rue Principale Nord</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="57">
+        <v>96.5</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>339</v>
+      </c>
+      <c r="D32" s="61" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="57">
+        <v>96.6</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>333</v>
+      </c>
+      <c r="D33" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>1re Avenue Est</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="57">
+        <v>96.8</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>334</v>
+      </c>
+      <c r="D34" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>1re Rue Est</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="57">
+        <v>97.2</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>335</v>
+      </c>
+      <c r="D35" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>4e Avenue Est</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="57">
+        <v>97.7</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>341</v>
+      </c>
+      <c r="D36" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>4e Rue Est</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="57">
+        <v>98.8</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="54" t="s">
+        <v>336</v>
+      </c>
+      <c r="D37" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>14e Avenue Est</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="57">
+        <v>99.5</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="D38" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>Rue Principale Sud</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="57">
+        <v>100</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="54" t="s">
+        <v>338</v>
+      </c>
+      <c r="D39" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>10e Avenue Est</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="57">
+        <v>100.7</v>
+      </c>
+      <c r="B40" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="54" t="s">
+        <v>289</v>
+      </c>
+      <c r="D40" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>2e Avenue Ouest</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="57">
+        <v>100.9</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="54" t="s">
+        <v>290</v>
+      </c>
+      <c r="D41" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>1re Rue Ouest</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="57">
+        <v>101.3</v>
+      </c>
+      <c r="B42" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="54" t="s">
+        <v>291</v>
+      </c>
+      <c r="D42" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>5e Avenue Ouest</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="57">
+        <v>101.5</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="54" t="s">
+        <v>292</v>
+      </c>
+      <c r="D43" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>Rue Principale Nord</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="57">
+        <f>A32+5.4</f>
+        <v>101.9</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>342</v>
+      </c>
+      <c r="D44" s="61" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="57">
+        <v>107.3</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>284</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="57">
+        <f>A44+5.4</f>
+        <v>107.30000000000001</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="D46" s="61" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="57">
+        <f t="shared" ref="A47:A49" si="1">A46+5.4</f>
+        <v>112.70000000000002</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="D47" s="61" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="57">
+        <f t="shared" si="1"/>
+        <v>118.10000000000002</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>346</v>
+      </c>
+      <c r="D48" s="61" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="57">
+        <f t="shared" si="1"/>
+        <v>123.50000000000003</v>
+      </c>
+      <c r="B49" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="61" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="57"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="57"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="57"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="35"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="57"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="35"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="57"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="35"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="57"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="35"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="35"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="57"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="35"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="57"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="35"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="57"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="35"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="57"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="35"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="57"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="35"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="57"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="35"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="57"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="35"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="57"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="35"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="57"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="35"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="57"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="57"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="35"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="57"/>
+      <c r="B68" s="55"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="35"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="57"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="35"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="57"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="35"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="57"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="35"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="57"/>
+      <c r="B72" s="55"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="35"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="57"/>
+      <c r="B73" s="55"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="35"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="57"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="35"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="57"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="57"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="57"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="57"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="57"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="54"/>
+      <c r="D79" s="35"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="57"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="54"/>
+      <c r="D80" s="35"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="57"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="54"/>
+      <c r="D81" s="35"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="57"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="54"/>
+      <c r="D82" s="35"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="57"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="54"/>
+      <c r="D83" s="35"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="57"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="54"/>
+      <c r="D84" s="35"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="57"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="54"/>
+      <c r="D85" s="35"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="57"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="54"/>
+      <c r="D86" s="35"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="57"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="54"/>
+      <c r="D87" s="35"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="57"/>
+      <c r="B88" s="55"/>
+      <c r="C88" s="54"/>
+      <c r="D88" s="35"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="57"/>
+      <c r="B89" s="55"/>
+      <c r="C89" s="54"/>
+      <c r="D89" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E32EA77D-D8A6-C046-A6FE-2ED5046B48E2}">
+          <x14:formula1>
+            <xm:f>Lexique!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2210,7 +3294,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2253,7 +3337,7 @@
         <v>132</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>20</v>
@@ -2281,7 +3365,7 @@
         <v>87</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>21</v>
@@ -2323,7 +3407,7 @@
         <v>123</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>22</v>
@@ -2351,7 +3435,7 @@
         <v>134</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>23</v>
@@ -2463,7 +3547,7 @@
         <v>131</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C18" t="s">
         <v>136</v>
@@ -2488,16 +3572,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2513,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3450,7 +4534,7 @@
         <v>193</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -4172,8 +5256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4227,10 +5311,10 @@
         <v>125</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F3" s="21"/>
       <c r="K3" s="35"/>
@@ -4243,10 +5327,10 @@
         <v>126</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="21"/>
       <c r="K4" s="35"/>
@@ -4259,10 +5343,10 @@
         <v>126</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F5" s="21"/>
       <c r="K5" s="35"/>
@@ -4275,10 +5359,10 @@
         <v>125</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F6" s="21"/>
       <c r="K6" s="35"/>
@@ -4291,10 +5375,10 @@
         <v>125</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F7" s="21"/>
       <c r="K7" s="35"/>
@@ -4307,16 +5391,16 @@
         <v>126</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="36">
+      <c r="A9" s="52">
         <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
@@ -4339,10 +5423,10 @@
         <v>135</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -4355,10 +5439,10 @@
         <v>124</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -4374,7 +5458,7 @@
         <v>258</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F12" s="21"/>
       <c r="K12" s="34"/>
@@ -4387,10 +5471,10 @@
         <v>134</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -4403,15 +5487,15 @@
         <v>131</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
     </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="26" x14ac:dyDescent="0.2">
       <c r="A15" s="36">
         <v>43.7</v>
       </c>
@@ -4419,10 +5503,10 @@
         <v>124</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -4435,10 +5519,10 @@
         <v>19</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -4451,10 +5535,10 @@
         <v>123</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>274</v>
+        <v>332</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -4467,10 +5551,10 @@
         <v>125</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F18" s="21"/>
       <c r="K18" s="35"/>
@@ -4483,10 +5567,10 @@
         <v>19</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F19" s="21"/>
       <c r="K19" s="35"/>
@@ -4496,13 +5580,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -4515,10 +5599,10 @@
         <v>126</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -4547,10 +5631,10 @@
         <v>125</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -4579,10 +5663,10 @@
         <v>19</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F25" s="21"/>
       <c r="K25" s="34"/>
@@ -4595,10 +5679,10 @@
         <v>134</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -4627,10 +5711,10 @@
         <v>19</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F28" s="21"/>
       <c r="K28" s="35"/>
@@ -4643,10 +5727,10 @@
         <v>131</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -4662,7 +5746,7 @@
         <v>176</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>291</v>
+        <v>331</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -4678,7 +5762,7 @@
         <v>143</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -4691,10 +5775,10 @@
         <v>126</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -4707,10 +5791,10 @@
         <v>125</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -4723,10 +5807,10 @@
         <v>126</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
@@ -4739,7 +5823,7 @@
         <v>179</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D35" s="37" t="s">
         <v>180</v>
@@ -4755,10 +5839,10 @@
         <v>125</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -4771,10 +5855,10 @@
         <v>125</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
@@ -4790,7 +5874,7 @@
         <v>174</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>259</v>
+        <v>350</v>
       </c>
       <c r="F38" s="21"/>
     </row>

</xml_diff>

<commit_message>
Compilation suite ajout Etape 1
- Correction erreurs programmation
- Correction staff
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CD6ED-0197-9040-9F78-642BD7C2428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8A6023-485F-8D4F-A6C5-51A86863CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="4380" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7880" yWindow="4380" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="349">
   <si>
     <t>GPM</t>
   </si>
@@ -460,9 +460,6 @@
     <t>Bypass</t>
   </si>
   <si>
-    <t>Caravan bypass on the right</t>
-  </si>
-  <si>
     <t>Déviation Caravane</t>
   </si>
   <si>
@@ -788,9 +785,6 @@
   </si>
   <si>
     <t>Rue Principale Nord</t>
-  </si>
-  <si>
-    <t>Dérivation caravane sur la droite</t>
   </si>
   <si>
     <t>Rond-point (prendre 1ère sortie)</t>
@@ -1106,13 +1100,13 @@
     <t>Start of 4th lap</t>
   </si>
   <si>
-    <t>Caravan bypass - Right on 3e avenue</t>
-  </si>
-  <si>
-    <t>Caravan bypass - à droite sur 3e avenue</t>
-  </si>
-  <si>
     <t>95.1 km + (4 x 5.4 km) = 116.7 km</t>
+  </si>
+  <si>
+    <t>Déviation de la caravance&lt;br/&gt; À droite sur 3e avenue</t>
+  </si>
+  <si>
+    <t>Caravan bypass&lt;br/&gt;Right on 3e avenue</t>
   </si>
 </sst>
 </file>
@@ -2272,10 +2266,10 @@
         <v>49</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2297,7 +2291,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2313,7 +2307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD90"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -2348,10 +2342,10 @@
         <v>80</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -2363,10 +2357,10 @@
         <v>90</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -2378,7 +2372,7 @@
         <v>89</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D4" s="35" t="str">
         <f>C4</f>
@@ -2393,7 +2387,7 @@
         <v>89</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D5" s="35" t="str">
         <f>C5</f>
@@ -2408,10 +2402,10 @@
         <v>90</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2450,10 +2444,10 @@
         <v>88</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2464,10 +2458,10 @@
         <v>98</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2492,10 +2486,10 @@
         <v>31</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2506,10 +2500,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2534,10 +2528,10 @@
         <v>95</v>
       </c>
       <c r="C15" s="54" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>241</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2548,10 +2542,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2576,10 +2570,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="D18" s="35" t="s">
         <v>228</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2590,10 +2584,10 @@
         <v>87</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2632,10 +2626,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2646,10 +2640,10 @@
         <v>98</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,10 +2654,10 @@
         <v>31</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2674,10 +2668,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="35" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2691,7 +2685,7 @@
         <v>137</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2702,7 +2696,7 @@
         <v>90</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D27" s="35" t="str">
         <f>C27</f>
@@ -2717,7 +2711,7 @@
         <v>89</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D28" s="35" t="str">
         <f t="shared" ref="D28:D43" si="0">C28</f>
@@ -2732,7 +2726,7 @@
         <v>90</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D29" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2747,7 +2741,7 @@
         <v>89</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D30" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2762,7 +2756,7 @@
         <v>89</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D31" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2777,10 +2771,10 @@
         <v>98</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2791,7 +2785,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D33" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2806,7 +2800,7 @@
         <v>90</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D34" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2821,7 +2815,7 @@
         <v>89</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D35" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2836,7 +2830,7 @@
         <v>89</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D36" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2851,7 +2845,7 @@
         <v>89</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D37" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2866,7 +2860,7 @@
         <v>89</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D38" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2881,7 +2875,7 @@
         <v>90</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D39" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2896,7 +2890,7 @@
         <v>89</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D40" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2911,7 +2905,7 @@
         <v>90</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D41" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2926,7 +2920,7 @@
         <v>89</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D42" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2941,7 +2935,7 @@
         <v>89</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D43" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2957,10 +2951,10 @@
         <v>98</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D44" s="61" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2971,10 +2965,10 @@
         <v>95</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2986,10 +2980,10 @@
         <v>98</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D46" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3001,10 +2995,10 @@
         <v>98</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3016,10 +3010,10 @@
         <v>98</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D48" s="61" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3029,10 +3023,10 @@
       <c r="B49" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="C49" s="54" t="s">
-        <v>349</v>
-      </c>
-      <c r="D49" s="35" t="s">
+      <c r="C49" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>348</v>
       </c>
       <c r="E49" s="57"/>
@@ -19428,7 +19422,7 @@
         <v>135</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="51" spans="1:16384" x14ac:dyDescent="0.2">
@@ -19737,7 +19731,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>6</v>
@@ -19765,7 +19759,7 @@
         <v>57</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>7</v>
@@ -19807,7 +19801,7 @@
         <v>87</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>8</v>
@@ -19835,7 +19829,7 @@
         <v>98</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>9</v>
@@ -19947,7 +19941,7 @@
         <v>95</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
         <v>100</v>
@@ -19961,27 +19955,27 @@
         <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" t="s">
         <v>140</v>
-      </c>
-      <c r="D19" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C20" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="16" t="s">
         <v>230</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -19997,7 +19991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -20103,61 +20097,61 @@
         <v>47</v>
       </c>
       <c r="U1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="V1" t="s">
+        <v>145</v>
+      </c>
+      <c r="W1" t="s">
+        <v>144</v>
+      </c>
+      <c r="X1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE1" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="V1" t="s">
-        <v>146</v>
-      </c>
-      <c r="W1" t="s">
-        <v>145</v>
-      </c>
-      <c r="X1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>176</v>
-      </c>
       <c r="AF1" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="AG1" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="AG1" s="16" t="s">
-        <v>156</v>
-      </c>
       <c r="AH1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="AI1" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="AI1" s="31" t="s">
-        <v>159</v>
-      </c>
       <c r="AJ1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AK1" t="s">
         <v>189</v>
       </c>
-      <c r="AK1" t="s">
-        <v>190</v>
-      </c>
       <c r="AL1" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AM1" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
@@ -20180,7 +20174,7 @@
         <v>136</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H2" s="63">
         <v>16</v>
@@ -20223,7 +20217,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20255,32 +20249,32 @@
         <v>0.8112689393939394</v>
       </c>
       <c r="AC2" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE2" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF2" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="AD2" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="AE2" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF2" s="31" t="s">
-        <v>163</v>
-      </c>
       <c r="AG2" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH2" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AK2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -20305,7 +20299,7 @@
         <v>41</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -20348,7 +20342,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20380,32 +20374,32 @@
         <v>0.80075757575757578</v>
       </c>
       <c r="AC3" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD3" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="AD3" s="31" t="s">
-        <v>154</v>
-      </c>
       <c r="AE3" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF3" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AG3" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH3" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AK3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -20472,7 +20466,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20504,31 +20498,31 @@
         <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD4" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE4" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AF4" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG4" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH4" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AI4" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AK4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -20602,7 +20596,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20634,33 +20628,33 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD5" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE5" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF5" s="32" t="s">
         <v>167</v>
-      </c>
-      <c r="AD5" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE5" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF5" s="32" t="s">
-        <v>168</v>
       </c>
       <c r="AG5" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AI5" s="30" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AK5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL5" s="30"/>
       <c r="AM5" s="30"/>
@@ -20679,7 +20673,7 @@
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F6" t="s">
         <v>46</v>
@@ -20728,7 +20722,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20760,32 +20754,32 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AD6" s="30" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF6" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="AG6" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="AG6" s="31" t="s">
+      <c r="AH6" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="AH6" s="31" t="s">
-        <v>173</v>
-      </c>
       <c r="AI6" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AJ6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AK6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -20853,7 +20847,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20885,31 +20879,31 @@
         <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AD7" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE7" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF7" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AH7" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AI7" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AK7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -20931,10 +20925,10 @@
         <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -20978,7 +20972,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21010,31 +21004,31 @@
         <v>0.70300387596899228</v>
       </c>
       <c r="AC8" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD8" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="AE8" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="AF8" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="AD8" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="AE8" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="AF8" s="31" t="s">
+      <c r="AG8" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH8" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="AG8" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="AH8" s="31" t="s">
-        <v>166</v>
-      </c>
       <c r="AI8" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AJ8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AK8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -21058,8 +21052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21092,10 +21086,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21106,10 +21100,10 @@
         <v>90</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21120,10 +21114,10 @@
         <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21134,7 +21128,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>27</v>
@@ -21148,10 +21142,10 @@
         <v>99</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21176,10 +21170,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21190,10 +21184,10 @@
         <v>88</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21204,10 +21198,10 @@
         <v>95</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>241</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21218,10 +21212,10 @@
         <v>87</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21232,10 +21226,10 @@
         <v>90</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21246,10 +21240,10 @@
         <v>88</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21260,7 +21254,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>27</v>
@@ -21274,10 +21268,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21288,10 +21282,10 @@
         <v>87</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21302,10 +21296,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21316,10 +21310,10 @@
         <v>89</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21330,10 +21324,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21344,10 +21338,10 @@
         <v>95</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21358,10 +21352,10 @@
         <v>99</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21372,10 +21366,10 @@
         <v>90</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21386,10 +21380,10 @@
         <v>89</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21400,10 +21394,10 @@
         <v>90</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21414,10 +21408,10 @@
         <v>89</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21428,10 +21422,10 @@
         <v>90</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21442,10 +21436,10 @@
         <v>89</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21456,10 +21450,10 @@
         <v>89</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21470,10 +21464,10 @@
         <v>98</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D29" s="66" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21484,10 +21478,10 @@
         <v>90</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21498,10 +21492,10 @@
         <v>90</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21512,10 +21506,10 @@
         <v>89</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21526,10 +21520,10 @@
         <v>89</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21540,10 +21534,10 @@
         <v>89</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21554,10 +21548,10 @@
         <v>89</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21568,10 +21562,10 @@
         <v>90</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21582,10 +21576,10 @@
         <v>89</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21596,10 +21590,10 @@
         <v>90</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21610,10 +21604,10 @@
         <v>89</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21624,10 +21618,10 @@
         <v>89</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21638,7 +21632,7 @@
         <v>93</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>24</v>
@@ -21652,10 +21646,10 @@
         <v>98</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D42" s="66" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21666,13 +21660,13 @@
         <v>97</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="7">
         <v>118.7</v>
       </c>
@@ -21680,7 +21674,7 @@
         <v>138</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>348</v>
@@ -21697,7 +21691,7 @@
         <v>135</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -21711,7 +21705,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21765,10 +21759,10 @@
         <v>89</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F3" s="21"/>
       <c r="K3" s="35"/>
@@ -21781,10 +21775,10 @@
         <v>90</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="21"/>
       <c r="K4" s="35"/>
@@ -21797,10 +21791,10 @@
         <v>90</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="21"/>
       <c r="K5" s="35"/>
@@ -21813,10 +21807,10 @@
         <v>89</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F6" s="21"/>
       <c r="K6" s="35"/>
@@ -21829,10 +21823,10 @@
         <v>89</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F7" s="21"/>
       <c r="K7" s="35"/>
@@ -21845,10 +21839,10 @@
         <v>90</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
@@ -21877,10 +21871,10 @@
         <v>99</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -21893,10 +21887,10 @@
         <v>88</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -21909,10 +21903,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F12" s="21"/>
       <c r="K12" s="34"/>
@@ -21925,10 +21919,10 @@
         <v>98</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -21941,10 +21935,10 @@
         <v>95</v>
       </c>
       <c r="C14" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="37" t="s">
         <v>241</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>242</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
@@ -21957,10 +21951,10 @@
         <v>88</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -21973,10 +21967,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>224</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>225</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -21989,10 +21983,10 @@
         <v>87</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -22005,10 +21999,10 @@
         <v>89</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F18" s="21"/>
       <c r="K18" s="35"/>
@@ -22021,10 +22015,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="37" t="s">
         <v>228</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>229</v>
       </c>
       <c r="F19" s="21"/>
       <c r="K19" s="35"/>
@@ -22034,13 +22028,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C20" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="37" t="s">
         <v>230</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>231</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -22053,10 +22047,10 @@
         <v>90</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -22085,10 +22079,10 @@
         <v>89</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -22117,10 +22111,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="37" t="s">
         <v>235</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>236</v>
       </c>
       <c r="F25" s="21"/>
       <c r="K25" s="34"/>
@@ -22133,10 +22127,10 @@
         <v>98</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -22165,10 +22159,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" s="37" t="s">
         <v>237</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>238</v>
       </c>
       <c r="F28" s="21"/>
       <c r="K28" s="35"/>
@@ -22181,10 +22175,10 @@
         <v>95</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -22200,7 +22194,7 @@
         <v>137</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -22216,7 +22210,7 @@
         <v>107</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -22229,10 +22223,10 @@
         <v>90</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -22245,10 +22239,10 @@
         <v>89</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -22261,26 +22255,26 @@
         <v>90</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="26" x14ac:dyDescent="0.2">
       <c r="A35" s="36">
         <v>129.80000000000001</v>
       </c>
       <c r="B35" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="C35" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>139</v>
+      <c r="C35" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>348</v>
       </c>
       <c r="F35" s="21"/>
       <c r="K35" s="35"/>
@@ -22293,10 +22287,10 @@
         <v>89</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -22309,10 +22303,10 @@
         <v>89</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
@@ -22328,7 +22322,7 @@
         <v>135</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F38" s="21"/>
     </row>
@@ -22390,7 +22384,7 @@
         <v>94</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Ajout Etape 3 course avant compilation
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10409"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8A6023-485F-8D4F-A6C5-51A86863CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2061FD3D-9A2C-B948-9213-7E100BB3AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="4380" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58600" yWindow="2780" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="351">
   <si>
     <t>GPM</t>
   </si>
@@ -1108,6 +1108,12 @@
   <si>
     <t>Caravan bypass&lt;br/&gt;Right on 3e avenue</t>
   </si>
+  <si>
+    <t>Arrivée Finale</t>
+  </si>
+  <si>
+    <t>Final Finish</t>
+  </si>
 </sst>
 </file>
 
@@ -1117,7 +1123,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1269,6 +1275,28 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1375,7 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1515,6 +1543,20 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1931,7 +1973,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1969,7 +2011,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2075,7 +2117,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2307,7 +2349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -19991,8 +20033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="Q1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21704,7 +21746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -22334,75 +22376,123 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F578A-E7BF-4EB0-BBD6-BC84A4E8AD52}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="14" customWidth="1"/>
-    <col min="3" max="4" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="71" customWidth="1"/>
+    <col min="3" max="4" width="35.83203125" style="70" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:13" ht="38" x14ac:dyDescent="0.15">
+      <c r="A1" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="67" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+      <c r="A2" s="68">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="72" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
+    <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+      <c r="A3" s="68">
+        <v>0.1</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="72" t="str">
+        <f>C3</f>
+        <v>4e Avenue Est</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+      <c r="A4" s="68">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D4" s="72" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+      <c r="A5" s="68">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" s="72" t="str">
+        <f>C5</f>
+        <v>Rue Principale Nord</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="19" x14ac:dyDescent="0.15">
+      <c r="A6" s="68">
         <v>10</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B6" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="C6" s="72" t="s">
+        <v>349</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="K6" s="65"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7" s="65"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8" s="65"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9" s="65"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout étape 3 CLMI
- Ajustement GPX course
- Ajout description itinéraire course
- Ajout images signalisation
- Ajout description signalisation
- Correction PDF pour ajout étapes 3 et 7
- Modif SnakeFiles
- Ajustement Rsync img, PDF et guide
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2061FD3D-9A2C-B948-9213-7E100BB3AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDC86C9-3778-1640-9066-117A26A8500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58600" yWindow="2780" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58600" yWindow="2780" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="348">
   <si>
     <t>GPM</t>
   </si>
@@ -154,12 +154,6 @@
     <t>Vit_lent</t>
   </si>
   <si>
-    <t>Départ - Val-d'OR</t>
-  </si>
-  <si>
-    <t>Start – Val-d'Or on the beach</t>
-  </si>
-  <si>
     <t>Descr_Villes</t>
   </si>
   <si>
@@ -596,9 +590,6 @@
   </si>
   <si>
     <t>(via Val-d'Or)</t>
-  </si>
-  <si>
-    <t>Demi tour</t>
   </si>
   <si>
     <t>Étape 1 - Val-d'Or</t>
@@ -1112,7 +1103,7 @@
     <t>Arrivée Finale</t>
   </si>
   <si>
-    <t>Final Finish</t>
+    <t>Demi-tour</t>
   </si>
 </sst>
 </file>
@@ -2305,18 +2296,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <f>20*6</f>
@@ -2328,12 +2319,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2364,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A1" s="56" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="47" t="s">
         <v>21</v>
@@ -2381,13 +2372,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -2396,13 +2387,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -2411,10 +2402,10 @@
         <v>0.1</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D4" s="35" t="str">
         <f>C4</f>
@@ -2426,10 +2417,10 @@
         <v>0.4</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D5" s="35" t="str">
         <f>C5</f>
@@ -2441,13 +2432,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2455,7 +2446,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="54" t="s">
         <v>12</v>
@@ -2483,13 +2474,13 @@
         <v>10.9</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2497,13 +2488,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2528,10 +2519,10 @@
         <v>31</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2542,10 +2533,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2567,13 +2558,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2584,10 +2575,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2612,10 +2603,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2623,13 +2614,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2668,10 +2659,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2679,13 +2670,13 @@
         <v>60.9</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2696,10 +2687,10 @@
         <v>31</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2710,10 +2701,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="54" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2721,13 +2712,13 @@
         <v>78.900000000000006</v>
       </c>
       <c r="B26" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2735,10 +2726,10 @@
         <v>95.2</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D27" s="35" t="str">
         <f>C27</f>
@@ -2750,10 +2741,10 @@
         <v>95.3</v>
       </c>
       <c r="B28" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D28" s="35" t="str">
         <f t="shared" ref="D28:D43" si="0">C28</f>
@@ -2765,10 +2756,10 @@
         <v>95.6</v>
       </c>
       <c r="B29" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D29" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2780,10 +2771,10 @@
         <v>96</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D30" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2795,10 +2786,10 @@
         <v>96.1</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D31" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2810,13 +2801,13 @@
         <v>96.5</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2824,10 +2815,10 @@
         <v>96.6</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D33" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2839,10 +2830,10 @@
         <v>96.8</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D34" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2854,10 +2845,10 @@
         <v>97.2</v>
       </c>
       <c r="B35" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D35" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2869,10 +2860,10 @@
         <v>97.7</v>
       </c>
       <c r="B36" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D36" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2884,10 +2875,10 @@
         <v>98.8</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D37" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2899,10 +2890,10 @@
         <v>99.5</v>
       </c>
       <c r="B38" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D38" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2914,10 +2905,10 @@
         <v>100</v>
       </c>
       <c r="B39" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D39" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2929,10 +2920,10 @@
         <v>100.7</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D40" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2944,10 +2935,10 @@
         <v>100.9</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D41" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2959,10 +2950,10 @@
         <v>101.3</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D42" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2974,10 +2965,10 @@
         <v>101.5</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D43" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2990,13 +2981,13 @@
         <v>101.9</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D44" s="61" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3004,13 +2995,13 @@
         <v>107.3</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3019,13 +3010,13 @@
         <v>107.30000000000001</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C46" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="D46" s="61" t="s">
         <v>298</v>
-      </c>
-      <c r="D46" s="61" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3034,13 +3025,13 @@
         <v>112.70000000000002</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47" s="53" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47" s="61" t="s">
         <v>299</v>
-      </c>
-      <c r="D47" s="61" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3049,13 +3040,13 @@
         <v>118.10000000000002</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="53" t="s">
+        <v>297</v>
+      </c>
+      <c r="D48" s="61" t="s">
         <v>300</v>
-      </c>
-      <c r="D48" s="61" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3063,13 +3054,13 @@
         <v>122.5</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E49" s="57"/>
       <c r="F49" s="55"/>
@@ -19458,13 +19449,13 @@
         <v>123.50000000000003</v>
       </c>
       <c r="B50" s="55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" s="53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:16384" x14ac:dyDescent="0.2">
@@ -19748,66 +19739,66 @@
         <v>4</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -19815,7 +19806,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>31</v>
@@ -19829,7 +19820,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -19840,184 +19831,184 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" t="s">
         <v>138</v>
-      </c>
-      <c r="B19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -20033,8 +20024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20082,22 +20073,22 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -20106,25 +20097,25 @@
         <v>33</v>
       </c>
       <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O1" t="s">
         <v>109</v>
       </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="P1" s="45" t="s">
         <v>110</v>
-      </c>
-      <c r="N1" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>112</v>
       </c>
       <c r="Q1" t="s">
         <v>34</v>
@@ -20136,64 +20127,64 @@
         <v>36</v>
       </c>
       <c r="T1" s="28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="V1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="W1" t="s">
+        <v>142</v>
+      </c>
+      <c r="X1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z1" t="s">
         <v>144</v>
       </c>
-      <c r="X1" t="s">
-        <v>142</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>146</v>
-      </c>
       <c r="AA1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD1" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="AC1" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>175</v>
-      </c>
       <c r="AF1" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AG1" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="AH1" s="31" t="s">
-        <v>157</v>
-      </c>
       <c r="AI1" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AJ1" t="s">
-        <v>188</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>189</v>
+        <v>185</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="AL1" s="16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AM1" s="16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
@@ -20201,22 +20192,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D2" s="25">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H2" s="63">
         <v>16</v>
@@ -20259,7 +20250,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20291,32 +20282,32 @@
         <v>0.8112689393939394</v>
       </c>
       <c r="AC2" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AE2" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AF2" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH2" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AJ2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AK2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -20326,22 +20317,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" s="25">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -20384,7 +20375,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20416,32 +20407,32 @@
         <v>0.80075757575757578</v>
       </c>
       <c r="AC3" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AD3" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AE3" s="31" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF3" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AG3" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH3" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AJ3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AK3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -20451,22 +20442,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="25">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H4">
         <v>9</v>
@@ -20508,7 +20499,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20540,31 +20531,31 @@
         <v>0.40509259259259256</v>
       </c>
       <c r="AC4" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AD4" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AE4" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AF4" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AG4" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH4" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AI4" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AJ4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AK4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -20580,22 +20571,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="25">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -20638,7 +20629,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20670,33 +20661,33 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AD5" s="31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AE5" s="31" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AF5" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG5" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AI5" s="30" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AK5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AL5" s="30"/>
       <c r="AM5" s="30"/>
@@ -20706,22 +20697,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="25">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -20764,7 +20755,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20796,32 +20787,32 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AD6" s="30" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AF6" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG6" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH6" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="AG6" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH6" s="31" t="s">
-        <v>172</v>
-      </c>
       <c r="AI6" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AJ6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AK6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -20831,22 +20822,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7" s="25">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -20889,7 +20880,7 @@
         <v>41</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20921,31 +20912,31 @@
         <v>0.80271317829457367</v>
       </c>
       <c r="AC7" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AD7" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AE7" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AF7" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AH7" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AI7" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AJ7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AK7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -20955,22 +20946,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D8" s="25">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -21014,7 +21005,7 @@
         <v>41</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21046,31 +21037,31 @@
         <v>0.70300387596899228</v>
       </c>
       <c r="AC8" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD8" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE8" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF8" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG8" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH8" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="AD8" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="AE8" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="AF8" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="AG8" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH8" s="31" t="s">
-        <v>165</v>
-      </c>
       <c r="AI8" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AJ8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AK8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -21094,8 +21085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:D44"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21108,7 +21099,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>21</v>
@@ -21125,13 +21116,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21139,13 +21130,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21153,13 +21144,13 @@
         <v>0.3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21170,7 +21161,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>27</v>
@@ -21181,13 +21172,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21195,7 +21186,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -21212,10 +21203,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21223,13 +21214,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21237,13 +21228,13 @@
         <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21251,13 +21242,13 @@
         <v>47.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21265,13 +21256,13 @@
         <v>58.9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21279,13 +21270,13 @@
         <v>71.599999999999994</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21296,7 +21287,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>27</v>
@@ -21310,10 +21301,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21321,13 +21312,13 @@
         <v>81.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21338,10 +21329,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21349,13 +21340,13 @@
         <v>89.1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21366,10 +21357,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21377,13 +21368,13 @@
         <v>94.5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21391,13 +21382,13 @@
         <v>94.6</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21405,13 +21396,13 @@
         <v>95.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21419,13 +21410,13 @@
         <v>95.8</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21433,13 +21424,13 @@
         <v>96.3</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21447,13 +21438,13 @@
         <v>97</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21461,13 +21452,13 @@
         <v>97.3</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21475,13 +21466,13 @@
         <v>97.7</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21489,13 +21480,13 @@
         <v>97.8</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21503,13 +21494,13 @@
         <v>98.1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D29" s="66" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21517,13 +21508,13 @@
         <v>98.3</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21531,13 +21522,13 @@
         <v>98.5</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21545,13 +21536,13 @@
         <v>98.8</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21559,13 +21550,13 @@
         <v>99.4</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21573,13 +21564,13 @@
         <v>100.5</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21587,13 +21578,13 @@
         <v>101.2</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21601,13 +21592,13 @@
         <v>101.6</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21615,13 +21606,13 @@
         <v>102.3</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21629,13 +21620,13 @@
         <v>102.6</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21643,13 +21634,13 @@
         <v>103</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21657,13 +21648,13 @@
         <v>103.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21671,10 +21662,10 @@
         <v>103.5</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>24</v>
@@ -21685,13 +21676,13 @@
         <v>108.9</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D42" s="66" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21699,13 +21690,13 @@
         <v>114.3</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21713,13 +21704,13 @@
         <v>118.7</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21727,13 +21718,13 @@
         <v>119.7</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -21764,7 +21755,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>21</v>
@@ -21782,7 +21773,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" s="38" t="s">
         <v>10</v>
@@ -21798,13 +21789,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F3" s="21"/>
       <c r="K3" s="35"/>
@@ -21814,13 +21805,13 @@
         <v>0.2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F4" s="21"/>
       <c r="K4" s="35"/>
@@ -21830,13 +21821,13 @@
         <v>0.8</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F5" s="21"/>
       <c r="K5" s="35"/>
@@ -21846,13 +21837,13 @@
         <v>0.9</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F6" s="21"/>
       <c r="K6" s="35"/>
@@ -21862,13 +21853,13 @@
         <v>2.7</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F7" s="21"/>
       <c r="K7" s="35"/>
@@ -21878,13 +21869,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
@@ -21894,7 +21885,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>12</v>
@@ -21910,13 +21901,13 @@
         <v>9.1</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -21926,13 +21917,13 @@
         <v>13.4</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -21945,10 +21936,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F12" s="21"/>
       <c r="K12" s="34"/>
@@ -21958,13 +21949,13 @@
         <v>34.700000000000003</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -21974,13 +21965,13 @@
         <v>35</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
@@ -21990,13 +21981,13 @@
         <v>43.7</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -22009,10 +22000,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -22022,13 +22013,13 @@
         <v>60.2</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -22038,13 +22029,13 @@
         <v>60.4</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F18" s="21"/>
       <c r="K18" s="35"/>
@@ -22057,10 +22048,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F19" s="21"/>
       <c r="K19" s="35"/>
@@ -22070,13 +22061,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -22086,13 +22077,13 @@
         <v>83</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -22118,13 +22109,13 @@
         <v>83.2</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -22153,10 +22144,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F25" s="21"/>
       <c r="K25" s="34"/>
@@ -22166,13 +22157,13 @@
         <v>95</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -22201,10 +22192,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F28" s="21"/>
       <c r="K28" s="35"/>
@@ -22214,13 +22205,13 @@
         <v>110.6</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -22230,13 +22221,13 @@
         <v>112.9</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -22249,10 +22240,10 @@
         <v>5</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -22262,13 +22253,13 @@
         <v>129.4</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -22278,13 +22269,13 @@
         <v>129.5</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -22294,13 +22285,13 @@
         <v>129.69999999999999</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
@@ -22310,13 +22301,13 @@
         <v>129.80000000000001</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F35" s="21"/>
       <c r="K35" s="35"/>
@@ -22326,13 +22317,13 @@
         <v>130.1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -22342,13 +22333,13 @@
         <v>130.30000000000001</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
@@ -22358,13 +22349,13 @@
         <v>130.6</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F38" s="21"/>
     </row>
@@ -22378,21 +22369,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105F578A-E7BF-4EB0-BBD6-BC84A4E8AD52}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="70" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="71" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="12" style="71" customWidth="1"/>
     <col min="3" max="4" width="35.83203125" style="70" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="38" x14ac:dyDescent="0.15">
       <c r="A1" s="67" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="67" t="s">
         <v>21</v>
@@ -22409,13 +22400,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -22423,10 +22414,10 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D3" s="72" t="str">
         <f>C3</f>
@@ -22438,13 +22429,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>185</v>
+        <v>347</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -22452,10 +22443,10 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D5" s="72" t="str">
         <f>C5</f>
@@ -22467,13 +22458,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>350</v>
+        <v>55</v>
       </c>
       <c r="K6" s="65"/>
       <c r="L6" s="34"/>
@@ -22518,7 +22509,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>21</v>
@@ -22535,13 +22526,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -22550,7 +22541,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -22565,7 +22556,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>23</v>
@@ -22580,13 +22571,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="21"/>
     </row>
@@ -22867,7 +22858,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>21</v>
@@ -22884,13 +22875,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22898,7 +22889,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -22912,7 +22903,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>23</v>
@@ -22926,13 +22917,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
@@ -23176,7 +23167,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>21</v>
@@ -23193,13 +23184,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -23208,7 +23199,7 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>22</v>
@@ -23223,7 +23214,7 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>23</v>
@@ -23238,13 +23229,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="21"/>
     </row>

</xml_diff>

<commit_message>
Ajustement article 11 et modif min horaires
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDC86C9-3778-1640-9066-117A26A8500D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C4DDE2-B298-DD4F-BB9C-DC28E3C823C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58600" yWindow="2780" windowWidth="37920" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29460" yWindow="4340" windowWidth="16320" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="354">
   <si>
     <t>GPM</t>
   </si>
@@ -73,12 +73,6 @@
     <t>Sprint Maire $</t>
   </si>
   <si>
-    <t>Départ - Cegep</t>
-  </si>
-  <si>
-    <t>Start – Cegep</t>
-  </si>
-  <si>
     <t>Départ officiel</t>
   </si>
   <si>
@@ -109,18 +103,9 @@
     <t>Symbol</t>
   </si>
   <si>
-    <t>Début du 2e tour</t>
-  </si>
-  <si>
-    <t>Début du 3e tour</t>
-  </si>
-  <si>
     <t>Start of 2nd lap</t>
   </si>
   <si>
-    <t>Start of 3rd lap</t>
-  </si>
-  <si>
     <t>Dernier passage</t>
   </si>
   <si>
@@ -272,9 +257,6 @@
   </si>
   <si>
     <t>Final Finish&lt;br/&gt;Time and points bonus</t>
-  </si>
-  <si>
-    <t>Départ</t>
   </si>
   <si>
     <t>Start</t>
@@ -1034,9 +1016,6 @@
     <t>Round about (1st exit, right)</t>
   </si>
   <si>
-    <t>14e Avenue E.</t>
-  </si>
-  <si>
     <t>Rue Principale S</t>
   </si>
   <si>
@@ -1104,6 +1083,45 @@
   </si>
   <si>
     <t>Demi-tour</t>
+  </si>
+  <si>
+    <t>Entrée sur le circuit d'arrivée&lt;br/&gt;Boulevard Mercier</t>
+  </si>
+  <si>
+    <t>Circuit finish entrance&lt;br/&gt;Boulevard Mercier</t>
+  </si>
+  <si>
+    <t>Circuit finish entrance&lt;br/&gt;14e Avenue E.</t>
+  </si>
+  <si>
+    <t>Entrée sur le circuit d'arrivée&lt;br/&gt;14e Avenue E.</t>
+  </si>
+  <si>
+    <t>Départ - Cegep de l'Abitibi-Témiscamingue</t>
+  </si>
+  <si>
+    <t>Start – Cegep of Abitibi-Témiscamingue</t>
+  </si>
+  <si>
+    <t>Départ - Parc de la Cathédrale</t>
+  </si>
+  <si>
+    <t>Start - Cathedral</t>
+  </si>
+  <si>
+    <t>Départ - École secondaire le Tremplin</t>
+  </si>
+  <si>
+    <t>Start - Le Tremplin High School</t>
+  </si>
+  <si>
+    <t>Départ - Hôtel de Ville Senneterre</t>
+  </si>
+  <si>
+    <t>Start - Senneterre City Hall</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -2296,18 +2314,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <f>20*6</f>
@@ -2319,12 +2337,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -2340,8 +2358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD90"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2355,16 +2373,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.15">
       <c r="A1" s="56" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.15">
@@ -2372,13 +2390,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -2387,13 +2405,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -2402,10 +2420,10 @@
         <v>0.1</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D4" s="35" t="str">
         <f>C4</f>
@@ -2417,10 +2435,10 @@
         <v>0.4</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D5" s="35" t="str">
         <f>C5</f>
@@ -2432,13 +2450,13 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2446,13 +2464,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2460,13 +2478,13 @@
         <v>7.4</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2474,13 +2492,13 @@
         <v>10.9</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,13 +2506,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2502,7 +2520,7 @@
         <v>18.7</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" s="54" t="s">
         <v>2</v>
@@ -2516,13 +2534,13 @@
         <v>28.4</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2533,10 +2551,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2544,13 +2562,13 @@
         <v>31.3</v>
       </c>
       <c r="B14" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2558,13 +2576,13 @@
         <v>33</v>
       </c>
       <c r="B15" s="55" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2572,13 +2590,13 @@
         <v>35.200000000000003</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2586,13 +2604,13 @@
         <v>44.9</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2603,10 +2621,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2614,13 +2632,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="55" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2628,7 +2646,7 @@
         <v>49.5</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C20" s="54" t="s">
         <v>2</v>
@@ -2642,13 +2660,13 @@
         <v>52.7</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2659,10 +2677,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2670,13 +2688,13 @@
         <v>60.9</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2684,13 +2702,13 @@
         <v>72.5</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2701,10 +2719,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="54" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2712,13 +2730,13 @@
         <v>78.900000000000006</v>
       </c>
       <c r="B26" s="55" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2726,14 +2744,13 @@
         <v>95.2</v>
       </c>
       <c r="B27" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>240</v>
-      </c>
-      <c r="D27" s="35" t="str">
-        <f>C27</f>
-        <v>Boulevard Mercier</v>
+        <v>341</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2741,10 +2758,10 @@
         <v>95.3</v>
       </c>
       <c r="B28" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D28" s="35" t="str">
         <f t="shared" ref="D28:D43" si="0">C28</f>
@@ -2756,10 +2773,10 @@
         <v>95.6</v>
       </c>
       <c r="B29" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D29" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2771,10 +2788,10 @@
         <v>96</v>
       </c>
       <c r="B30" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D30" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2786,10 +2803,10 @@
         <v>96.1</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D31" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2801,13 +2818,13 @@
         <v>96.5</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D32" s="61" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2815,10 +2832,10 @@
         <v>96.6</v>
       </c>
       <c r="B33" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D33" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2830,10 +2847,10 @@
         <v>96.8</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D34" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2845,10 +2862,10 @@
         <v>97.2</v>
       </c>
       <c r="B35" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D35" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2860,10 +2877,10 @@
         <v>97.7</v>
       </c>
       <c r="B36" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D36" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2875,10 +2892,10 @@
         <v>98.8</v>
       </c>
       <c r="B37" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D37" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2890,10 +2907,10 @@
         <v>99.5</v>
       </c>
       <c r="B38" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D38" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2905,10 +2922,10 @@
         <v>100</v>
       </c>
       <c r="B39" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D39" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2920,10 +2937,10 @@
         <v>100.7</v>
       </c>
       <c r="B40" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D40" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2935,10 +2952,10 @@
         <v>100.9</v>
       </c>
       <c r="B41" s="55" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D41" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2950,10 +2967,10 @@
         <v>101.3</v>
       </c>
       <c r="B42" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D42" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2965,10 +2982,10 @@
         <v>101.5</v>
       </c>
       <c r="B43" s="55" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D43" s="35" t="str">
         <f t="shared" si="0"/>
@@ -2981,13 +2998,13 @@
         <v>101.9</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D44" s="61" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2995,13 +3012,13 @@
         <v>107.3</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3010,13 +3027,13 @@
         <v>107.30000000000001</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D46" s="61" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3025,13 +3042,13 @@
         <v>112.70000000000002</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D47" s="61" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3040,13 +3057,13 @@
         <v>118.10000000000002</v>
       </c>
       <c r="B48" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D48" s="61" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3054,13 +3071,13 @@
         <v>122.5</v>
       </c>
       <c r="B49" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>345</v>
+        <v>130</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="E49" s="57"/>
       <c r="F49" s="55"/>
@@ -19449,13 +19466,13 @@
         <v>123.50000000000003</v>
       </c>
       <c r="B50" s="55" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C50" s="53" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D50" s="61" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="51" spans="1:16384" x14ac:dyDescent="0.2">
@@ -19703,7 +19720,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E32EA77D-D8A6-C046-A6FE-2ED5046B48E2}">
           <x14:formula1>
             <xm:f>Lexique!$A:$A</xm:f>
@@ -19733,86 +19750,86 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -19820,7 +19837,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -19831,184 +19848,184 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
         <v>93</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -20024,8 +20041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AD21" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20070,121 +20087,121 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="O1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P1" s="45" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S1" s="24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="T1" s="28" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="V1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" t="s">
+        <v>136</v>
+      </c>
+      <c r="X1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="W1" t="s">
-        <v>142</v>
-      </c>
-      <c r="X1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>141</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AH1" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI1" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL1" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="AC1" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="AG1" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="AH1" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="AI1" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>177</v>
-      </c>
       <c r="AM1" s="16" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.15">
@@ -20192,22 +20209,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D2" s="25">
         <v>43656</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="H2" s="63">
         <v>16</v>
@@ -20250,7 +20267,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20282,32 +20299,32 @@
         <v>0.8112689393939394</v>
       </c>
       <c r="AC2" s="31" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AE2" s="31" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="AF2" s="31" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AH2" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Place Agnico-Eagle</v>
       </c>
       <c r="AI2" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AJ2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AK2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -20317,22 +20334,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D3" s="25">
         <v>43657</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H3">
         <v>16</v>
@@ -20375,7 +20392,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20407,32 +20424,32 @@
         <v>0.80075757575757578</v>
       </c>
       <c r="AC3" s="31" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="AD3" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE3" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF3" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="AE3" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="AF3" s="31" t="s">
-        <v>157</v>
-      </c>
       <c r="AG3" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AH3" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI3" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AJ3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="AK3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -20442,22 +20459,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D4" s="25">
         <v>43658</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>9</v>
@@ -20490,16 +20507,16 @@
         <v>10</v>
       </c>
       <c r="Q4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="S4" s="24">
         <v>42</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20528,34 +20545,34 @@
       </c>
       <c r="AB4" s="30">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.40509259259259256</v>
+        <v>0.40489130434782605</v>
       </c>
       <c r="AC4" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AD4" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AE4" s="31" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="AF4" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AG4" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AH4" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AI4" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AJ4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="AK4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
@@ -20571,22 +20588,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D5" s="25">
         <v>43658</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H5">
         <v>18</v>
@@ -20619,7 +20636,7 @@
         <v>57.4</v>
       </c>
       <c r="Q5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="R5">
         <v>46</v>
@@ -20629,7 +20646,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20661,33 +20678,33 @@
         <v>0.81422101449275353</v>
       </c>
       <c r="AC5" s="31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AD5" s="31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AE5" s="31" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="AF5" s="32" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="AG5" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>École secondaire le Tremplin</v>
       </c>
       <c r="AH5" s="31" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="AI5" s="30" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
         <v>Le Tremplin High School</v>
       </c>
       <c r="AJ5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK5" t="s">
         <v>188</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>194</v>
       </c>
       <c r="AL5" s="30"/>
       <c r="AM5" s="30"/>
@@ -20697,22 +20714,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D6" s="25">
         <v>43659</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H6">
         <v>14</v>
@@ -20755,7 +20772,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20787,32 +20804,32 @@
         <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="31" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="AD6" s="30" t="str">
         <f>Tableau2[[#This Row],[VilleDep]]</f>
         <v>Senneterre</v>
       </c>
       <c r="AE6" s="31" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="AF6" s="31" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="AG6" s="31" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AH6" s="31" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AI6" s="31" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AJ6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AK6" t="s">
         <v>189</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>195</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -20822,22 +20839,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D7" s="25">
         <v>43660</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H7">
         <v>16</v>
@@ -20870,17 +20887,17 @@
         <v>115.9</v>
       </c>
       <c r="Q7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S7" s="24">
         <f t="shared" ref="S7:S8" si="1">IF(R7&gt;0,R7-2,"")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -20905,38 +20922,38 @@
       </c>
       <c r="AA7" s="30" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>19:15</v>
+        <v>19:12</v>
       </c>
       <c r="AB7" s="30">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.80271317829457367</v>
+        <v>0.80009469696969693</v>
       </c>
       <c r="AC7" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AD7" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AE7" s="31" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="AF7" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AG7" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AH7" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AI7" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AJ7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="AK7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -20946,22 +20963,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D8" s="25">
         <v>43661</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H8">
         <v>14</v>
@@ -20995,17 +21012,17 @@
         <v>120.5</v>
       </c>
       <c r="Q8">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S8" s="24">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21030,38 +21047,38 @@
       </c>
       <c r="AA8" s="30" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>16:14</v>
+        <v>16:11</v>
       </c>
       <c r="AB8" s="30">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.70300387596899228</v>
+        <v>0.70028409090909094</v>
       </c>
       <c r="AC8" s="31" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="AD8" s="31" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AE8" s="31" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="AF8" s="31" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="AG8" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AH8" s="31" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="AI8" s="31" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AJ8" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="AK8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -21086,7 +21103,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21099,16 +21116,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21116,13 +21133,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21130,13 +21147,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21144,13 +21161,13 @@
         <v>0.3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21158,13 +21175,13 @@
         <v>0.5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21172,13 +21189,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21186,13 +21203,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21203,10 +21220,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21214,13 +21231,13 @@
         <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21228,13 +21245,13 @@
         <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21242,13 +21259,13 @@
         <v>47.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21256,13 +21273,13 @@
         <v>58.9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21270,13 +21287,13 @@
         <v>71.599999999999994</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21284,13 +21301,13 @@
         <v>79.5</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21301,10 +21318,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21312,13 +21329,13 @@
         <v>81.8</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21329,10 +21346,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21340,13 +21357,13 @@
         <v>89.1</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21357,10 +21374,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21368,13 +21385,13 @@
         <v>94.5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21382,13 +21399,13 @@
         <v>94.6</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21396,13 +21413,13 @@
         <v>95.1</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>324</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21410,13 +21427,13 @@
         <v>95.8</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21424,13 +21441,13 @@
         <v>96.3</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21438,13 +21455,13 @@
         <v>97</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21452,13 +21469,13 @@
         <v>97.3</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21466,13 +21483,13 @@
         <v>97.7</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21480,13 +21497,13 @@
         <v>97.8</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21494,13 +21511,13 @@
         <v>98.1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C29" s="65" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D29" s="66" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21508,13 +21525,13 @@
         <v>98.3</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21522,13 +21539,13 @@
         <v>98.5</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21536,13 +21553,13 @@
         <v>98.8</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21550,13 +21567,13 @@
         <v>99.4</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21564,13 +21581,13 @@
         <v>100.5</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21578,13 +21595,13 @@
         <v>101.2</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21592,13 +21609,13 @@
         <v>101.6</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21606,13 +21623,13 @@
         <v>102.3</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21620,13 +21637,13 @@
         <v>102.6</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21634,13 +21651,13 @@
         <v>103</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21648,13 +21665,13 @@
         <v>103.2</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21662,13 +21679,13 @@
         <v>103.5</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21676,13 +21693,13 @@
         <v>108.9</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C42" s="65" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D42" s="66" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21690,13 +21707,13 @@
         <v>114.3</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -21704,13 +21721,13 @@
         <v>118.7</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21718,13 +21735,13 @@
         <v>119.7</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C45" s="65" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -21738,7 +21755,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21755,16 +21772,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" s="35"/>
     </row>
@@ -21773,13 +21790,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>10</v>
+        <v>345</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>11</v>
+        <v>346</v>
       </c>
       <c r="F2" s="21"/>
       <c r="K2" s="35"/>
@@ -21789,13 +21806,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F3" s="21"/>
       <c r="K3" s="35"/>
@@ -21805,13 +21822,13 @@
         <v>0.2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F4" s="21"/>
       <c r="K4" s="35"/>
@@ -21821,13 +21838,13 @@
         <v>0.8</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F5" s="21"/>
       <c r="K5" s="35"/>
@@ -21837,13 +21854,13 @@
         <v>0.9</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F6" s="21"/>
       <c r="K6" s="35"/>
@@ -21853,13 +21870,13 @@
         <v>2.7</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F7" s="21"/>
       <c r="K7" s="35"/>
@@ -21869,13 +21886,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
@@ -21885,13 +21902,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" s="21"/>
       <c r="K9" s="35"/>
@@ -21901,13 +21918,13 @@
         <v>9.1</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -21917,13 +21934,13 @@
         <v>13.4</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -21936,10 +21953,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F12" s="21"/>
       <c r="K12" s="34"/>
@@ -21949,13 +21966,13 @@
         <v>34.700000000000003</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -21965,13 +21982,13 @@
         <v>35</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
@@ -21981,13 +21998,13 @@
         <v>43.7</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -22000,10 +22017,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -22013,13 +22030,13 @@
         <v>60.2</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -22029,13 +22046,13 @@
         <v>60.4</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F18" s="21"/>
       <c r="K18" s="35"/>
@@ -22048,10 +22065,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F19" s="21"/>
       <c r="K19" s="35"/>
@@ -22061,13 +22078,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -22077,13 +22094,13 @@
         <v>83</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -22093,13 +22110,13 @@
         <v>83.1</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F22" s="21"/>
       <c r="K22" s="35"/>
@@ -22109,13 +22126,13 @@
         <v>83.2</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -22125,13 +22142,13 @@
         <v>86.8</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F24" s="21"/>
       <c r="K24" s="35"/>
@@ -22144,10 +22161,10 @@
         <v>5</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F25" s="21"/>
       <c r="K25" s="34"/>
@@ -22157,13 +22174,13 @@
         <v>95</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -22173,13 +22190,13 @@
         <v>106.6</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F27" s="21"/>
       <c r="K27" s="35"/>
@@ -22192,10 +22209,10 @@
         <v>5</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F28" s="21"/>
       <c r="K28" s="35"/>
@@ -22205,13 +22222,13 @@
         <v>110.6</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -22221,13 +22238,13 @@
         <v>112.9</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -22240,10 +22257,10 @@
         <v>5</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -22253,13 +22270,13 @@
         <v>129.4</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -22269,13 +22286,13 @@
         <v>129.5</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -22285,13 +22302,13 @@
         <v>129.69999999999999</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
@@ -22301,13 +22318,13 @@
         <v>129.80000000000001</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F35" s="21"/>
       <c r="K35" s="35"/>
@@ -22317,13 +22334,13 @@
         <v>130.1</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -22333,13 +22350,13 @@
         <v>130.30000000000001</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
@@ -22349,13 +22366,13 @@
         <v>130.6</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F38" s="21"/>
     </row>
@@ -22370,7 +22387,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -22381,18 +22398,18 @@
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="38" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.15">
       <c r="A1" s="67" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="67" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -22400,13 +22417,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>77</v>
+        <v>347</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>78</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -22414,10 +22431,10 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D3" s="72" t="str">
         <f>C3</f>
@@ -22429,13 +22446,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D4" s="72" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -22443,10 +22460,10 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D5" s="72" t="str">
         <f>C5</f>
@@ -22458,13 +22475,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D6" s="72" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K6" s="65"/>
       <c r="L6" s="34"/>
@@ -22496,7 +22513,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22509,16 +22526,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -22526,13 +22543,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>349</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>78</v>
+        <v>350</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -22541,13 +22558,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>353</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>24</v>
+        <v>353</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -22556,13 +22573,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>25</v>
+        <v>353</v>
       </c>
       <c r="F4" s="21"/>
     </row>
@@ -22571,13 +22588,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F5" s="21"/>
     </row>
@@ -22845,7 +22862,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22858,16 +22875,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22875,13 +22892,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>351</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>78</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22889,13 +22906,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>353</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>24</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22903,13 +22920,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>25</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -22917,13 +22934,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
@@ -23154,7 +23171,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23167,16 +23184,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -23184,13 +23201,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>347</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>78</v>
+        <v>348</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -23199,13 +23216,13 @@
         <v>111.2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>353</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>24</v>
+        <v>353</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -23214,13 +23231,13 @@
         <v>114.4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>25</v>
+        <v>353</v>
       </c>
       <c r="F4" s="21"/>
     </row>
@@ -23229,13 +23246,13 @@
         <v>115</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F5" s="21"/>
     </row>

</xml_diff>

<commit_message>
Ajout sign etape 6 et corrections, closes #41
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C4DDE2-B298-DD4F-BB9C-DC28E3C823C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2A2C2-4A49-9C45-831E-5ED0BB94ED3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="4340" windowWidth="16320" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23720" yWindow="2040" windowWidth="22580" windowHeight="24960" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="381">
   <si>
     <t>GPM</t>
   </si>
@@ -1122,6 +1122,87 @@
   </si>
   <si>
     <t>xx</t>
+  </si>
+  <si>
+    <t>Départ - Parc de la Cathédrale d'Amos</t>
+  </si>
+  <si>
+    <t>Start - Parc de la Cathédrale d'Amos</t>
+  </si>
+  <si>
+    <t>Route 109</t>
+  </si>
+  <si>
+    <t>Official Start</t>
+  </si>
+  <si>
+    <t>St-Mathieu-d'Harricana</t>
+  </si>
+  <si>
+    <t>Preissac Mayor's sprint $250 &lt;br/&gt;Intersection chemin St-Luc</t>
+  </si>
+  <si>
+    <t>Rivière-Heva</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;Intersection bretelle rue Principale</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - times and points&lt;br/&gt;Intersection Rue Principale</t>
+  </si>
+  <si>
+    <t>Route 117</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt; Halte routière Cadillac</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - times and points&lt;br/&gt; Rest Area Cadillac</t>
+  </si>
+  <si>
+    <t>Route 395</t>
+  </si>
+  <si>
+    <t>Preissac</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt; Tour d'observation Preissac</t>
+  </si>
+  <si>
+    <t>KOM Points&lt;br/&gt;Observation tower Preissac</t>
+  </si>
+  <si>
+    <t>Sprint du maire Preissac $250&lt;br/&gt;Station service Preissac</t>
+  </si>
+  <si>
+    <t>Mayor's sprint $250&lt;br/&gt;Gas Station Preissac</t>
+  </si>
+  <si>
+    <t>Ste-Gertrude</t>
+  </si>
+  <si>
+    <t>Carrefour giratoire, 1ère sortie à gauche</t>
+  </si>
+  <si>
+    <t>Round about 1st exit, left</t>
+  </si>
+  <si>
+    <t>Arrivée&lt;br/&gt; Bonification en temps et points</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt;Côte de St-Mathieu</t>
+  </si>
+  <si>
+    <t>KOM Points&lt;br/&gt;Côte de St-Mathieu</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Preissac $250 &lt;br/&gt;Intersection chemin St-Luc</t>
+  </si>
+  <si>
+    <t>Carrefour giratoire&lt;br/&gt;1ère sortie à droite sur Rte 111 E</t>
+  </si>
+  <si>
+    <t>Round about&lt;br/&gt;1st exit right on Rte 111 E</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1565,6 +1646,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1980,9 +2064,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2020,9 +2104,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2055,26 +2139,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2107,26 +2174,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -20041,8 +20091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AD21" sqref="AD21"/>
+    <sheetView topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21102,8 +21152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -21284,7 +21334,7 @@
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
-        <v>71.599999999999994</v>
+        <v>72.3</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>80</v>
@@ -23168,10 +23218,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23197,203 +23247,363 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+      <c r="A2" s="73">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A3" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="F3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>111.2</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>12.3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>30</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
+        <v>41.7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
+        <v>42</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
+        <v>42.6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>55.2</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>56</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>59.5</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="9">
+        <v>72.3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A18" s="9">
+        <v>82.3</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="9">
+        <v>82.5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
+        <v>98.2</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A21" s="9">
+        <v>98.9</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="9">
+        <v>115.9</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>114.4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="C22" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="9">
+        <v>117.3</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
+        <v>118.6</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="9">
+        <v>118.9</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="15"/>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19"/>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="17"/>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="17"/>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="18"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="15"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="15"/>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="17"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="15"/>
-      <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="15"/>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="15"/>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="15"/>
+      <c r="C25" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>295</v>
+      </c>
       <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" ht="12" x14ac:dyDescent="0.15">
@@ -23439,17 +23649,17 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="15"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="19"/>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="19"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="15"/>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
@@ -23467,21 +23677,21 @@
       <c r="F35" s="21"/>
     </row>
     <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A36" s="9"/>
+      <c r="A36" s="3"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A37" s="3"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
+      <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
@@ -23496,19 +23706,12 @@
     </row>
     <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="15"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="17"/>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A41" s="3"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="17"/>
-      <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Début montage Etape 5,vref #46
- Ajout des images signalisations
- Ajout tableau Excel `signalisation.xlsx`
- Ajout détails des étapes course dans `itineraires.xlsx`
- Manque les `gpx` et `csv`
- Manque compilation en ajoutant l'étape 5 aux boucles de signalisation
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2A2C2-4A49-9C45-831E-5ED0BB94ED3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFA809C-3A39-C249-B8EA-429D380D11E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23720" yWindow="2040" windowWidth="22580" windowHeight="24960" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="419">
   <si>
     <t>GPM</t>
   </si>
@@ -1118,9 +1118,6 @@
     <t>Départ - Hôtel de Ville Senneterre</t>
   </si>
   <si>
-    <t>Start - Senneterre City Hall</t>
-  </si>
-  <si>
     <t>xx</t>
   </si>
   <si>
@@ -1203,6 +1200,123 @@
   </si>
   <si>
     <t>Round about&lt;br/&gt;1st exit right on Rte 111 E</t>
+  </si>
+  <si>
+    <t>Start - Senneterre Town Hall</t>
+  </si>
+  <si>
+    <t>Continuer sur QC-386 O</t>
+  </si>
+  <si>
+    <t>Stay on QC-386 O</t>
+  </si>
+  <si>
+    <t>Belcourt</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Intersection avenue Goulet)</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - times and points&lt;br/&gt;(Intersection avenue Goulet)</t>
+  </si>
+  <si>
+    <t>Points GPM&lt;br/&gt;(Intersection sentier le Kao)</t>
+  </si>
+  <si>
+    <t>KOM points&lt;br/&gt;(Intersection sentier le Kao)</t>
+  </si>
+  <si>
+    <t>Ravito ouvert</t>
+  </si>
+  <si>
+    <t>Sprint bonification temps et points&lt;br/&gt;(Intersectoin rue Alix)</t>
+  </si>
+  <si>
+    <t>Bonification Sprint - times and points&lt;br/&gt;(Intersection rue Alix)</t>
+  </si>
+  <si>
+    <t>Au rond point, prendre la 3e sortie sur route Transcanadienne/QC-117 S</t>
+  </si>
+  <si>
+    <t>At the round about, take the 3rd exit on route Transcanadienne/QC-117 S</t>
+  </si>
+  <si>
+    <t>Rail road</t>
+  </si>
+  <si>
+    <t>Au rond point, prend la 3e sortie et continuer sur route Transcanadienne/QC-117 S</t>
+  </si>
+  <si>
+    <t>At the round about, take the 3rd exit and stay on Route Transcanadienne/QC-117 S</t>
+  </si>
+  <si>
+    <t>Obaska</t>
+  </si>
+  <si>
+    <t>Ravito fermé</t>
+  </si>
+  <si>
+    <t>Continuer sur 6e rue Ouest</t>
+  </si>
+  <si>
+    <t>Stay on 6e rue Ouest</t>
+  </si>
+  <si>
+    <t>Dérivation de la caravane à droite&lt;br/&gt;Palais de Justice</t>
+  </si>
+  <si>
+    <t>Caravane by pass to the right&lt;br/&gt; Courthouse</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(École St-Isidore)</t>
+  </si>
+  <si>
+    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(École St-Isidore)</t>
+  </si>
+  <si>
+    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Camping le Huard)</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Camping le Huard)</t>
+  </si>
+  <si>
+    <t>Arrivée Finale au sommet&lt;br/&gt;Points double GPM&lt;br/&gt;Arrivée&lt;br/&gt;Bonification en temps et points</t>
+  </si>
+  <si>
+    <t>Final summit Finish&lt;br/&gt;Double points KOM&lt;br/&gt;Time and points bonus</t>
+  </si>
+  <si>
+    <t>QC-397 S</t>
+  </si>
+  <si>
+    <t>QC-113 N</t>
+  </si>
+  <si>
+    <t>10e Avenue/QC 386 E</t>
+  </si>
+  <si>
+    <t>Rue du Parc</t>
+  </si>
+  <si>
+    <t>Chemin du Mont Bell</t>
+  </si>
+  <si>
+    <t>Montée de la Tour</t>
+  </si>
+  <si>
+    <t>Montée de la tour</t>
+  </si>
+  <si>
+    <t>Trash Zone &lt;br/&gt;Orbit Garant area</t>
+  </si>
+  <si>
+    <t>Zone déchets &lt;br/&gt;Secteur Orbit Garant</t>
+  </si>
+  <si>
+    <t>Points GPM &lt;br/&gt;(Mine Aur Ressource)</t>
+  </si>
+  <si>
+    <t>KOM Points &lt;br/&gt;(Mine Aur Ressource)</t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD90"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C49" sqref="C49:D49"/>
     </sheetView>
   </sheetViews>
@@ -19788,7 +19902,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21152,7 +21266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -21804,8 +21918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22611,10 +22725,10 @@
         <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -22626,10 +22740,10 @@
         <v>91</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F4" s="21"/>
     </row>
@@ -22909,10 +23023,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61388227-0C5A-4795-A5A0-4EE10C974F3C}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22938,216 +23052,424 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+      <c r="A2" s="13">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>351</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>352</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="3">
-        <v>111.2</v>
+      <c r="A3" s="7">
+        <v>0.7</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>353</v>
+        <v>381</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>353</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
-        <v>114.4</v>
+      <c r="A4" s="7">
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>353</v>
+        <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="3">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>29.6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A8" s="7">
+        <v>35</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A9" s="7">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>55.8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>56.5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>67.3</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>71</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A14" s="7">
+        <v>72.3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="7">
+        <v>72.8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="7">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A17" s="7">
+        <v>74.8</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="7">
+        <v>96.1</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="7">
+        <v>103.3</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>116.6</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A21" s="7">
+        <v>117</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A22" s="7">
+        <v>125</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="7">
+        <v>139</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="7">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="7">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="7">
+        <v>140.5</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="7">
+        <v>142.1</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A28" s="7">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
+        <v>144.6</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+      <c r="A30" s="7">
+        <v>144.9</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+      <c r="A31" s="7">
+        <v>145</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="17"/>
-    </row>
-    <row r="12" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="18"/>
-    </row>
-    <row r="15" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="18"/>
-    </row>
-    <row r="16" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="18"/>
-    </row>
-    <row r="17" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A26" s="3"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="15"/>
-    </row>
-    <row r="27" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A28" s="3"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="15"/>
+      <c r="C31" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
@@ -23156,16 +23478,16 @@
       <c r="D32" s="15"/>
     </row>
     <row r="33" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
+      <c r="A33" s="3"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="19"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="15"/>
     </row>
     <row r="34" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="15"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="19"/>
     </row>
     <row r="35" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9"/>
@@ -23180,19 +23502,19 @@
       <c r="D36" s="15"/>
     </row>
     <row r="37" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A37" s="3"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
     </row>
     <row r="38" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A38" s="9"/>
+      <c r="A38" s="3"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" ht="12" x14ac:dyDescent="0.15">
-      <c r="A39" s="3"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5"/>
       <c r="D39" s="15"/>
@@ -23205,11 +23527,17 @@
     </row>
     <row r="41" spans="1:4" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="42" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="12" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23221,7 +23549,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23254,10 +23582,10 @@
         <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>354</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>355</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -23269,10 +23597,10 @@
         <v>81</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>379</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>380</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -23284,10 +23612,10 @@
         <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F4" s="21"/>
     </row>
@@ -23302,7 +23630,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F5" s="21"/>
     </row>
@@ -23314,10 +23642,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F6" s="21"/>
     </row>
@@ -23329,10 +23657,10 @@
         <v>80</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>376</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>377</v>
       </c>
       <c r="F7" s="21"/>
     </row>
@@ -23344,10 +23672,10 @@
         <v>90</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F8" s="21"/>
     </row>
@@ -23374,10 +23702,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F10" s="21"/>
     </row>
@@ -23389,10 +23717,10 @@
         <v>79</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>361</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>362</v>
       </c>
       <c r="F11" s="21"/>
     </row>
@@ -23404,10 +23732,10 @@
         <v>84</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F12" s="21"/>
     </row>
@@ -23434,10 +23762,10 @@
         <v>79</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>364</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>365</v>
       </c>
       <c r="F14" s="21"/>
     </row>
@@ -23449,10 +23777,10 @@
         <v>81</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F15" s="21"/>
     </row>
@@ -23464,10 +23792,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F16" s="21"/>
     </row>
@@ -23479,10 +23807,10 @@
         <v>80</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>368</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>369</v>
       </c>
       <c r="F17" s="21"/>
     </row>
@@ -23494,10 +23822,10 @@
         <v>90</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>371</v>
       </c>
       <c r="F18" s="21"/>
     </row>
@@ -23524,10 +23852,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F20" s="21"/>
     </row>
@@ -23566,13 +23894,13 @@
         <v>117.3</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>373</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>374</v>
       </c>
       <c r="F23" s="21"/>
     </row>
@@ -23599,7 +23927,7 @@
         <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>295</v>

</xml_diff>

<commit_message>
Correction sprint maire E5
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1761F8-7BE7-A84C-ADEC-3006334DCB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B075072F-4438-B24A-83CE-DF7B6B1022D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42600" yWindow="4460" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -23188,8 +23188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61388227-0C5A-4795-A5A0-4EE10C974F3C}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23345,7 +23345,7 @@
         <v>56.5</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>378</v>

</xml_diff>

<commit_message>
Ajout fichiers post Senneterre
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AC7A7E-437A-0F49-9837-969DD8DB770B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2E4B25-7FB2-1842-B8F4-2F8EE24EC3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <sheet name="Etape_7" sheetId="28" r:id="rId10"/>
     <sheet name="Etape_5_Senneterre_annulee" sheetId="26" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23831,7 +23831,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23976,7 +23976,7 @@
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
-        <v>46</v>
+        <v>45.5</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Ajustement du nombre d'équipe pour calcul heure fin du CLMI
- 13 équipes de 6 coureurs
- Annulation de la présence de l'Algérie
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF19A8-F1FC-134A-B28E-1F7A7144F2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC9559-FAC3-B644-AF4E-43D874A291D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2520,7 +2520,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2545,8 +2545,8 @@
         <v>40</v>
       </c>
       <c r="B2">
-        <f>20*6</f>
-        <v>120</v>
+        <f>13*6</f>
+        <v>78</v>
       </c>
       <c r="C2" s="33">
         <v>6.9444444444444447E-4</v>
@@ -20846,8 +20846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21381,11 +21381,11 @@
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
-        <v>11:40</v>
+        <v>10:58</v>
       </c>
       <c r="AM4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[DerDep]],"HH:MM")</f>
-        <v>11:53</v>
+        <v>11:11</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
retour commit dimanche soir
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF19A8-F1FC-134A-B28E-1F7A7144F2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC9559-FAC3-B644-AF4E-43D874A291D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2520,7 +2520,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2545,8 +2545,8 @@
         <v>40</v>
       </c>
       <c r="B2">
-        <f>20*6</f>
-        <v>120</v>
+        <f>13*6</f>
+        <v>78</v>
       </c>
       <c r="C2" s="33">
         <v>6.9444444444444447E-4</v>
@@ -20846,8 +20846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21381,11 +21381,11 @@
       </c>
       <c r="AL4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
-        <v>11:40</v>
+        <v>10:58</v>
       </c>
       <c r="AM4" s="30" t="str">
         <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[DerDep]],"HH:MM")</f>
-        <v>11:53</v>
+        <v>11:11</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ajustement masso et zone déchet etape 5
- Zone déchet déplacée de R-H à Preissac
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DC9559-FAC3-B644-AF4E-43D874A291D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA0BB2F-4C56-1D4D-B654-02415D2F1339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="433">
   <si>
     <t>GPM</t>
   </si>
@@ -1354,6 +1354,12 @@
   </si>
   <si>
     <t>(via Preissac &amp; Rivière-Héva )</t>
+  </si>
+  <si>
+    <t>Zone déchets (après le pont, sur 200 m)</t>
+  </si>
+  <si>
+    <t>Trash zone (after the bridge, on 200 m)</t>
   </si>
 </sst>
 </file>
@@ -2575,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD94"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2740,10 +2746,10 @@
       <c r="B11" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2868,10 +2874,10 @@
       <c r="B20" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>389</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="53" t="s">
         <v>390</v>
       </c>
     </row>
@@ -2939,10 +2945,10 @@
       <c r="B25" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="53" t="s">
         <v>226</v>
       </c>
     </row>
@@ -20846,7 +20852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="X1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
@@ -22575,8 +22581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23831,7 +23837,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23991,107 +23997,107 @@
     </row>
     <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
-        <v>59.4</v>
+        <v>53.4</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>279</v>
+        <v>197</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>432</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
+        <v>59.4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
         <v>62.5</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A13" s="9">
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
         <v>62.9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="9">
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
         <v>76.099999999999994</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A15" s="9">
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
         <v>76.3</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D16" s="17" t="s">
         <v>422</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="9">
-        <v>76.599999999999994</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="D16" s="15" t="str">
-        <f>C16</f>
-        <v>Rue des Quatre-Coins</v>
       </c>
       <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
-        <v>76.7</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>411</v>
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D17" s="15" t="str">
+        <f>C17</f>
+        <v>Rue des Quatre-Coins</v>
       </c>
       <c r="F17" s="21"/>
     </row>

</xml_diff>

<commit_message>
Correction St-Mathieu etape 5
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA0BB2F-4C56-1D4D-B654-02415D2F1339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A7C692-4498-CB44-8B84-01A074D5AB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33140" yWindow="3180" windowWidth="57000" windowHeight="21400" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -2581,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBABC76-FD83-474C-AEDA-AED834DA5AED}">
   <dimension ref="A1:XFD94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -23836,8 +23836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -24163,7 +24163,7 @@
     </row>
     <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
-        <v>15.71</v>
+        <v>105.71</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Ajout pont de bois, etape 6
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A7C692-4498-CB44-8B84-01A074D5AB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E27FB4-AAC4-1D4C-B02D-82680522B414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="435">
   <si>
     <t>GPM</t>
   </si>
@@ -1360,6 +1360,12 @@
   </si>
   <si>
     <t>Trash zone (after the bridge, on 200 m)</t>
+  </si>
+  <si>
+    <t>Pont de bois</t>
+  </si>
+  <si>
+    <t>Wooden bridge</t>
   </si>
 </sst>
 </file>
@@ -23836,7 +23842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -24358,10 +24364,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -24656,114 +24662,122 @@
     </row>
     <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
-        <v>98.2</v>
+        <v>88</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>287</v>
+        <v>25</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>434</v>
       </c>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
-        <v>98.9</v>
+        <v>98.2</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>200</v>
+        <v>287</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
       <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
+        <v>98.9</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="9">
         <v>115.9</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A23" s="9">
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
         <v>117.3</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="9">
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="9">
         <v>118.6</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="F25" s="21"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
         <v>118.8</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C26" s="73" t="s">
         <v>313</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D26" s="74" t="s">
         <v>314</v>
       </c>
-      <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="9">
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="9">
         <v>118.9</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D27" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="15"/>
       <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
@@ -24795,17 +24809,17 @@
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
+      <c r="A32" s="3"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="15"/>
       <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="15"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="19"/>
       <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" ht="12" x14ac:dyDescent="0.15">
@@ -24823,21 +24837,21 @@
       <c r="F35" s="21"/>
     </row>
     <row r="36" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A36" s="3"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5"/>
       <c r="D36" s="15"/>
       <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A37" s="9"/>
+      <c r="A37" s="3"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5"/>
       <c r="D37" s="15"/>
       <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A38" s="3"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5"/>
       <c r="D38" s="15"/>
@@ -24852,12 +24866,19 @@
     </row>
     <row r="40" spans="1:6" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="17"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="15"/>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:6" ht="12" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="17"/>
+      <c r="F41" s="21"/>
+    </row>
+    <row r="42" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>